<commit_message>
Refactor column name generation and enhance database table creation logic; streamline complex column handling and improve naming conventions
</commit_message>
<xml_diff>
--- a/datasheets/20250708 Runsheet.xlsx
+++ b/datasheets/20250708 Runsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Morgano\CVD Runsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C376038\Documents\python_code\cvd_sql\datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6E4111-D862-4540-BDC1-CC3FD1FE0319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7A6CBC-6C09-4209-8A03-8D50572C750F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="135" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Run 1" sheetId="26" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="128">
   <si>
     <t>Lab 104D SierraTherm CVD Coater Data Sheet</t>
   </si>
@@ -441,6 +441,12 @@
 Mix: 95% MBTC:5% DMTC
 Sample on boro, Header and trailer on refractory
 </t>
+  </si>
+  <si>
+    <t>Reagent</t>
+  </si>
+  <si>
+    <t>Condenser Temperature ©</t>
   </si>
 </sst>
 </file>
@@ -2323,51 +2329,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="I21" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="40" workbookViewId="0">
+      <selection activeCell="V38" sqref="V38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="10" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31" style="119" customWidth="1"/>
     <col min="2" max="2" width="9.33203125" style="119"/>
     <col min="3" max="3" width="21.6640625" style="119" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" style="119" customWidth="1"/>
-    <col min="5" max="5" width="25.83203125" style="119" customWidth="1"/>
+    <col min="5" max="5" width="25.77734375" style="119" customWidth="1"/>
     <col min="6" max="6" width="22.6640625" style="119" customWidth="1"/>
-    <col min="7" max="7" width="11.5" style="119" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5" style="119" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.1640625" style="119" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" style="119" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" style="119" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.109375" style="119" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.33203125" style="119" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.83203125" style="119" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" style="119" customWidth="1"/>
     <col min="12" max="12" width="9.33203125" style="119"/>
     <col min="13" max="13" width="24" style="119" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.5" style="119" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="3.5" style="119" customWidth="1"/>
-    <col min="16" max="16" width="11.83203125" style="119" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.44140625" style="119" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.44140625" style="119" customWidth="1"/>
+    <col min="16" max="16" width="11.77734375" style="119" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14.33203125" style="119" customWidth="1"/>
-    <col min="18" max="18" width="16.1640625" style="119" customWidth="1"/>
+    <col min="18" max="18" width="16.109375" style="119" customWidth="1"/>
     <col min="19" max="19" width="18" style="119" customWidth="1"/>
     <col min="20" max="20" width="9.33203125" style="119"/>
-    <col min="21" max="21" width="31.5" style="119" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="31.44140625" style="119" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="9.33203125" style="119"/>
     <col min="23" max="23" width="11.33203125" style="119" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="11.6640625" style="119" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.83203125" style="119" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="32.1640625" style="119" customWidth="1"/>
-    <col min="27" max="27" width="11.5" style="119" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.77734375" style="119" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="32.109375" style="119" customWidth="1"/>
+    <col min="27" max="27" width="11.44140625" style="119" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="9.33203125" style="119"/>
-    <col min="29" max="29" width="18.5" style="119" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.44140625" style="119" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="19.33203125" style="119" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.5" style="119" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.44140625" style="119" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="15.6640625" style="119" customWidth="1"/>
     <col min="33" max="33" width="24" style="119" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="3.6640625" style="119" customWidth="1"/>
-    <col min="35" max="35" width="2.83203125" style="119" customWidth="1"/>
+    <col min="35" max="35" width="2.77734375" style="119" customWidth="1"/>
     <col min="36" max="16384" width="9.33203125" style="119"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="30" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:25" ht="30" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2387,7 +2393,7 @@
       <c r="O1" s="2"/>
       <c r="Y1" s="29"/>
     </row>
-    <row r="2" spans="1:25" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="233" t="s">
         <v>119</v>
@@ -2407,7 +2413,7 @@
       <c r="O2" s="3"/>
       <c r="Y2" s="29"/>
     </row>
-    <row r="3" spans="1:25" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" ht="20" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -2435,7 +2441,7 @@
       <c r="O3" s="156"/>
       <c r="Y3" s="29"/>
     </row>
-    <row r="4" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="10"/>
       <c r="B4" s="11"/>
       <c r="C4" s="5"/>
@@ -2453,7 +2459,7 @@
       <c r="O4" s="3"/>
       <c r="Y4" s="29"/>
     </row>
-    <row r="5" spans="1:25" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" ht="20" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -2479,10 +2485,10 @@
       <c r="O5" s="155"/>
       <c r="Y5" s="29"/>
     </row>
-    <row r="6" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="Y6" s="29"/>
     </row>
-    <row r="7" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" ht="14" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>6</v>
       </c>
@@ -2501,7 +2507,7 @@
       <c r="M7" s="123"/>
       <c r="Y7" s="29"/>
     </row>
-    <row r="8" spans="1:25" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="16"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -2514,7 +2520,7 @@
       <c r="M8" s="126"/>
       <c r="Y8" s="29"/>
     </row>
-    <row r="9" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="127" t="s">
         <v>9</v>
       </c>
@@ -2549,7 +2555,7 @@
       </c>
       <c r="Y9" s="29"/>
     </row>
-    <row r="10" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="132" t="s">
         <v>15</v>
       </c>
@@ -2584,7 +2590,7 @@
       </c>
       <c r="Y10" s="29"/>
     </row>
-    <row r="11" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="132" t="s">
         <v>20</v>
       </c>
@@ -2619,7 +2625,7 @@
       </c>
       <c r="Y11" s="29"/>
     </row>
-    <row r="12" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="132" t="s">
         <v>26</v>
       </c>
@@ -2647,7 +2653,7 @@
       </c>
       <c r="Y12" s="29"/>
     </row>
-    <row r="13" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="132" t="s">
         <v>30</v>
       </c>
@@ -2674,7 +2680,7 @@
       </c>
       <c r="Y13" s="29"/>
     </row>
-    <row r="14" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="135" t="s">
         <v>34</v>
       </c>
@@ -2701,7 +2707,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" ht="14" x14ac:dyDescent="0.3">
       <c r="A15" s="60"/>
       <c r="B15" s="29"/>
       <c r="C15" s="29"/>
@@ -2725,7 +2731,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="17" spans="1:39" ht="18.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" ht="18.5" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A17" s="91" t="s">
         <v>40</v>
       </c>
@@ -2743,7 +2749,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="18" spans="1:39" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="94" t="s">
         <v>42</v>
       </c>
@@ -2761,7 +2767,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="19" spans="1:39" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="96" t="s">
         <v>45</v>
       </c>
@@ -2783,7 +2789,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="20" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="98" t="s">
         <v>48</v>
       </c>
@@ -2797,7 +2803,7 @@
       </c>
       <c r="H20" s="97"/>
     </row>
-    <row r="21" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="99" t="s">
         <v>50</v>
       </c>
@@ -2811,7 +2817,7 @@
       </c>
       <c r="H21" s="97"/>
     </row>
-    <row r="22" spans="1:39" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:39" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="100" t="s">
         <v>52</v>
       </c>
@@ -2825,7 +2831,7 @@
       </c>
       <c r="H22" s="101"/>
     </row>
-    <row r="23" spans="1:39" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:39" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="102" t="s">
         <v>54</v>
       </c>
@@ -2841,7 +2847,7 @@
       </c>
       <c r="H23" s="101"/>
     </row>
-    <row r="24" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="102" t="s">
         <v>56</v>
       </c>
@@ -2857,7 +2863,7 @@
       </c>
       <c r="H24" s="101"/>
     </row>
-    <row r="25" spans="1:39" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="103" t="s">
         <v>58</v>
       </c>
@@ -2871,7 +2877,7 @@
       <c r="G25" s="105"/>
       <c r="H25" s="106"/>
     </row>
-    <row r="26" spans="1:39" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" ht="10.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="140"/>
       <c r="B26" s="141"/>
       <c r="C26" s="141"/>
@@ -2881,8 +2887,8 @@
       <c r="G26" s="141"/>
       <c r="H26" s="142"/>
     </row>
-    <row r="27" spans="1:39" ht="12" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:39" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:39" ht="10.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:39" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A28" s="217" t="s">
         <v>59</v>
       </c>
@@ -2924,7 +2930,7 @@
       <c r="AJ28" s="218"/>
       <c r="AM28" s="51"/>
     </row>
-    <row r="29" spans="1:39" ht="18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:39" ht="18" x14ac:dyDescent="0.4">
       <c r="A29" s="192"/>
       <c r="B29" s="232"/>
       <c r="C29" s="54" t="s">
@@ -2940,7 +2946,7 @@
         <v>3</v>
       </c>
       <c r="L29" s="192" t="s">
-        <v>62</v>
+        <v>127</v>
       </c>
       <c r="M29" s="193"/>
       <c r="N29" s="157"/>
@@ -2976,7 +2982,7 @@
       <c r="AK29" s="216"/>
       <c r="AL29" s="193"/>
     </row>
-    <row r="30" spans="1:39" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:39" ht="20" x14ac:dyDescent="0.4">
       <c r="A30" s="230" t="s">
         <v>64</v>
       </c>
@@ -3026,7 +3032,7 @@
       <c r="AK30" s="144"/>
       <c r="AL30" s="145"/>
     </row>
-    <row r="31" spans="1:39" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:39" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A31" s="198" t="s">
         <v>67</v>
       </c>
@@ -3076,7 +3082,7 @@
       <c r="AK31" s="144"/>
       <c r="AL31" s="145"/>
     </row>
-    <row r="32" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:39" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="146"/>
       <c r="B32" s="29"/>
       <c r="C32" s="29"/>
@@ -3100,7 +3106,7 @@
       <c r="AK32" s="144"/>
       <c r="AL32" s="145"/>
     </row>
-    <row r="33" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:38" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="147"/>
       <c r="B33" s="30" t="s">
         <v>71</v>
@@ -3168,7 +3174,7 @@
       <c r="AK33" s="144"/>
       <c r="AL33" s="145"/>
     </row>
-    <row r="34" spans="1:38" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:38" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C34" s="33">
         <v>160</v>
       </c>
@@ -3210,7 +3216,7 @@
       <c r="AK34" s="144"/>
       <c r="AL34" s="145"/>
     </row>
-    <row r="35" spans="1:38" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:38" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C35" s="166"/>
       <c r="D35" s="155"/>
       <c r="G35" s="166"/>
@@ -3270,7 +3276,7 @@
       <c r="AK36" s="149"/>
       <c r="AL36" s="150"/>
     </row>
-    <row r="37" spans="1:38" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:38" ht="18.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="173" t="s">
         <v>79</v>
       </c>
@@ -3304,11 +3310,13 @@
       <c r="AG37" s="75"/>
       <c r="AH37" s="165"/>
     </row>
-    <row r="38" spans="1:38" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:38" ht="36" x14ac:dyDescent="0.4">
       <c r="A38" s="107" t="s">
         <v>80</v>
       </c>
-      <c r="B38" s="79"/>
+      <c r="B38" s="79" t="s">
+        <v>126</v>
+      </c>
       <c r="C38" s="79" t="s">
         <v>81</v>
       </c>
@@ -3350,7 +3358,9 @@
       <c r="U38" s="107" t="s">
         <v>80</v>
       </c>
-      <c r="V38" s="79"/>
+      <c r="V38" s="79" t="s">
+        <v>126</v>
+      </c>
       <c r="W38" s="79" t="s">
         <v>81</v>
       </c>
@@ -3384,7 +3394,7 @@
       </c>
       <c r="AH38" s="165"/>
     </row>
-    <row r="39" spans="1:38" ht="30" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:38" ht="31" x14ac:dyDescent="0.35">
       <c r="A39" s="108" t="s">
         <v>92</v>
       </c>
@@ -3464,7 +3474,7 @@
       </c>
       <c r="AH39" s="165"/>
     </row>
-    <row r="40" spans="1:38" ht="20.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:38" ht="20" x14ac:dyDescent="0.35">
       <c r="A40" s="108" t="s">
         <v>101</v>
       </c>
@@ -3538,7 +3548,7 @@
       <c r="AG40" s="40"/>
       <c r="AH40" s="165"/>
     </row>
-    <row r="41" spans="1:38" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:38" ht="20.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="108" t="s">
         <v>105</v>
       </c>
@@ -3610,7 +3620,7 @@
       <c r="AG41" s="40"/>
       <c r="AH41" s="165"/>
     </row>
-    <row r="42" spans="1:38" ht="20.25" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:38" ht="20" x14ac:dyDescent="0.2">
       <c r="A42" s="108" t="s">
         <v>109</v>
       </c>
@@ -3672,7 +3682,7 @@
       <c r="AG42" s="40"/>
       <c r="AH42" s="165"/>
     </row>
-    <row r="43" spans="1:38" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:38" ht="20.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="109" t="s">
         <v>112</v>
       </c>
@@ -3738,14 +3748,14 @@
       <c r="AG43" s="43"/>
       <c r="AH43" s="165"/>
     </row>
-    <row r="44" spans="1:38" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:38" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A44" s="174"/>
       <c r="B44" s="44"/>
       <c r="C44" s="18"/>
       <c r="D44" s="18"/>
       <c r="E44" s="18"/>
-      <c r="F44" s="68" t="s">
-        <v>115</v>
+      <c r="F44" s="68">
+        <v>2</v>
       </c>
       <c r="G44" s="161"/>
       <c r="H44" s="162"/>
@@ -3772,7 +3782,7 @@
       <c r="AG44" s="163"/>
       <c r="AH44" s="165"/>
     </row>
-    <row r="45" spans="1:38" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:38" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A45" s="110"/>
       <c r="B45" s="111"/>
       <c r="C45" s="112"/>
@@ -4485,47 +4495,47 @@
       <selection activeCell="B23" sqref="B23:B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="10" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31" style="119" customWidth="1"/>
     <col min="2" max="2" width="9.33203125" style="119"/>
     <col min="3" max="3" width="21.6640625" style="119" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" style="119" customWidth="1"/>
-    <col min="5" max="5" width="25.83203125" style="119" customWidth="1"/>
+    <col min="5" max="5" width="25.77734375" style="119" customWidth="1"/>
     <col min="6" max="6" width="22.6640625" style="119" customWidth="1"/>
-    <col min="7" max="7" width="11.5" style="119" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5" style="119" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.1640625" style="119" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" style="119" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" style="119" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.109375" style="119" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.33203125" style="119" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.83203125" style="119" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" style="119" customWidth="1"/>
     <col min="12" max="12" width="9.33203125" style="119"/>
     <col min="13" max="13" width="24" style="119" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.5" style="119" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="3.5" style="119" customWidth="1"/>
-    <col min="16" max="16" width="11.83203125" style="119" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.44140625" style="119" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.44140625" style="119" customWidth="1"/>
+    <col min="16" max="16" width="11.77734375" style="119" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14.33203125" style="119" customWidth="1"/>
-    <col min="18" max="18" width="16.1640625" style="119" customWidth="1"/>
+    <col min="18" max="18" width="16.109375" style="119" customWidth="1"/>
     <col min="19" max="19" width="18" style="119" customWidth="1"/>
     <col min="20" max="20" width="9.33203125" style="119"/>
-    <col min="21" max="21" width="31.5" style="119" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="31.44140625" style="119" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="9.33203125" style="119"/>
     <col min="23" max="23" width="11.33203125" style="119" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="11.6640625" style="119" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.83203125" style="119" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="32.1640625" style="119" customWidth="1"/>
-    <col min="27" max="27" width="11.5" style="119" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.77734375" style="119" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="32.109375" style="119" customWidth="1"/>
+    <col min="27" max="27" width="11.44140625" style="119" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="9.33203125" style="119"/>
-    <col min="29" max="29" width="18.5" style="119" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.44140625" style="119" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="19.33203125" style="119" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.5" style="119" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.44140625" style="119" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="15.6640625" style="119" customWidth="1"/>
     <col min="33" max="33" width="24" style="119" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="3.6640625" style="119" customWidth="1"/>
-    <col min="35" max="35" width="2.83203125" style="119" customWidth="1"/>
+    <col min="35" max="35" width="2.77734375" style="119" customWidth="1"/>
     <col min="36" max="16384" width="9.33203125" style="119"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="30" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:25" ht="30" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4545,7 +4555,7 @@
       <c r="O1" s="2"/>
       <c r="Y1" s="29"/>
     </row>
-    <row r="2" spans="1:25" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="233" t="s">
         <v>119</v>
@@ -4565,7 +4575,7 @@
       <c r="O2" s="3"/>
       <c r="Y2" s="29"/>
     </row>
-    <row r="3" spans="1:25" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" ht="20" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -4593,7 +4603,7 @@
       <c r="O3" s="156"/>
       <c r="Y3" s="29"/>
     </row>
-    <row r="4" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="10"/>
       <c r="B4" s="11"/>
       <c r="C4" s="5"/>
@@ -4611,7 +4621,7 @@
       <c r="O4" s="3"/>
       <c r="Y4" s="29"/>
     </row>
-    <row r="5" spans="1:25" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" ht="20" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -4637,10 +4647,10 @@
       <c r="O5" s="155"/>
       <c r="Y5" s="29"/>
     </row>
-    <row r="6" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="Y6" s="29"/>
     </row>
-    <row r="7" spans="1:25" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" ht="14" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>6</v>
       </c>
@@ -4659,7 +4669,7 @@
       <c r="M7" s="123"/>
       <c r="Y7" s="29"/>
     </row>
-    <row r="8" spans="1:25" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="16"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4672,7 +4682,7 @@
       <c r="M8" s="126"/>
       <c r="Y8" s="29"/>
     </row>
-    <row r="9" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="127" t="s">
         <v>9</v>
       </c>
@@ -4707,7 +4717,7 @@
       </c>
       <c r="Y9" s="29"/>
     </row>
-    <row r="10" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="132" t="s">
         <v>15</v>
       </c>
@@ -4742,7 +4752,7 @@
       </c>
       <c r="Y10" s="29"/>
     </row>
-    <row r="11" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="132" t="s">
         <v>20</v>
       </c>
@@ -4777,7 +4787,7 @@
       </c>
       <c r="Y11" s="29"/>
     </row>
-    <row r="12" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="132" t="s">
         <v>26</v>
       </c>
@@ -4805,7 +4815,7 @@
       </c>
       <c r="Y12" s="29"/>
     </row>
-    <row r="13" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="132" t="s">
         <v>30</v>
       </c>
@@ -4832,7 +4842,7 @@
       </c>
       <c r="Y13" s="29"/>
     </row>
-    <row r="14" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="135" t="s">
         <v>34</v>
       </c>
@@ -4859,7 +4869,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" ht="14" x14ac:dyDescent="0.3">
       <c r="A15" s="60"/>
       <c r="B15" s="29"/>
       <c r="C15" s="29"/>
@@ -4883,7 +4893,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="17" spans="1:39" ht="18.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" ht="18.5" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A17" s="91" t="s">
         <v>40</v>
       </c>
@@ -4901,7 +4911,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="18" spans="1:39" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="94" t="s">
         <v>42</v>
       </c>
@@ -4919,7 +4929,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="19" spans="1:39" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="96" t="s">
         <v>45</v>
       </c>
@@ -4941,7 +4951,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="20" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="98" t="s">
         <v>48</v>
       </c>
@@ -4955,7 +4965,7 @@
       </c>
       <c r="H20" s="97"/>
     </row>
-    <row r="21" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="99" t="s">
         <v>50</v>
       </c>
@@ -4969,7 +4979,7 @@
       </c>
       <c r="H21" s="97"/>
     </row>
-    <row r="22" spans="1:39" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:39" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="100" t="s">
         <v>52</v>
       </c>
@@ -4983,7 +4993,7 @@
       </c>
       <c r="H22" s="101"/>
     </row>
-    <row r="23" spans="1:39" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:39" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="102" t="s">
         <v>54</v>
       </c>
@@ -4999,7 +5009,7 @@
       </c>
       <c r="H23" s="101"/>
     </row>
-    <row r="24" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="102" t="s">
         <v>56</v>
       </c>
@@ -5015,7 +5025,7 @@
       </c>
       <c r="H24" s="101"/>
     </row>
-    <row r="25" spans="1:39" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:39" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="103" t="s">
         <v>58</v>
       </c>
@@ -5029,7 +5039,7 @@
       <c r="G25" s="105"/>
       <c r="H25" s="106"/>
     </row>
-    <row r="26" spans="1:39" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" ht="10.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="140"/>
       <c r="B26" s="141"/>
       <c r="C26" s="141"/>
@@ -5039,8 +5049,8 @@
       <c r="G26" s="141"/>
       <c r="H26" s="142"/>
     </row>
-    <row r="27" spans="1:39" ht="12" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:39" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:39" ht="10.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:39" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A28" s="217" t="s">
         <v>59</v>
       </c>
@@ -5082,7 +5092,7 @@
       <c r="AJ28" s="218"/>
       <c r="AM28" s="51"/>
     </row>
-    <row r="29" spans="1:39" ht="18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:39" ht="18" x14ac:dyDescent="0.4">
       <c r="A29" s="192"/>
       <c r="B29" s="232"/>
       <c r="C29" s="54" t="s">
@@ -5134,7 +5144,7 @@
       <c r="AK29" s="216"/>
       <c r="AL29" s="193"/>
     </row>
-    <row r="30" spans="1:39" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:39" ht="20" x14ac:dyDescent="0.4">
       <c r="A30" s="230" t="s">
         <v>64</v>
       </c>
@@ -5184,7 +5194,7 @@
       <c r="AK30" s="144"/>
       <c r="AL30" s="145"/>
     </row>
-    <row r="31" spans="1:39" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:39" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A31" s="198" t="s">
         <v>67</v>
       </c>
@@ -5234,7 +5244,7 @@
       <c r="AK31" s="144"/>
       <c r="AL31" s="145"/>
     </row>
-    <row r="32" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:39" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="146"/>
       <c r="B32" s="29"/>
       <c r="C32" s="29"/>
@@ -5258,7 +5268,7 @@
       <c r="AK32" s="144"/>
       <c r="AL32" s="145"/>
     </row>
-    <row r="33" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:38" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="147"/>
       <c r="B33" s="30" t="s">
         <v>71</v>
@@ -5326,7 +5336,7 @@
       <c r="AK33" s="144"/>
       <c r="AL33" s="145"/>
     </row>
-    <row r="34" spans="1:38" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:38" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C34" s="33">
         <v>160</v>
       </c>
@@ -5368,7 +5378,7 @@
       <c r="AK34" s="144"/>
       <c r="AL34" s="145"/>
     </row>
-    <row r="35" spans="1:38" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:38" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C35" s="166"/>
       <c r="D35" s="155"/>
       <c r="G35" s="166"/>
@@ -5428,7 +5438,7 @@
       <c r="AK36" s="149"/>
       <c r="AL36" s="150"/>
     </row>
-    <row r="37" spans="1:38" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:38" ht="18.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="173" t="s">
         <v>79</v>
       </c>
@@ -5462,7 +5472,7 @@
       <c r="AG37" s="75"/>
       <c r="AH37" s="165"/>
     </row>
-    <row r="38" spans="1:38" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:38" ht="36" x14ac:dyDescent="0.4">
       <c r="A38" s="107" t="s">
         <v>80</v>
       </c>
@@ -5542,7 +5552,7 @@
       </c>
       <c r="AH38" s="165"/>
     </row>
-    <row r="39" spans="1:38" ht="30" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:38" ht="31" x14ac:dyDescent="0.35">
       <c r="A39" s="108" t="s">
         <v>92</v>
       </c>
@@ -5622,7 +5632,7 @@
       </c>
       <c r="AH39" s="165"/>
     </row>
-    <row r="40" spans="1:38" ht="20.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:38" ht="20" x14ac:dyDescent="0.35">
       <c r="A40" s="108" t="s">
         <v>101</v>
       </c>
@@ -5696,7 +5706,7 @@
       <c r="AG40" s="40"/>
       <c r="AH40" s="165"/>
     </row>
-    <row r="41" spans="1:38" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:38" ht="20.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="108" t="s">
         <v>105</v>
       </c>
@@ -5768,7 +5778,7 @@
       <c r="AG41" s="40"/>
       <c r="AH41" s="165"/>
     </row>
-    <row r="42" spans="1:38" ht="20.25" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:38" ht="20" x14ac:dyDescent="0.2">
       <c r="A42" s="108" t="s">
         <v>109</v>
       </c>
@@ -5830,7 +5840,7 @@
       <c r="AG42" s="40"/>
       <c r="AH42" s="165"/>
     </row>
-    <row r="43" spans="1:38" ht="21" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:38" ht="20.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="109" t="s">
         <v>112</v>
       </c>
@@ -5896,7 +5906,7 @@
       <c r="AG43" s="43"/>
       <c r="AH43" s="165"/>
     </row>
-    <row r="44" spans="1:38" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:38" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A44" s="174"/>
       <c r="B44" s="44"/>
       <c r="C44" s="18"/>
@@ -5930,7 +5940,7 @@
       <c r="AG44" s="163"/>
       <c r="AH44" s="165"/>
     </row>
-    <row r="45" spans="1:38" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:38" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A45" s="110"/>
       <c r="B45" s="111"/>
       <c r="C45" s="112"/>
@@ -6879,13 +6889,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06F01092-7808-4B5B-B1FD-E5562EA3D919}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06F01092-7808-4B5B-B1FD-E5562EA3D919}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3314f2a4-48e9-4e28-8da9-3bfbc3a74041"/>
+    <ds:schemaRef ds:uri="03fd382f-fd16-45b5-8306-1be73a58e004"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74D37766-22C8-4101-A6A1-3DEEE84685D8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74D37766-22C8-4101-A6A1-3DEEE84685D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49A4B1E7-D809-4F18-8A5B-250753158AE8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49A4B1E7-D809-4F18-8A5B-250753158AE8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="03fd382f-fd16-45b5-8306-1be73a58e004"/>
+    <ds:schemaRef ds:uri="3314f2a4-48e9-4e28-8da9-3bfbc3a74041"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Enhance SQL table creation logic; improve column name handling by adding quotes and removing invalid characters
</commit_message>
<xml_diff>
--- a/datasheets/20250708 Runsheet.xlsx
+++ b/datasheets/20250708 Runsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C376038\Documents\python_code\cvd_sql\datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7A6CBC-6C09-4209-8A03-8D50572C750F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE8F530-BF56-4DD9-ACB4-7148B1684636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="135" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38340" yWindow="2865" windowWidth="14400" windowHeight="7365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Run 1" sheetId="26" r:id="rId1"/>
@@ -1816,6 +1816,114 @@
     <xf numFmtId="0" fontId="22" fillId="2" borderId="58" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="38" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="30" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="39" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="40" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1826,6 +1934,39 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1865,147 +2006,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="16" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="39" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="40" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="38" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="30" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2329,8 +2329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I21" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="V38" sqref="V38"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="40" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47:M47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="10" x14ac:dyDescent="0.2"/>
@@ -2395,12 +2395,12 @@
     </row>
     <row r="2" spans="1:25" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
-      <c r="B2" s="233" t="s">
+      <c r="B2" s="175" t="s">
         <v>119</v>
       </c>
-      <c r="C2" s="233"/>
-      <c r="D2" s="233"/>
-      <c r="E2" s="233"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -2417,21 +2417,21 @@
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="234"/>
-      <c r="C3" s="234"/>
-      <c r="D3" s="234"/>
-      <c r="E3" s="234"/>
+      <c r="B3" s="176"/>
+      <c r="C3" s="176"/>
+      <c r="D3" s="176"/>
+      <c r="E3" s="176"/>
       <c r="F3" s="5"/>
       <c r="G3" s="6"/>
       <c r="H3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="235">
+      <c r="I3" s="177">
         <v>20250708</v>
       </c>
-      <c r="J3" s="235"/>
-      <c r="K3" s="235"/>
-      <c r="L3" s="235"/>
+      <c r="J3" s="177"/>
+      <c r="K3" s="177"/>
+      <c r="L3" s="177"/>
       <c r="M3" s="8" t="s">
         <v>3</v>
       </c>
@@ -2463,25 +2463,25 @@
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="236">
+      <c r="B5" s="178">
         <v>45846</v>
       </c>
-      <c r="C5" s="236"/>
-      <c r="D5" s="236"/>
-      <c r="E5" s="236"/>
+      <c r="C5" s="178"/>
+      <c r="D5" s="178"/>
+      <c r="E5" s="178"/>
       <c r="F5" s="5"/>
       <c r="G5" s="6"/>
       <c r="H5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="235" t="s">
+      <c r="I5" s="177" t="s">
         <v>120</v>
       </c>
-      <c r="J5" s="235"/>
-      <c r="K5" s="235"/>
-      <c r="L5" s="235"/>
-      <c r="M5" s="235"/>
-      <c r="N5" s="235"/>
+      <c r="J5" s="177"/>
+      <c r="K5" s="177"/>
+      <c r="L5" s="177"/>
+      <c r="M5" s="177"/>
+      <c r="N5" s="177"/>
       <c r="O5" s="155"/>
       <c r="Y5" s="29"/>
     </row>
@@ -2539,11 +2539,11 @@
       <c r="F9" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="237" t="s">
+      <c r="G9" s="179" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="238"/>
-      <c r="I9" s="238"/>
+      <c r="H9" s="180"/>
+      <c r="I9" s="180"/>
       <c r="J9" s="19" t="s">
         <v>10</v>
       </c>
@@ -2574,11 +2574,11 @@
       <c r="F10" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="222" t="s">
+      <c r="G10" s="189" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="223"/>
-      <c r="I10" s="223"/>
+      <c r="H10" s="190"/>
+      <c r="I10" s="190"/>
       <c r="J10" s="21" t="s">
         <v>10</v>
       </c>
@@ -2609,11 +2609,11 @@
       <c r="F11" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="224" t="s">
+      <c r="G11" s="191" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="225"/>
-      <c r="I11" s="225"/>
+      <c r="H11" s="192"/>
+      <c r="I11" s="192"/>
       <c r="J11" s="62" t="s">
         <v>10</v>
       </c>
@@ -2774,10 +2774,10 @@
       <c r="B19" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="194" t="s">
+      <c r="E19" s="221" t="s">
         <v>46</v>
       </c>
-      <c r="F19" s="195"/>
+      <c r="F19" s="222"/>
       <c r="G19" s="20">
         <v>200</v>
       </c>
@@ -2794,10 +2794,10 @@
         <v>48</v>
       </c>
       <c r="B20" s="21"/>
-      <c r="E20" s="196" t="s">
+      <c r="E20" s="223" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="197"/>
+      <c r="F20" s="224"/>
       <c r="G20" s="22">
         <v>100</v>
       </c>
@@ -2808,10 +2808,10 @@
         <v>50</v>
       </c>
       <c r="B21" s="65"/>
-      <c r="E21" s="196" t="s">
+      <c r="E21" s="223" t="s">
         <v>51</v>
       </c>
-      <c r="F21" s="197"/>
+      <c r="F21" s="224"/>
       <c r="G21" s="22">
         <v>50</v>
       </c>
@@ -2822,10 +2822,10 @@
         <v>52</v>
       </c>
       <c r="B22" s="66"/>
-      <c r="E22" s="196" t="s">
+      <c r="E22" s="223" t="s">
         <v>53</v>
       </c>
-      <c r="F22" s="197"/>
+      <c r="F22" s="224"/>
       <c r="G22" s="23">
         <v>120</v>
       </c>
@@ -2838,10 +2838,10 @@
       <c r="B23" s="24">
         <v>5</v>
       </c>
-      <c r="E23" s="196" t="s">
+      <c r="E23" s="223" t="s">
         <v>55</v>
       </c>
-      <c r="F23" s="197"/>
+      <c r="F23" s="224"/>
       <c r="G23" s="23">
         <v>200</v>
       </c>
@@ -2854,10 +2854,10 @@
       <c r="B24" s="24">
         <v>5</v>
       </c>
-      <c r="E24" s="184" t="s">
+      <c r="E24" s="231" t="s">
         <v>57</v>
       </c>
-      <c r="F24" s="185"/>
+      <c r="F24" s="232"/>
       <c r="G24" s="25">
         <v>0.03</v>
       </c>
@@ -2889,50 +2889,50 @@
     </row>
     <row r="27" spans="1:39" ht="10.5" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="1:39" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="217" t="s">
+      <c r="A28" s="184" t="s">
         <v>59</v>
       </c>
-      <c r="B28" s="217"/>
-      <c r="C28" s="217"/>
-      <c r="D28" s="217"/>
-      <c r="E28" s="217"/>
-      <c r="F28" s="217"/>
-      <c r="G28" s="218"/>
-      <c r="H28" s="218"/>
-      <c r="I28" s="218"/>
-      <c r="J28" s="218"/>
-      <c r="K28" s="218"/>
-      <c r="L28" s="218"/>
-      <c r="M28" s="218"/>
-      <c r="N28" s="218"/>
-      <c r="O28" s="218"/>
-      <c r="P28" s="218"/>
-      <c r="Q28" s="218"/>
-      <c r="R28" s="218"/>
-      <c r="S28" s="218"/>
-      <c r="U28" s="218" t="s">
+      <c r="B28" s="184"/>
+      <c r="C28" s="184"/>
+      <c r="D28" s="184"/>
+      <c r="E28" s="184"/>
+      <c r="F28" s="184"/>
+      <c r="G28" s="185"/>
+      <c r="H28" s="185"/>
+      <c r="I28" s="185"/>
+      <c r="J28" s="185"/>
+      <c r="K28" s="185"/>
+      <c r="L28" s="185"/>
+      <c r="M28" s="185"/>
+      <c r="N28" s="185"/>
+      <c r="O28" s="185"/>
+      <c r="P28" s="185"/>
+      <c r="Q28" s="185"/>
+      <c r="R28" s="185"/>
+      <c r="S28" s="185"/>
+      <c r="U28" s="185" t="s">
         <v>60</v>
       </c>
-      <c r="V28" s="218"/>
-      <c r="W28" s="218"/>
-      <c r="X28" s="218"/>
-      <c r="Y28" s="218"/>
-      <c r="Z28" s="218"/>
-      <c r="AA28" s="218"/>
-      <c r="AB28" s="218"/>
-      <c r="AC28" s="218"/>
-      <c r="AD28" s="218"/>
-      <c r="AE28" s="218"/>
-      <c r="AF28" s="218"/>
-      <c r="AG28" s="218"/>
-      <c r="AH28" s="218"/>
-      <c r="AI28" s="218"/>
-      <c r="AJ28" s="218"/>
+      <c r="V28" s="185"/>
+      <c r="W28" s="185"/>
+      <c r="X28" s="185"/>
+      <c r="Y28" s="185"/>
+      <c r="Z28" s="185"/>
+      <c r="AA28" s="185"/>
+      <c r="AB28" s="185"/>
+      <c r="AC28" s="185"/>
+      <c r="AD28" s="185"/>
+      <c r="AE28" s="185"/>
+      <c r="AF28" s="185"/>
+      <c r="AG28" s="185"/>
+      <c r="AH28" s="185"/>
+      <c r="AI28" s="185"/>
+      <c r="AJ28" s="185"/>
       <c r="AM28" s="51"/>
     </row>
     <row r="29" spans="1:39" ht="18" x14ac:dyDescent="0.4">
-      <c r="A29" s="192"/>
-      <c r="B29" s="232"/>
+      <c r="A29" s="181"/>
+      <c r="B29" s="199"/>
       <c r="C29" s="54" t="s">
         <v>61</v>
       </c>
@@ -2945,19 +2945,19 @@
       <c r="F29" s="28">
         <v>3</v>
       </c>
-      <c r="L29" s="192" t="s">
+      <c r="L29" s="181" t="s">
         <v>127</v>
       </c>
-      <c r="M29" s="193"/>
+      <c r="M29" s="183"/>
       <c r="N29" s="157"/>
       <c r="O29" s="158"/>
-      <c r="P29" s="192" t="s">
+      <c r="P29" s="181" t="s">
         <v>63</v>
       </c>
-      <c r="Q29" s="216"/>
-      <c r="R29" s="193"/>
-      <c r="U29" s="186"/>
-      <c r="V29" s="187"/>
+      <c r="Q29" s="182"/>
+      <c r="R29" s="183"/>
+      <c r="U29" s="233"/>
+      <c r="V29" s="234"/>
       <c r="W29" s="54" t="s">
         <v>61</v>
       </c>
@@ -2971,22 +2971,22 @@
         <v>3</v>
       </c>
       <c r="AE29" s="121"/>
-      <c r="AF29" s="192" t="s">
+      <c r="AF29" s="181" t="s">
         <v>62</v>
       </c>
-      <c r="AG29" s="193"/>
+      <c r="AG29" s="183"/>
       <c r="AH29" s="153"/>
-      <c r="AJ29" s="192" t="s">
+      <c r="AJ29" s="181" t="s">
         <v>63</v>
       </c>
-      <c r="AK29" s="216"/>
-      <c r="AL29" s="193"/>
+      <c r="AK29" s="182"/>
+      <c r="AL29" s="183"/>
     </row>
     <row r="30" spans="1:39" ht="20" x14ac:dyDescent="0.4">
-      <c r="A30" s="230" t="s">
+      <c r="A30" s="197" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="231"/>
+      <c r="B30" s="198"/>
       <c r="C30" s="52">
         <v>6</v>
       </c>
@@ -3010,12 +3010,12 @@
       <c r="P30" s="125" t="s">
         <v>66</v>
       </c>
-      <c r="Q30" s="226"/>
-      <c r="R30" s="227"/>
-      <c r="U30" s="188" t="s">
+      <c r="Q30" s="193"/>
+      <c r="R30" s="194"/>
+      <c r="U30" s="235" t="s">
         <v>64</v>
       </c>
-      <c r="V30" s="189"/>
+      <c r="V30" s="236"/>
       <c r="W30" s="52"/>
       <c r="X30" s="53"/>
       <c r="Y30" s="53"/>
@@ -3033,10 +3033,10 @@
       <c r="AL30" s="145"/>
     </row>
     <row r="31" spans="1:39" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="198" t="s">
+      <c r="A31" s="200" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="199"/>
+      <c r="B31" s="201"/>
       <c r="C31" s="56">
         <v>46.2</v>
       </c>
@@ -3060,12 +3060,12 @@
       <c r="P31" s="125" t="s">
         <v>69</v>
       </c>
-      <c r="Q31" s="226"/>
-      <c r="R31" s="227"/>
-      <c r="U31" s="190" t="s">
+      <c r="Q31" s="193"/>
+      <c r="R31" s="194"/>
+      <c r="U31" s="237" t="s">
         <v>67</v>
       </c>
-      <c r="V31" s="191"/>
+      <c r="V31" s="238"/>
       <c r="W31" s="56"/>
       <c r="X31" s="56"/>
       <c r="Y31" s="56"/>
@@ -3092,8 +3092,8 @@
       <c r="P32" s="125" t="s">
         <v>70</v>
       </c>
-      <c r="Q32" s="226"/>
-      <c r="R32" s="227"/>
+      <c r="Q32" s="193"/>
+      <c r="R32" s="194"/>
       <c r="U32" s="146"/>
       <c r="V32" s="29"/>
       <c r="W32" s="29"/>
@@ -3138,8 +3138,8 @@
       <c r="P33" s="125" t="s">
         <v>76</v>
       </c>
-      <c r="Q33" s="226"/>
-      <c r="R33" s="227"/>
+      <c r="Q33" s="193"/>
+      <c r="R33" s="194"/>
       <c r="U33" s="147"/>
       <c r="V33" s="30" t="s">
         <v>71</v>
@@ -3196,8 +3196,8 @@
       <c r="P34" s="125" t="s">
         <v>77</v>
       </c>
-      <c r="Q34" s="226"/>
-      <c r="R34" s="227"/>
+      <c r="Q34" s="193"/>
+      <c r="R34" s="194"/>
       <c r="W34" s="33">
         <v>160</v>
       </c>
@@ -3254,8 +3254,8 @@
       <c r="P36" s="148" t="s">
         <v>78</v>
       </c>
-      <c r="Q36" s="228"/>
-      <c r="R36" s="229"/>
+      <c r="Q36" s="195"/>
+      <c r="R36" s="196"/>
       <c r="U36" s="169"/>
       <c r="V36" s="170"/>
       <c r="W36" s="170"/>
@@ -3349,12 +3349,12 @@
         <v>90</v>
       </c>
       <c r="N38" s="165"/>
-      <c r="P38" s="219" t="s">
+      <c r="P38" s="186" t="s">
         <v>91</v>
       </c>
-      <c r="Q38" s="220"/>
-      <c r="R38" s="220"/>
-      <c r="S38" s="221"/>
+      <c r="Q38" s="187"/>
+      <c r="R38" s="187"/>
+      <c r="S38" s="188"/>
       <c r="U38" s="107" t="s">
         <v>80</v>
       </c>
@@ -3814,527 +3814,527 @@
     </row>
     <row r="46" spans="1:38" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="1:38" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="206" t="s">
+      <c r="A47" s="208" t="s">
         <v>116</v>
       </c>
-      <c r="B47" s="207"/>
-      <c r="C47" s="207"/>
-      <c r="D47" s="207"/>
-      <c r="E47" s="208"/>
-      <c r="F47" s="175" t="s">
+      <c r="B47" s="209"/>
+      <c r="C47" s="209"/>
+      <c r="D47" s="209"/>
+      <c r="E47" s="210"/>
+      <c r="F47" s="211" t="s">
         <v>117</v>
       </c>
-      <c r="G47" s="176"/>
-      <c r="H47" s="176"/>
-      <c r="I47" s="176"/>
-      <c r="J47" s="176"/>
-      <c r="K47" s="176"/>
-      <c r="L47" s="176"/>
-      <c r="M47" s="177"/>
+      <c r="G47" s="212"/>
+      <c r="H47" s="212"/>
+      <c r="I47" s="212"/>
+      <c r="J47" s="212"/>
+      <c r="K47" s="212"/>
+      <c r="L47" s="212"/>
+      <c r="M47" s="213"/>
       <c r="N47" s="50"/>
       <c r="O47" s="49"/>
-      <c r="U47" s="206" t="s">
+      <c r="U47" s="208" t="s">
         <v>118</v>
       </c>
-      <c r="V47" s="207"/>
-      <c r="W47" s="207"/>
-      <c r="X47" s="207"/>
-      <c r="Y47" s="208"/>
-      <c r="Z47" s="175" t="s">
+      <c r="V47" s="209"/>
+      <c r="W47" s="209"/>
+      <c r="X47" s="209"/>
+      <c r="Y47" s="210"/>
+      <c r="Z47" s="211" t="s">
         <v>117</v>
       </c>
-      <c r="AA47" s="176"/>
-      <c r="AB47" s="176"/>
-      <c r="AC47" s="176"/>
-      <c r="AD47" s="176"/>
-      <c r="AE47" s="176"/>
-      <c r="AF47" s="176"/>
-      <c r="AG47" s="176"/>
-      <c r="AH47" s="177"/>
+      <c r="AA47" s="212"/>
+      <c r="AB47" s="212"/>
+      <c r="AC47" s="212"/>
+      <c r="AD47" s="212"/>
+      <c r="AE47" s="212"/>
+      <c r="AF47" s="212"/>
+      <c r="AG47" s="212"/>
+      <c r="AH47" s="213"/>
       <c r="AI47" s="50"/>
     </row>
     <row r="48" spans="1:38" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="200" t="s">
+      <c r="A48" s="202" t="s">
         <v>124</v>
       </c>
-      <c r="B48" s="201"/>
-      <c r="C48" s="201"/>
-      <c r="D48" s="201"/>
-      <c r="E48" s="202"/>
-      <c r="F48" s="209" t="s">
+      <c r="B48" s="203"/>
+      <c r="C48" s="203"/>
+      <c r="D48" s="203"/>
+      <c r="E48" s="204"/>
+      <c r="F48" s="214" t="s">
         <v>122</v>
       </c>
-      <c r="G48" s="210"/>
-      <c r="H48" s="210"/>
-      <c r="I48" s="210"/>
-      <c r="J48" s="210"/>
-      <c r="K48" s="210"/>
-      <c r="L48" s="210"/>
-      <c r="M48" s="211"/>
+      <c r="G48" s="215"/>
+      <c r="H48" s="215"/>
+      <c r="I48" s="215"/>
+      <c r="J48" s="215"/>
+      <c r="K48" s="215"/>
+      <c r="L48" s="215"/>
+      <c r="M48" s="216"/>
       <c r="N48" s="50"/>
       <c r="O48" s="49"/>
-      <c r="U48" s="200"/>
-      <c r="V48" s="201"/>
-      <c r="W48" s="201"/>
-      <c r="X48" s="201"/>
-      <c r="Y48" s="202"/>
-      <c r="Z48" s="178"/>
-      <c r="AA48" s="179"/>
-      <c r="AB48" s="179"/>
-      <c r="AC48" s="179"/>
-      <c r="AD48" s="179"/>
-      <c r="AE48" s="179"/>
-      <c r="AF48" s="179"/>
-      <c r="AG48" s="179"/>
-      <c r="AH48" s="180"/>
+      <c r="U48" s="202"/>
+      <c r="V48" s="203"/>
+      <c r="W48" s="203"/>
+      <c r="X48" s="203"/>
+      <c r="Y48" s="204"/>
+      <c r="Z48" s="225"/>
+      <c r="AA48" s="226"/>
+      <c r="AB48" s="226"/>
+      <c r="AC48" s="226"/>
+      <c r="AD48" s="226"/>
+      <c r="AE48" s="226"/>
+      <c r="AF48" s="226"/>
+      <c r="AG48" s="226"/>
+      <c r="AH48" s="227"/>
       <c r="AI48" s="50"/>
     </row>
     <row r="49" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="200"/>
-      <c r="B49" s="201"/>
-      <c r="C49" s="201"/>
-      <c r="D49" s="201"/>
-      <c r="E49" s="202"/>
-      <c r="F49" s="212"/>
-      <c r="G49" s="210"/>
-      <c r="H49" s="210"/>
-      <c r="I49" s="210"/>
-      <c r="J49" s="210"/>
-      <c r="K49" s="210"/>
-      <c r="L49" s="210"/>
-      <c r="M49" s="211"/>
+      <c r="A49" s="202"/>
+      <c r="B49" s="203"/>
+      <c r="C49" s="203"/>
+      <c r="D49" s="203"/>
+      <c r="E49" s="204"/>
+      <c r="F49" s="217"/>
+      <c r="G49" s="215"/>
+      <c r="H49" s="215"/>
+      <c r="I49" s="215"/>
+      <c r="J49" s="215"/>
+      <c r="K49" s="215"/>
+      <c r="L49" s="215"/>
+      <c r="M49" s="216"/>
       <c r="N49" s="50"/>
       <c r="O49" s="49"/>
-      <c r="U49" s="200"/>
-      <c r="V49" s="201"/>
-      <c r="W49" s="201"/>
-      <c r="X49" s="201"/>
-      <c r="Y49" s="202"/>
-      <c r="Z49" s="178"/>
-      <c r="AA49" s="179"/>
-      <c r="AB49" s="179"/>
-      <c r="AC49" s="179"/>
-      <c r="AD49" s="179"/>
-      <c r="AE49" s="179"/>
-      <c r="AF49" s="179"/>
-      <c r="AG49" s="179"/>
-      <c r="AH49" s="180"/>
+      <c r="U49" s="202"/>
+      <c r="V49" s="203"/>
+      <c r="W49" s="203"/>
+      <c r="X49" s="203"/>
+      <c r="Y49" s="204"/>
+      <c r="Z49" s="225"/>
+      <c r="AA49" s="226"/>
+      <c r="AB49" s="226"/>
+      <c r="AC49" s="226"/>
+      <c r="AD49" s="226"/>
+      <c r="AE49" s="226"/>
+      <c r="AF49" s="226"/>
+      <c r="AG49" s="226"/>
+      <c r="AH49" s="227"/>
       <c r="AI49" s="50"/>
     </row>
     <row r="50" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="200"/>
-      <c r="B50" s="201"/>
-      <c r="C50" s="201"/>
-      <c r="D50" s="201"/>
-      <c r="E50" s="202"/>
-      <c r="F50" s="212"/>
-      <c r="G50" s="210"/>
-      <c r="H50" s="210"/>
-      <c r="I50" s="210"/>
-      <c r="J50" s="210"/>
-      <c r="K50" s="210"/>
-      <c r="L50" s="210"/>
-      <c r="M50" s="211"/>
+      <c r="A50" s="202"/>
+      <c r="B50" s="203"/>
+      <c r="C50" s="203"/>
+      <c r="D50" s="203"/>
+      <c r="E50" s="204"/>
+      <c r="F50" s="217"/>
+      <c r="G50" s="215"/>
+      <c r="H50" s="215"/>
+      <c r="I50" s="215"/>
+      <c r="J50" s="215"/>
+      <c r="K50" s="215"/>
+      <c r="L50" s="215"/>
+      <c r="M50" s="216"/>
       <c r="N50" s="50"/>
       <c r="O50" s="49"/>
-      <c r="U50" s="200"/>
-      <c r="V50" s="201"/>
-      <c r="W50" s="201"/>
-      <c r="X50" s="201"/>
-      <c r="Y50" s="202"/>
-      <c r="Z50" s="178"/>
-      <c r="AA50" s="179"/>
-      <c r="AB50" s="179"/>
-      <c r="AC50" s="179"/>
-      <c r="AD50" s="179"/>
-      <c r="AE50" s="179"/>
-      <c r="AF50" s="179"/>
-      <c r="AG50" s="179"/>
-      <c r="AH50" s="180"/>
+      <c r="U50" s="202"/>
+      <c r="V50" s="203"/>
+      <c r="W50" s="203"/>
+      <c r="X50" s="203"/>
+      <c r="Y50" s="204"/>
+      <c r="Z50" s="225"/>
+      <c r="AA50" s="226"/>
+      <c r="AB50" s="226"/>
+      <c r="AC50" s="226"/>
+      <c r="AD50" s="226"/>
+      <c r="AE50" s="226"/>
+      <c r="AF50" s="226"/>
+      <c r="AG50" s="226"/>
+      <c r="AH50" s="227"/>
       <c r="AI50" s="50"/>
     </row>
     <row r="51" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="200"/>
-      <c r="B51" s="201"/>
-      <c r="C51" s="201"/>
-      <c r="D51" s="201"/>
-      <c r="E51" s="202"/>
-      <c r="F51" s="212"/>
-      <c r="G51" s="210"/>
-      <c r="H51" s="210"/>
-      <c r="I51" s="210"/>
-      <c r="J51" s="210"/>
-      <c r="K51" s="210"/>
-      <c r="L51" s="210"/>
-      <c r="M51" s="211"/>
+      <c r="A51" s="202"/>
+      <c r="B51" s="203"/>
+      <c r="C51" s="203"/>
+      <c r="D51" s="203"/>
+      <c r="E51" s="204"/>
+      <c r="F51" s="217"/>
+      <c r="G51" s="215"/>
+      <c r="H51" s="215"/>
+      <c r="I51" s="215"/>
+      <c r="J51" s="215"/>
+      <c r="K51" s="215"/>
+      <c r="L51" s="215"/>
+      <c r="M51" s="216"/>
       <c r="N51" s="50"/>
       <c r="O51" s="49"/>
-      <c r="U51" s="200"/>
-      <c r="V51" s="201"/>
-      <c r="W51" s="201"/>
-      <c r="X51" s="201"/>
-      <c r="Y51" s="202"/>
-      <c r="Z51" s="178"/>
-      <c r="AA51" s="179"/>
-      <c r="AB51" s="179"/>
-      <c r="AC51" s="179"/>
-      <c r="AD51" s="179"/>
-      <c r="AE51" s="179"/>
-      <c r="AF51" s="179"/>
-      <c r="AG51" s="179"/>
-      <c r="AH51" s="180"/>
+      <c r="U51" s="202"/>
+      <c r="V51" s="203"/>
+      <c r="W51" s="203"/>
+      <c r="X51" s="203"/>
+      <c r="Y51" s="204"/>
+      <c r="Z51" s="225"/>
+      <c r="AA51" s="226"/>
+      <c r="AB51" s="226"/>
+      <c r="AC51" s="226"/>
+      <c r="AD51" s="226"/>
+      <c r="AE51" s="226"/>
+      <c r="AF51" s="226"/>
+      <c r="AG51" s="226"/>
+      <c r="AH51" s="227"/>
       <c r="AI51" s="50"/>
     </row>
     <row r="52" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="200"/>
-      <c r="B52" s="201"/>
-      <c r="C52" s="201"/>
-      <c r="D52" s="201"/>
-      <c r="E52" s="202"/>
-      <c r="F52" s="212"/>
-      <c r="G52" s="210"/>
-      <c r="H52" s="210"/>
-      <c r="I52" s="210"/>
-      <c r="J52" s="210"/>
-      <c r="K52" s="210"/>
-      <c r="L52" s="210"/>
-      <c r="M52" s="211"/>
+      <c r="A52" s="202"/>
+      <c r="B52" s="203"/>
+      <c r="C52" s="203"/>
+      <c r="D52" s="203"/>
+      <c r="E52" s="204"/>
+      <c r="F52" s="217"/>
+      <c r="G52" s="215"/>
+      <c r="H52" s="215"/>
+      <c r="I52" s="215"/>
+      <c r="J52" s="215"/>
+      <c r="K52" s="215"/>
+      <c r="L52" s="215"/>
+      <c r="M52" s="216"/>
       <c r="N52" s="50"/>
       <c r="O52" s="49"/>
-      <c r="U52" s="200"/>
-      <c r="V52" s="201"/>
-      <c r="W52" s="201"/>
-      <c r="X52" s="201"/>
-      <c r="Y52" s="202"/>
-      <c r="Z52" s="178"/>
-      <c r="AA52" s="179"/>
-      <c r="AB52" s="179"/>
-      <c r="AC52" s="179"/>
-      <c r="AD52" s="179"/>
-      <c r="AE52" s="179"/>
-      <c r="AF52" s="179"/>
-      <c r="AG52" s="179"/>
-      <c r="AH52" s="180"/>
+      <c r="U52" s="202"/>
+      <c r="V52" s="203"/>
+      <c r="W52" s="203"/>
+      <c r="X52" s="203"/>
+      <c r="Y52" s="204"/>
+      <c r="Z52" s="225"/>
+      <c r="AA52" s="226"/>
+      <c r="AB52" s="226"/>
+      <c r="AC52" s="226"/>
+      <c r="AD52" s="226"/>
+      <c r="AE52" s="226"/>
+      <c r="AF52" s="226"/>
+      <c r="AG52" s="226"/>
+      <c r="AH52" s="227"/>
       <c r="AI52" s="50"/>
     </row>
     <row r="53" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="200"/>
-      <c r="B53" s="201"/>
-      <c r="C53" s="201"/>
-      <c r="D53" s="201"/>
-      <c r="E53" s="202"/>
-      <c r="F53" s="212"/>
-      <c r="G53" s="210"/>
-      <c r="H53" s="210"/>
-      <c r="I53" s="210"/>
-      <c r="J53" s="210"/>
-      <c r="K53" s="210"/>
-      <c r="L53" s="210"/>
-      <c r="M53" s="211"/>
+      <c r="A53" s="202"/>
+      <c r="B53" s="203"/>
+      <c r="C53" s="203"/>
+      <c r="D53" s="203"/>
+      <c r="E53" s="204"/>
+      <c r="F53" s="217"/>
+      <c r="G53" s="215"/>
+      <c r="H53" s="215"/>
+      <c r="I53" s="215"/>
+      <c r="J53" s="215"/>
+      <c r="K53" s="215"/>
+      <c r="L53" s="215"/>
+      <c r="M53" s="216"/>
       <c r="N53" s="50"/>
       <c r="O53" s="49"/>
-      <c r="U53" s="200"/>
-      <c r="V53" s="201"/>
-      <c r="W53" s="201"/>
-      <c r="X53" s="201"/>
-      <c r="Y53" s="202"/>
-      <c r="Z53" s="178"/>
-      <c r="AA53" s="179"/>
-      <c r="AB53" s="179"/>
-      <c r="AC53" s="179"/>
-      <c r="AD53" s="179"/>
-      <c r="AE53" s="179"/>
-      <c r="AF53" s="179"/>
-      <c r="AG53" s="179"/>
-      <c r="AH53" s="180"/>
+      <c r="U53" s="202"/>
+      <c r="V53" s="203"/>
+      <c r="W53" s="203"/>
+      <c r="X53" s="203"/>
+      <c r="Y53" s="204"/>
+      <c r="Z53" s="225"/>
+      <c r="AA53" s="226"/>
+      <c r="AB53" s="226"/>
+      <c r="AC53" s="226"/>
+      <c r="AD53" s="226"/>
+      <c r="AE53" s="226"/>
+      <c r="AF53" s="226"/>
+      <c r="AG53" s="226"/>
+      <c r="AH53" s="227"/>
       <c r="AI53" s="50"/>
     </row>
     <row r="54" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="200"/>
-      <c r="B54" s="201"/>
-      <c r="C54" s="201"/>
-      <c r="D54" s="201"/>
-      <c r="E54" s="202"/>
-      <c r="F54" s="212"/>
-      <c r="G54" s="210"/>
-      <c r="H54" s="210"/>
-      <c r="I54" s="210"/>
-      <c r="J54" s="210"/>
-      <c r="K54" s="210"/>
-      <c r="L54" s="210"/>
-      <c r="M54" s="211"/>
+      <c r="A54" s="202"/>
+      <c r="B54" s="203"/>
+      <c r="C54" s="203"/>
+      <c r="D54" s="203"/>
+      <c r="E54" s="204"/>
+      <c r="F54" s="217"/>
+      <c r="G54" s="215"/>
+      <c r="H54" s="215"/>
+      <c r="I54" s="215"/>
+      <c r="J54" s="215"/>
+      <c r="K54" s="215"/>
+      <c r="L54" s="215"/>
+      <c r="M54" s="216"/>
       <c r="N54" s="50"/>
       <c r="O54" s="49"/>
-      <c r="U54" s="200"/>
-      <c r="V54" s="201"/>
-      <c r="W54" s="201"/>
-      <c r="X54" s="201"/>
-      <c r="Y54" s="202"/>
-      <c r="Z54" s="178"/>
-      <c r="AA54" s="179"/>
-      <c r="AB54" s="179"/>
-      <c r="AC54" s="179"/>
-      <c r="AD54" s="179"/>
-      <c r="AE54" s="179"/>
-      <c r="AF54" s="179"/>
-      <c r="AG54" s="179"/>
-      <c r="AH54" s="180"/>
+      <c r="U54" s="202"/>
+      <c r="V54" s="203"/>
+      <c r="W54" s="203"/>
+      <c r="X54" s="203"/>
+      <c r="Y54" s="204"/>
+      <c r="Z54" s="225"/>
+      <c r="AA54" s="226"/>
+      <c r="AB54" s="226"/>
+      <c r="AC54" s="226"/>
+      <c r="AD54" s="226"/>
+      <c r="AE54" s="226"/>
+      <c r="AF54" s="226"/>
+      <c r="AG54" s="226"/>
+      <c r="AH54" s="227"/>
       <c r="AI54" s="50"/>
     </row>
     <row r="55" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="200"/>
-      <c r="B55" s="201"/>
-      <c r="C55" s="201"/>
-      <c r="D55" s="201"/>
-      <c r="E55" s="202"/>
-      <c r="F55" s="212"/>
-      <c r="G55" s="210"/>
-      <c r="H55" s="210"/>
-      <c r="I55" s="210"/>
-      <c r="J55" s="210"/>
-      <c r="K55" s="210"/>
-      <c r="L55" s="210"/>
-      <c r="M55" s="211"/>
+      <c r="A55" s="202"/>
+      <c r="B55" s="203"/>
+      <c r="C55" s="203"/>
+      <c r="D55" s="203"/>
+      <c r="E55" s="204"/>
+      <c r="F55" s="217"/>
+      <c r="G55" s="215"/>
+      <c r="H55" s="215"/>
+      <c r="I55" s="215"/>
+      <c r="J55" s="215"/>
+      <c r="K55" s="215"/>
+      <c r="L55" s="215"/>
+      <c r="M55" s="216"/>
       <c r="N55" s="50"/>
       <c r="O55" s="49"/>
-      <c r="U55" s="200"/>
-      <c r="V55" s="201"/>
-      <c r="W55" s="201"/>
-      <c r="X55" s="201"/>
-      <c r="Y55" s="202"/>
-      <c r="Z55" s="178"/>
-      <c r="AA55" s="179"/>
-      <c r="AB55" s="179"/>
-      <c r="AC55" s="179"/>
-      <c r="AD55" s="179"/>
-      <c r="AE55" s="179"/>
-      <c r="AF55" s="179"/>
-      <c r="AG55" s="179"/>
-      <c r="AH55" s="180"/>
+      <c r="U55" s="202"/>
+      <c r="V55" s="203"/>
+      <c r="W55" s="203"/>
+      <c r="X55" s="203"/>
+      <c r="Y55" s="204"/>
+      <c r="Z55" s="225"/>
+      <c r="AA55" s="226"/>
+      <c r="AB55" s="226"/>
+      <c r="AC55" s="226"/>
+      <c r="AD55" s="226"/>
+      <c r="AE55" s="226"/>
+      <c r="AF55" s="226"/>
+      <c r="AG55" s="226"/>
+      <c r="AH55" s="227"/>
       <c r="AI55" s="50"/>
     </row>
     <row r="56" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="200"/>
-      <c r="B56" s="201"/>
-      <c r="C56" s="201"/>
-      <c r="D56" s="201"/>
-      <c r="E56" s="202"/>
-      <c r="F56" s="212"/>
-      <c r="G56" s="210"/>
-      <c r="H56" s="210"/>
-      <c r="I56" s="210"/>
-      <c r="J56" s="210"/>
-      <c r="K56" s="210"/>
-      <c r="L56" s="210"/>
-      <c r="M56" s="211"/>
+      <c r="A56" s="202"/>
+      <c r="B56" s="203"/>
+      <c r="C56" s="203"/>
+      <c r="D56" s="203"/>
+      <c r="E56" s="204"/>
+      <c r="F56" s="217"/>
+      <c r="G56" s="215"/>
+      <c r="H56" s="215"/>
+      <c r="I56" s="215"/>
+      <c r="J56" s="215"/>
+      <c r="K56" s="215"/>
+      <c r="L56" s="215"/>
+      <c r="M56" s="216"/>
       <c r="N56" s="50"/>
       <c r="O56" s="49"/>
-      <c r="U56" s="200"/>
-      <c r="V56" s="201"/>
-      <c r="W56" s="201"/>
-      <c r="X56" s="201"/>
-      <c r="Y56" s="202"/>
-      <c r="Z56" s="178"/>
-      <c r="AA56" s="179"/>
-      <c r="AB56" s="179"/>
-      <c r="AC56" s="179"/>
-      <c r="AD56" s="179"/>
-      <c r="AE56" s="179"/>
-      <c r="AF56" s="179"/>
-      <c r="AG56" s="179"/>
-      <c r="AH56" s="180"/>
+      <c r="U56" s="202"/>
+      <c r="V56" s="203"/>
+      <c r="W56" s="203"/>
+      <c r="X56" s="203"/>
+      <c r="Y56" s="204"/>
+      <c r="Z56" s="225"/>
+      <c r="AA56" s="226"/>
+      <c r="AB56" s="226"/>
+      <c r="AC56" s="226"/>
+      <c r="AD56" s="226"/>
+      <c r="AE56" s="226"/>
+      <c r="AF56" s="226"/>
+      <c r="AG56" s="226"/>
+      <c r="AH56" s="227"/>
       <c r="AI56" s="50"/>
     </row>
     <row r="57" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="200"/>
-      <c r="B57" s="201"/>
-      <c r="C57" s="201"/>
-      <c r="D57" s="201"/>
-      <c r="E57" s="202"/>
-      <c r="F57" s="212"/>
-      <c r="G57" s="210"/>
-      <c r="H57" s="210"/>
-      <c r="I57" s="210"/>
-      <c r="J57" s="210"/>
-      <c r="K57" s="210"/>
-      <c r="L57" s="210"/>
-      <c r="M57" s="211"/>
+      <c r="A57" s="202"/>
+      <c r="B57" s="203"/>
+      <c r="C57" s="203"/>
+      <c r="D57" s="203"/>
+      <c r="E57" s="204"/>
+      <c r="F57" s="217"/>
+      <c r="G57" s="215"/>
+      <c r="H57" s="215"/>
+      <c r="I57" s="215"/>
+      <c r="J57" s="215"/>
+      <c r="K57" s="215"/>
+      <c r="L57" s="215"/>
+      <c r="M57" s="216"/>
       <c r="N57" s="50"/>
       <c r="O57" s="49"/>
-      <c r="U57" s="200"/>
-      <c r="V57" s="201"/>
-      <c r="W57" s="201"/>
-      <c r="X57" s="201"/>
-      <c r="Y57" s="202"/>
-      <c r="Z57" s="178"/>
-      <c r="AA57" s="179"/>
-      <c r="AB57" s="179"/>
-      <c r="AC57" s="179"/>
-      <c r="AD57" s="179"/>
-      <c r="AE57" s="179"/>
-      <c r="AF57" s="179"/>
-      <c r="AG57" s="179"/>
-      <c r="AH57" s="180"/>
+      <c r="U57" s="202"/>
+      <c r="V57" s="203"/>
+      <c r="W57" s="203"/>
+      <c r="X57" s="203"/>
+      <c r="Y57" s="204"/>
+      <c r="Z57" s="225"/>
+      <c r="AA57" s="226"/>
+      <c r="AB57" s="226"/>
+      <c r="AC57" s="226"/>
+      <c r="AD57" s="226"/>
+      <c r="AE57" s="226"/>
+      <c r="AF57" s="226"/>
+      <c r="AG57" s="226"/>
+      <c r="AH57" s="227"/>
       <c r="AI57" s="50"/>
     </row>
     <row r="58" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="200"/>
-      <c r="B58" s="201"/>
-      <c r="C58" s="201"/>
-      <c r="D58" s="201"/>
-      <c r="E58" s="202"/>
-      <c r="F58" s="212"/>
-      <c r="G58" s="210"/>
-      <c r="H58" s="210"/>
-      <c r="I58" s="210"/>
-      <c r="J58" s="210"/>
-      <c r="K58" s="210"/>
-      <c r="L58" s="210"/>
-      <c r="M58" s="211"/>
+      <c r="A58" s="202"/>
+      <c r="B58" s="203"/>
+      <c r="C58" s="203"/>
+      <c r="D58" s="203"/>
+      <c r="E58" s="204"/>
+      <c r="F58" s="217"/>
+      <c r="G58" s="215"/>
+      <c r="H58" s="215"/>
+      <c r="I58" s="215"/>
+      <c r="J58" s="215"/>
+      <c r="K58" s="215"/>
+      <c r="L58" s="215"/>
+      <c r="M58" s="216"/>
       <c r="N58" s="50"/>
       <c r="O58" s="49"/>
-      <c r="U58" s="200"/>
-      <c r="V58" s="201"/>
-      <c r="W58" s="201"/>
-      <c r="X58" s="201"/>
-      <c r="Y58" s="202"/>
-      <c r="Z58" s="178"/>
-      <c r="AA58" s="179"/>
-      <c r="AB58" s="179"/>
-      <c r="AC58" s="179"/>
-      <c r="AD58" s="179"/>
-      <c r="AE58" s="179"/>
-      <c r="AF58" s="179"/>
-      <c r="AG58" s="179"/>
-      <c r="AH58" s="180"/>
+      <c r="U58" s="202"/>
+      <c r="V58" s="203"/>
+      <c r="W58" s="203"/>
+      <c r="X58" s="203"/>
+      <c r="Y58" s="204"/>
+      <c r="Z58" s="225"/>
+      <c r="AA58" s="226"/>
+      <c r="AB58" s="226"/>
+      <c r="AC58" s="226"/>
+      <c r="AD58" s="226"/>
+      <c r="AE58" s="226"/>
+      <c r="AF58" s="226"/>
+      <c r="AG58" s="226"/>
+      <c r="AH58" s="227"/>
       <c r="AI58" s="50"/>
     </row>
     <row r="59" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="200"/>
-      <c r="B59" s="201"/>
-      <c r="C59" s="201"/>
-      <c r="D59" s="201"/>
-      <c r="E59" s="202"/>
-      <c r="F59" s="212"/>
-      <c r="G59" s="210"/>
-      <c r="H59" s="210"/>
-      <c r="I59" s="210"/>
-      <c r="J59" s="210"/>
-      <c r="K59" s="210"/>
-      <c r="L59" s="210"/>
-      <c r="M59" s="211"/>
+      <c r="A59" s="202"/>
+      <c r="B59" s="203"/>
+      <c r="C59" s="203"/>
+      <c r="D59" s="203"/>
+      <c r="E59" s="204"/>
+      <c r="F59" s="217"/>
+      <c r="G59" s="215"/>
+      <c r="H59" s="215"/>
+      <c r="I59" s="215"/>
+      <c r="J59" s="215"/>
+      <c r="K59" s="215"/>
+      <c r="L59" s="215"/>
+      <c r="M59" s="216"/>
       <c r="N59" s="50"/>
       <c r="O59" s="49"/>
-      <c r="U59" s="200"/>
-      <c r="V59" s="201"/>
-      <c r="W59" s="201"/>
-      <c r="X59" s="201"/>
-      <c r="Y59" s="202"/>
-      <c r="Z59" s="178"/>
-      <c r="AA59" s="179"/>
-      <c r="AB59" s="179"/>
-      <c r="AC59" s="179"/>
-      <c r="AD59" s="179"/>
-      <c r="AE59" s="179"/>
-      <c r="AF59" s="179"/>
-      <c r="AG59" s="179"/>
-      <c r="AH59" s="180"/>
+      <c r="U59" s="202"/>
+      <c r="V59" s="203"/>
+      <c r="W59" s="203"/>
+      <c r="X59" s="203"/>
+      <c r="Y59" s="204"/>
+      <c r="Z59" s="225"/>
+      <c r="AA59" s="226"/>
+      <c r="AB59" s="226"/>
+      <c r="AC59" s="226"/>
+      <c r="AD59" s="226"/>
+      <c r="AE59" s="226"/>
+      <c r="AF59" s="226"/>
+      <c r="AG59" s="226"/>
+      <c r="AH59" s="227"/>
       <c r="AI59" s="50"/>
     </row>
     <row r="60" spans="1:35" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="200"/>
-      <c r="B60" s="201"/>
-      <c r="C60" s="201"/>
-      <c r="D60" s="201"/>
-      <c r="E60" s="202"/>
-      <c r="F60" s="212"/>
-      <c r="G60" s="210"/>
-      <c r="H60" s="210"/>
-      <c r="I60" s="210"/>
-      <c r="J60" s="210"/>
-      <c r="K60" s="210"/>
-      <c r="L60" s="210"/>
-      <c r="M60" s="211"/>
+      <c r="A60" s="202"/>
+      <c r="B60" s="203"/>
+      <c r="C60" s="203"/>
+      <c r="D60" s="203"/>
+      <c r="E60" s="204"/>
+      <c r="F60" s="217"/>
+      <c r="G60" s="215"/>
+      <c r="H60" s="215"/>
+      <c r="I60" s="215"/>
+      <c r="J60" s="215"/>
+      <c r="K60" s="215"/>
+      <c r="L60" s="215"/>
+      <c r="M60" s="216"/>
       <c r="N60" s="50"/>
       <c r="O60" s="49"/>
-      <c r="U60" s="200"/>
-      <c r="V60" s="201"/>
-      <c r="W60" s="201"/>
-      <c r="X60" s="201"/>
-      <c r="Y60" s="202"/>
-      <c r="Z60" s="178"/>
-      <c r="AA60" s="179"/>
-      <c r="AB60" s="179"/>
-      <c r="AC60" s="179"/>
-      <c r="AD60" s="179"/>
-      <c r="AE60" s="179"/>
-      <c r="AF60" s="179"/>
-      <c r="AG60" s="179"/>
-      <c r="AH60" s="180"/>
+      <c r="U60" s="202"/>
+      <c r="V60" s="203"/>
+      <c r="W60" s="203"/>
+      <c r="X60" s="203"/>
+      <c r="Y60" s="204"/>
+      <c r="Z60" s="225"/>
+      <c r="AA60" s="226"/>
+      <c r="AB60" s="226"/>
+      <c r="AC60" s="226"/>
+      <c r="AD60" s="226"/>
+      <c r="AE60" s="226"/>
+      <c r="AF60" s="226"/>
+      <c r="AG60" s="226"/>
+      <c r="AH60" s="227"/>
       <c r="AI60" s="50"/>
     </row>
     <row r="61" spans="1:35" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="200"/>
-      <c r="B61" s="201"/>
-      <c r="C61" s="201"/>
-      <c r="D61" s="201"/>
-      <c r="E61" s="202"/>
-      <c r="F61" s="212"/>
-      <c r="G61" s="210"/>
-      <c r="H61" s="210"/>
-      <c r="I61" s="210"/>
-      <c r="J61" s="210"/>
-      <c r="K61" s="210"/>
-      <c r="L61" s="210"/>
-      <c r="M61" s="211"/>
+      <c r="A61" s="202"/>
+      <c r="B61" s="203"/>
+      <c r="C61" s="203"/>
+      <c r="D61" s="203"/>
+      <c r="E61" s="204"/>
+      <c r="F61" s="217"/>
+      <c r="G61" s="215"/>
+      <c r="H61" s="215"/>
+      <c r="I61" s="215"/>
+      <c r="J61" s="215"/>
+      <c r="K61" s="215"/>
+      <c r="L61" s="215"/>
+      <c r="M61" s="216"/>
       <c r="N61" s="50"/>
       <c r="O61" s="49"/>
-      <c r="U61" s="200"/>
-      <c r="V61" s="201"/>
-      <c r="W61" s="201"/>
-      <c r="X61" s="201"/>
-      <c r="Y61" s="202"/>
-      <c r="Z61" s="178"/>
-      <c r="AA61" s="179"/>
-      <c r="AB61" s="179"/>
-      <c r="AC61" s="179"/>
-      <c r="AD61" s="179"/>
-      <c r="AE61" s="179"/>
-      <c r="AF61" s="179"/>
-      <c r="AG61" s="179"/>
-      <c r="AH61" s="180"/>
+      <c r="U61" s="202"/>
+      <c r="V61" s="203"/>
+      <c r="W61" s="203"/>
+      <c r="X61" s="203"/>
+      <c r="Y61" s="204"/>
+      <c r="Z61" s="225"/>
+      <c r="AA61" s="226"/>
+      <c r="AB61" s="226"/>
+      <c r="AC61" s="226"/>
+      <c r="AD61" s="226"/>
+      <c r="AE61" s="226"/>
+      <c r="AF61" s="226"/>
+      <c r="AG61" s="226"/>
+      <c r="AH61" s="227"/>
       <c r="AI61" s="50"/>
     </row>
     <row r="62" spans="1:35" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="203"/>
-      <c r="B62" s="204"/>
-      <c r="C62" s="204"/>
-      <c r="D62" s="204"/>
-      <c r="E62" s="205"/>
-      <c r="F62" s="213"/>
-      <c r="G62" s="214"/>
-      <c r="H62" s="214"/>
-      <c r="I62" s="214"/>
-      <c r="J62" s="214"/>
-      <c r="K62" s="214"/>
-      <c r="L62" s="214"/>
-      <c r="M62" s="215"/>
+      <c r="A62" s="205"/>
+      <c r="B62" s="206"/>
+      <c r="C62" s="206"/>
+      <c r="D62" s="206"/>
+      <c r="E62" s="207"/>
+      <c r="F62" s="218"/>
+      <c r="G62" s="219"/>
+      <c r="H62" s="219"/>
+      <c r="I62" s="219"/>
+      <c r="J62" s="219"/>
+      <c r="K62" s="219"/>
+      <c r="L62" s="219"/>
+      <c r="M62" s="220"/>
       <c r="N62" s="50"/>
       <c r="O62" s="49"/>
-      <c r="U62" s="203"/>
-      <c r="V62" s="204"/>
-      <c r="W62" s="204"/>
-      <c r="X62" s="204"/>
-      <c r="Y62" s="205"/>
-      <c r="Z62" s="181"/>
-      <c r="AA62" s="182"/>
-      <c r="AB62" s="182"/>
-      <c r="AC62" s="182"/>
-      <c r="AD62" s="182"/>
-      <c r="AE62" s="182"/>
-      <c r="AF62" s="182"/>
-      <c r="AG62" s="182"/>
-      <c r="AH62" s="183"/>
+      <c r="U62" s="205"/>
+      <c r="V62" s="206"/>
+      <c r="W62" s="206"/>
+      <c r="X62" s="206"/>
+      <c r="Y62" s="207"/>
+      <c r="Z62" s="228"/>
+      <c r="AA62" s="229"/>
+      <c r="AB62" s="229"/>
+      <c r="AC62" s="229"/>
+      <c r="AD62" s="229"/>
+      <c r="AE62" s="229"/>
+      <c r="AF62" s="229"/>
+      <c r="AG62" s="229"/>
+      <c r="AH62" s="230"/>
       <c r="AI62" s="50"/>
     </row>
     <row r="63" spans="1:35" x14ac:dyDescent="0.2">
@@ -4437,11 +4437,25 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="B2:E3"/>
-    <mergeCell ref="I3:L3"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="I5:N5"/>
-    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="Z47:AH47"/>
+    <mergeCell ref="Z48:AH62"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="U29:V29"/>
+    <mergeCell ref="U30:V30"/>
+    <mergeCell ref="U31:V31"/>
+    <mergeCell ref="AF29:AG29"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="U48:Y62"/>
+    <mergeCell ref="U47:Y47"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="A48:E62"/>
+    <mergeCell ref="F47:M47"/>
+    <mergeCell ref="F48:M62"/>
     <mergeCell ref="AJ29:AL29"/>
     <mergeCell ref="A28:S28"/>
     <mergeCell ref="P38:S38"/>
@@ -4458,25 +4472,11 @@
     <mergeCell ref="U28:AJ28"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="U48:Y62"/>
-    <mergeCell ref="U47:Y47"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="A48:E62"/>
-    <mergeCell ref="F47:M47"/>
-    <mergeCell ref="F48:M62"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="Z47:AH47"/>
-    <mergeCell ref="Z48:AH62"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="U29:V29"/>
-    <mergeCell ref="U30:V30"/>
-    <mergeCell ref="U31:V31"/>
-    <mergeCell ref="AF29:AG29"/>
+    <mergeCell ref="B2:E3"/>
+    <mergeCell ref="I3:L3"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="I5:N5"/>
+    <mergeCell ref="G9:I9"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4557,12 +4557,12 @@
     </row>
     <row r="2" spans="1:25" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
-      <c r="B2" s="233" t="s">
+      <c r="B2" s="175" t="s">
         <v>119</v>
       </c>
-      <c r="C2" s="233"/>
-      <c r="D2" s="233"/>
-      <c r="E2" s="233"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -4579,21 +4579,21 @@
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="234"/>
-      <c r="C3" s="234"/>
-      <c r="D3" s="234"/>
-      <c r="E3" s="234"/>
+      <c r="B3" s="176"/>
+      <c r="C3" s="176"/>
+      <c r="D3" s="176"/>
+      <c r="E3" s="176"/>
       <c r="F3" s="5"/>
       <c r="G3" s="6"/>
       <c r="H3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="235">
+      <c r="I3" s="177">
         <v>20250708</v>
       </c>
-      <c r="J3" s="235"/>
-      <c r="K3" s="235"/>
-      <c r="L3" s="235"/>
+      <c r="J3" s="177"/>
+      <c r="K3" s="177"/>
+      <c r="L3" s="177"/>
       <c r="M3" s="8" t="s">
         <v>3</v>
       </c>
@@ -4625,25 +4625,25 @@
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="236">
+      <c r="B5" s="178">
         <v>45846</v>
       </c>
-      <c r="C5" s="236"/>
-      <c r="D5" s="236"/>
-      <c r="E5" s="236"/>
+      <c r="C5" s="178"/>
+      <c r="D5" s="178"/>
+      <c r="E5" s="178"/>
       <c r="F5" s="5"/>
       <c r="G5" s="6"/>
       <c r="H5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="235" t="s">
+      <c r="I5" s="177" t="s">
         <v>120</v>
       </c>
-      <c r="J5" s="235"/>
-      <c r="K5" s="235"/>
-      <c r="L5" s="235"/>
-      <c r="M5" s="235"/>
-      <c r="N5" s="235"/>
+      <c r="J5" s="177"/>
+      <c r="K5" s="177"/>
+      <c r="L5" s="177"/>
+      <c r="M5" s="177"/>
+      <c r="N5" s="177"/>
       <c r="O5" s="155"/>
       <c r="Y5" s="29"/>
     </row>
@@ -4701,11 +4701,11 @@
       <c r="F9" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="237" t="s">
+      <c r="G9" s="179" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="238"/>
-      <c r="I9" s="238"/>
+      <c r="H9" s="180"/>
+      <c r="I9" s="180"/>
       <c r="J9" s="19" t="s">
         <v>10</v>
       </c>
@@ -4736,11 +4736,11 @@
       <c r="F10" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="222" t="s">
+      <c r="G10" s="189" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="223"/>
-      <c r="I10" s="223"/>
+      <c r="H10" s="190"/>
+      <c r="I10" s="190"/>
       <c r="J10" s="21" t="s">
         <v>10</v>
       </c>
@@ -4771,11 +4771,11 @@
       <c r="F11" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="224" t="s">
+      <c r="G11" s="191" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="225"/>
-      <c r="I11" s="225"/>
+      <c r="H11" s="192"/>
+      <c r="I11" s="192"/>
       <c r="J11" s="62" t="s">
         <v>10</v>
       </c>
@@ -4936,10 +4936,10 @@
       <c r="B19" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="194" t="s">
+      <c r="E19" s="221" t="s">
         <v>46</v>
       </c>
-      <c r="F19" s="195"/>
+      <c r="F19" s="222"/>
       <c r="G19" s="20">
         <v>200</v>
       </c>
@@ -4956,10 +4956,10 @@
         <v>48</v>
       </c>
       <c r="B20" s="21"/>
-      <c r="E20" s="196" t="s">
+      <c r="E20" s="223" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="197"/>
+      <c r="F20" s="224"/>
       <c r="G20" s="22">
         <v>100</v>
       </c>
@@ -4970,10 +4970,10 @@
         <v>50</v>
       </c>
       <c r="B21" s="65"/>
-      <c r="E21" s="196" t="s">
+      <c r="E21" s="223" t="s">
         <v>51</v>
       </c>
-      <c r="F21" s="197"/>
+      <c r="F21" s="224"/>
       <c r="G21" s="22">
         <v>50</v>
       </c>
@@ -4984,10 +4984,10 @@
         <v>52</v>
       </c>
       <c r="B22" s="66"/>
-      <c r="E22" s="196" t="s">
+      <c r="E22" s="223" t="s">
         <v>53</v>
       </c>
-      <c r="F22" s="197"/>
+      <c r="F22" s="224"/>
       <c r="G22" s="23">
         <v>120</v>
       </c>
@@ -5000,10 +5000,10 @@
       <c r="B23" s="24">
         <v>5</v>
       </c>
-      <c r="E23" s="196" t="s">
+      <c r="E23" s="223" t="s">
         <v>55</v>
       </c>
-      <c r="F23" s="197"/>
+      <c r="F23" s="224"/>
       <c r="G23" s="23">
         <v>200</v>
       </c>
@@ -5016,10 +5016,10 @@
       <c r="B24" s="24">
         <v>5</v>
       </c>
-      <c r="E24" s="184" t="s">
+      <c r="E24" s="231" t="s">
         <v>57</v>
       </c>
-      <c r="F24" s="185"/>
+      <c r="F24" s="232"/>
       <c r="G24" s="25">
         <v>0.03</v>
       </c>
@@ -5051,50 +5051,50 @@
     </row>
     <row r="27" spans="1:39" ht="10.5" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="1:39" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="217" t="s">
+      <c r="A28" s="184" t="s">
         <v>59</v>
       </c>
-      <c r="B28" s="217"/>
-      <c r="C28" s="217"/>
-      <c r="D28" s="217"/>
-      <c r="E28" s="217"/>
-      <c r="F28" s="217"/>
-      <c r="G28" s="218"/>
-      <c r="H28" s="218"/>
-      <c r="I28" s="218"/>
-      <c r="J28" s="218"/>
-      <c r="K28" s="218"/>
-      <c r="L28" s="218"/>
-      <c r="M28" s="218"/>
-      <c r="N28" s="218"/>
-      <c r="O28" s="218"/>
-      <c r="P28" s="218"/>
-      <c r="Q28" s="218"/>
-      <c r="R28" s="218"/>
-      <c r="S28" s="218"/>
-      <c r="U28" s="218" t="s">
+      <c r="B28" s="184"/>
+      <c r="C28" s="184"/>
+      <c r="D28" s="184"/>
+      <c r="E28" s="184"/>
+      <c r="F28" s="184"/>
+      <c r="G28" s="185"/>
+      <c r="H28" s="185"/>
+      <c r="I28" s="185"/>
+      <c r="J28" s="185"/>
+      <c r="K28" s="185"/>
+      <c r="L28" s="185"/>
+      <c r="M28" s="185"/>
+      <c r="N28" s="185"/>
+      <c r="O28" s="185"/>
+      <c r="P28" s="185"/>
+      <c r="Q28" s="185"/>
+      <c r="R28" s="185"/>
+      <c r="S28" s="185"/>
+      <c r="U28" s="185" t="s">
         <v>60</v>
       </c>
-      <c r="V28" s="218"/>
-      <c r="W28" s="218"/>
-      <c r="X28" s="218"/>
-      <c r="Y28" s="218"/>
-      <c r="Z28" s="218"/>
-      <c r="AA28" s="218"/>
-      <c r="AB28" s="218"/>
-      <c r="AC28" s="218"/>
-      <c r="AD28" s="218"/>
-      <c r="AE28" s="218"/>
-      <c r="AF28" s="218"/>
-      <c r="AG28" s="218"/>
-      <c r="AH28" s="218"/>
-      <c r="AI28" s="218"/>
-      <c r="AJ28" s="218"/>
+      <c r="V28" s="185"/>
+      <c r="W28" s="185"/>
+      <c r="X28" s="185"/>
+      <c r="Y28" s="185"/>
+      <c r="Z28" s="185"/>
+      <c r="AA28" s="185"/>
+      <c r="AB28" s="185"/>
+      <c r="AC28" s="185"/>
+      <c r="AD28" s="185"/>
+      <c r="AE28" s="185"/>
+      <c r="AF28" s="185"/>
+      <c r="AG28" s="185"/>
+      <c r="AH28" s="185"/>
+      <c r="AI28" s="185"/>
+      <c r="AJ28" s="185"/>
       <c r="AM28" s="51"/>
     </row>
     <row r="29" spans="1:39" ht="18" x14ac:dyDescent="0.4">
-      <c r="A29" s="192"/>
-      <c r="B29" s="232"/>
+      <c r="A29" s="181"/>
+      <c r="B29" s="199"/>
       <c r="C29" s="54" t="s">
         <v>61</v>
       </c>
@@ -5107,19 +5107,19 @@
       <c r="F29" s="28">
         <v>3</v>
       </c>
-      <c r="L29" s="192" t="s">
+      <c r="L29" s="181" t="s">
         <v>62</v>
       </c>
-      <c r="M29" s="193"/>
+      <c r="M29" s="183"/>
       <c r="N29" s="157"/>
       <c r="O29" s="158"/>
-      <c r="P29" s="192" t="s">
+      <c r="P29" s="181" t="s">
         <v>63</v>
       </c>
-      <c r="Q29" s="216"/>
-      <c r="R29" s="193"/>
-      <c r="U29" s="186"/>
-      <c r="V29" s="187"/>
+      <c r="Q29" s="182"/>
+      <c r="R29" s="183"/>
+      <c r="U29" s="233"/>
+      <c r="V29" s="234"/>
       <c r="W29" s="54" t="s">
         <v>61</v>
       </c>
@@ -5133,22 +5133,22 @@
         <v>3</v>
       </c>
       <c r="AE29" s="121"/>
-      <c r="AF29" s="192" t="s">
+      <c r="AF29" s="181" t="s">
         <v>62</v>
       </c>
-      <c r="AG29" s="193"/>
+      <c r="AG29" s="183"/>
       <c r="AH29" s="153"/>
-      <c r="AJ29" s="192" t="s">
+      <c r="AJ29" s="181" t="s">
         <v>63</v>
       </c>
-      <c r="AK29" s="216"/>
-      <c r="AL29" s="193"/>
+      <c r="AK29" s="182"/>
+      <c r="AL29" s="183"/>
     </row>
     <row r="30" spans="1:39" ht="20" x14ac:dyDescent="0.4">
-      <c r="A30" s="230" t="s">
+      <c r="A30" s="197" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="231"/>
+      <c r="B30" s="198"/>
       <c r="C30" s="52">
         <v>6</v>
       </c>
@@ -5172,12 +5172,12 @@
       <c r="P30" s="125" t="s">
         <v>66</v>
       </c>
-      <c r="Q30" s="226"/>
-      <c r="R30" s="227"/>
-      <c r="U30" s="188" t="s">
+      <c r="Q30" s="193"/>
+      <c r="R30" s="194"/>
+      <c r="U30" s="235" t="s">
         <v>64</v>
       </c>
-      <c r="V30" s="189"/>
+      <c r="V30" s="236"/>
       <c r="W30" s="52"/>
       <c r="X30" s="53"/>
       <c r="Y30" s="53"/>
@@ -5195,10 +5195,10 @@
       <c r="AL30" s="145"/>
     </row>
     <row r="31" spans="1:39" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="198" t="s">
+      <c r="A31" s="200" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="199"/>
+      <c r="B31" s="201"/>
       <c r="C31" s="56">
         <v>45.4</v>
       </c>
@@ -5222,12 +5222,12 @@
       <c r="P31" s="125" t="s">
         <v>69</v>
       </c>
-      <c r="Q31" s="226"/>
-      <c r="R31" s="227"/>
-      <c r="U31" s="190" t="s">
+      <c r="Q31" s="193"/>
+      <c r="R31" s="194"/>
+      <c r="U31" s="237" t="s">
         <v>67</v>
       </c>
-      <c r="V31" s="191"/>
+      <c r="V31" s="238"/>
       <c r="W31" s="56"/>
       <c r="X31" s="56"/>
       <c r="Y31" s="56"/>
@@ -5254,8 +5254,8 @@
       <c r="P32" s="125" t="s">
         <v>70</v>
       </c>
-      <c r="Q32" s="226"/>
-      <c r="R32" s="227"/>
+      <c r="Q32" s="193"/>
+      <c r="R32" s="194"/>
       <c r="U32" s="146"/>
       <c r="V32" s="29"/>
       <c r="W32" s="29"/>
@@ -5300,8 +5300,8 @@
       <c r="P33" s="125" t="s">
         <v>76</v>
       </c>
-      <c r="Q33" s="226"/>
-      <c r="R33" s="227"/>
+      <c r="Q33" s="193"/>
+      <c r="R33" s="194"/>
       <c r="U33" s="147"/>
       <c r="V33" s="30" t="s">
         <v>71</v>
@@ -5358,8 +5358,8 @@
       <c r="P34" s="125" t="s">
         <v>77</v>
       </c>
-      <c r="Q34" s="226"/>
-      <c r="R34" s="227"/>
+      <c r="Q34" s="193"/>
+      <c r="R34" s="194"/>
       <c r="W34" s="33">
         <v>160</v>
       </c>
@@ -5416,8 +5416,8 @@
       <c r="P36" s="148" t="s">
         <v>78</v>
       </c>
-      <c r="Q36" s="228"/>
-      <c r="R36" s="229"/>
+      <c r="Q36" s="195"/>
+      <c r="R36" s="196"/>
       <c r="U36" s="169"/>
       <c r="V36" s="170"/>
       <c r="W36" s="170"/>
@@ -5509,12 +5509,12 @@
         <v>90</v>
       </c>
       <c r="N38" s="165"/>
-      <c r="P38" s="219" t="s">
+      <c r="P38" s="186" t="s">
         <v>91</v>
       </c>
-      <c r="Q38" s="220"/>
-      <c r="R38" s="220"/>
-      <c r="S38" s="221"/>
+      <c r="Q38" s="187"/>
+      <c r="R38" s="187"/>
+      <c r="S38" s="188"/>
       <c r="U38" s="107" t="s">
         <v>80</v>
       </c>
@@ -5972,527 +5972,527 @@
     </row>
     <row r="46" spans="1:38" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="1:38" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="206" t="s">
+      <c r="A47" s="208" t="s">
         <v>116</v>
       </c>
-      <c r="B47" s="207"/>
-      <c r="C47" s="207"/>
-      <c r="D47" s="207"/>
-      <c r="E47" s="208"/>
-      <c r="F47" s="175" t="s">
+      <c r="B47" s="209"/>
+      <c r="C47" s="209"/>
+      <c r="D47" s="209"/>
+      <c r="E47" s="210"/>
+      <c r="F47" s="211" t="s">
         <v>117</v>
       </c>
-      <c r="G47" s="176"/>
-      <c r="H47" s="176"/>
-      <c r="I47" s="176"/>
-      <c r="J47" s="176"/>
-      <c r="K47" s="176"/>
-      <c r="L47" s="176"/>
-      <c r="M47" s="177"/>
+      <c r="G47" s="212"/>
+      <c r="H47" s="212"/>
+      <c r="I47" s="212"/>
+      <c r="J47" s="212"/>
+      <c r="K47" s="212"/>
+      <c r="L47" s="212"/>
+      <c r="M47" s="213"/>
       <c r="N47" s="50"/>
       <c r="O47" s="49"/>
-      <c r="U47" s="206" t="s">
+      <c r="U47" s="208" t="s">
         <v>118</v>
       </c>
-      <c r="V47" s="207"/>
-      <c r="W47" s="207"/>
-      <c r="X47" s="207"/>
-      <c r="Y47" s="208"/>
-      <c r="Z47" s="175" t="s">
+      <c r="V47" s="209"/>
+      <c r="W47" s="209"/>
+      <c r="X47" s="209"/>
+      <c r="Y47" s="210"/>
+      <c r="Z47" s="211" t="s">
         <v>117</v>
       </c>
-      <c r="AA47" s="176"/>
-      <c r="AB47" s="176"/>
-      <c r="AC47" s="176"/>
-      <c r="AD47" s="176"/>
-      <c r="AE47" s="176"/>
-      <c r="AF47" s="176"/>
-      <c r="AG47" s="176"/>
-      <c r="AH47" s="177"/>
+      <c r="AA47" s="212"/>
+      <c r="AB47" s="212"/>
+      <c r="AC47" s="212"/>
+      <c r="AD47" s="212"/>
+      <c r="AE47" s="212"/>
+      <c r="AF47" s="212"/>
+      <c r="AG47" s="212"/>
+      <c r="AH47" s="213"/>
       <c r="AI47" s="50"/>
     </row>
     <row r="48" spans="1:38" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="200" t="s">
+      <c r="A48" s="202" t="s">
         <v>125</v>
       </c>
-      <c r="B48" s="201"/>
-      <c r="C48" s="201"/>
-      <c r="D48" s="201"/>
-      <c r="E48" s="202"/>
-      <c r="F48" s="212" t="s">
+      <c r="B48" s="203"/>
+      <c r="C48" s="203"/>
+      <c r="D48" s="203"/>
+      <c r="E48" s="204"/>
+      <c r="F48" s="217" t="s">
         <v>123</v>
       </c>
-      <c r="G48" s="210"/>
-      <c r="H48" s="210"/>
-      <c r="I48" s="210"/>
-      <c r="J48" s="210"/>
-      <c r="K48" s="210"/>
-      <c r="L48" s="210"/>
-      <c r="M48" s="211"/>
+      <c r="G48" s="215"/>
+      <c r="H48" s="215"/>
+      <c r="I48" s="215"/>
+      <c r="J48" s="215"/>
+      <c r="K48" s="215"/>
+      <c r="L48" s="215"/>
+      <c r="M48" s="216"/>
       <c r="N48" s="50"/>
       <c r="O48" s="49"/>
-      <c r="U48" s="200"/>
-      <c r="V48" s="201"/>
-      <c r="W48" s="201"/>
-      <c r="X48" s="201"/>
-      <c r="Y48" s="202"/>
-      <c r="Z48" s="178"/>
-      <c r="AA48" s="179"/>
-      <c r="AB48" s="179"/>
-      <c r="AC48" s="179"/>
-      <c r="AD48" s="179"/>
-      <c r="AE48" s="179"/>
-      <c r="AF48" s="179"/>
-      <c r="AG48" s="179"/>
-      <c r="AH48" s="180"/>
+      <c r="U48" s="202"/>
+      <c r="V48" s="203"/>
+      <c r="W48" s="203"/>
+      <c r="X48" s="203"/>
+      <c r="Y48" s="204"/>
+      <c r="Z48" s="225"/>
+      <c r="AA48" s="226"/>
+      <c r="AB48" s="226"/>
+      <c r="AC48" s="226"/>
+      <c r="AD48" s="226"/>
+      <c r="AE48" s="226"/>
+      <c r="AF48" s="226"/>
+      <c r="AG48" s="226"/>
+      <c r="AH48" s="227"/>
       <c r="AI48" s="50"/>
     </row>
     <row r="49" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="200"/>
-      <c r="B49" s="201"/>
-      <c r="C49" s="201"/>
-      <c r="D49" s="201"/>
-      <c r="E49" s="202"/>
-      <c r="F49" s="212"/>
-      <c r="G49" s="210"/>
-      <c r="H49" s="210"/>
-      <c r="I49" s="210"/>
-      <c r="J49" s="210"/>
-      <c r="K49" s="210"/>
-      <c r="L49" s="210"/>
-      <c r="M49" s="211"/>
+      <c r="A49" s="202"/>
+      <c r="B49" s="203"/>
+      <c r="C49" s="203"/>
+      <c r="D49" s="203"/>
+      <c r="E49" s="204"/>
+      <c r="F49" s="217"/>
+      <c r="G49" s="215"/>
+      <c r="H49" s="215"/>
+      <c r="I49" s="215"/>
+      <c r="J49" s="215"/>
+      <c r="K49" s="215"/>
+      <c r="L49" s="215"/>
+      <c r="M49" s="216"/>
       <c r="N49" s="50"/>
       <c r="O49" s="49"/>
-      <c r="U49" s="200"/>
-      <c r="V49" s="201"/>
-      <c r="W49" s="201"/>
-      <c r="X49" s="201"/>
-      <c r="Y49" s="202"/>
-      <c r="Z49" s="178"/>
-      <c r="AA49" s="179"/>
-      <c r="AB49" s="179"/>
-      <c r="AC49" s="179"/>
-      <c r="AD49" s="179"/>
-      <c r="AE49" s="179"/>
-      <c r="AF49" s="179"/>
-      <c r="AG49" s="179"/>
-      <c r="AH49" s="180"/>
+      <c r="U49" s="202"/>
+      <c r="V49" s="203"/>
+      <c r="W49" s="203"/>
+      <c r="X49" s="203"/>
+      <c r="Y49" s="204"/>
+      <c r="Z49" s="225"/>
+      <c r="AA49" s="226"/>
+      <c r="AB49" s="226"/>
+      <c r="AC49" s="226"/>
+      <c r="AD49" s="226"/>
+      <c r="AE49" s="226"/>
+      <c r="AF49" s="226"/>
+      <c r="AG49" s="226"/>
+      <c r="AH49" s="227"/>
       <c r="AI49" s="50"/>
     </row>
     <row r="50" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="200"/>
-      <c r="B50" s="201"/>
-      <c r="C50" s="201"/>
-      <c r="D50" s="201"/>
-      <c r="E50" s="202"/>
-      <c r="F50" s="212"/>
-      <c r="G50" s="210"/>
-      <c r="H50" s="210"/>
-      <c r="I50" s="210"/>
-      <c r="J50" s="210"/>
-      <c r="K50" s="210"/>
-      <c r="L50" s="210"/>
-      <c r="M50" s="211"/>
+      <c r="A50" s="202"/>
+      <c r="B50" s="203"/>
+      <c r="C50" s="203"/>
+      <c r="D50" s="203"/>
+      <c r="E50" s="204"/>
+      <c r="F50" s="217"/>
+      <c r="G50" s="215"/>
+      <c r="H50" s="215"/>
+      <c r="I50" s="215"/>
+      <c r="J50" s="215"/>
+      <c r="K50" s="215"/>
+      <c r="L50" s="215"/>
+      <c r="M50" s="216"/>
       <c r="N50" s="50"/>
       <c r="O50" s="49"/>
-      <c r="U50" s="200"/>
-      <c r="V50" s="201"/>
-      <c r="W50" s="201"/>
-      <c r="X50" s="201"/>
-      <c r="Y50" s="202"/>
-      <c r="Z50" s="178"/>
-      <c r="AA50" s="179"/>
-      <c r="AB50" s="179"/>
-      <c r="AC50" s="179"/>
-      <c r="AD50" s="179"/>
-      <c r="AE50" s="179"/>
-      <c r="AF50" s="179"/>
-      <c r="AG50" s="179"/>
-      <c r="AH50" s="180"/>
+      <c r="U50" s="202"/>
+      <c r="V50" s="203"/>
+      <c r="W50" s="203"/>
+      <c r="X50" s="203"/>
+      <c r="Y50" s="204"/>
+      <c r="Z50" s="225"/>
+      <c r="AA50" s="226"/>
+      <c r="AB50" s="226"/>
+      <c r="AC50" s="226"/>
+      <c r="AD50" s="226"/>
+      <c r="AE50" s="226"/>
+      <c r="AF50" s="226"/>
+      <c r="AG50" s="226"/>
+      <c r="AH50" s="227"/>
       <c r="AI50" s="50"/>
     </row>
     <row r="51" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="200"/>
-      <c r="B51" s="201"/>
-      <c r="C51" s="201"/>
-      <c r="D51" s="201"/>
-      <c r="E51" s="202"/>
-      <c r="F51" s="212"/>
-      <c r="G51" s="210"/>
-      <c r="H51" s="210"/>
-      <c r="I51" s="210"/>
-      <c r="J51" s="210"/>
-      <c r="K51" s="210"/>
-      <c r="L51" s="210"/>
-      <c r="M51" s="211"/>
+      <c r="A51" s="202"/>
+      <c r="B51" s="203"/>
+      <c r="C51" s="203"/>
+      <c r="D51" s="203"/>
+      <c r="E51" s="204"/>
+      <c r="F51" s="217"/>
+      <c r="G51" s="215"/>
+      <c r="H51" s="215"/>
+      <c r="I51" s="215"/>
+      <c r="J51" s="215"/>
+      <c r="K51" s="215"/>
+      <c r="L51" s="215"/>
+      <c r="M51" s="216"/>
       <c r="N51" s="50"/>
       <c r="O51" s="49"/>
-      <c r="U51" s="200"/>
-      <c r="V51" s="201"/>
-      <c r="W51" s="201"/>
-      <c r="X51" s="201"/>
-      <c r="Y51" s="202"/>
-      <c r="Z51" s="178"/>
-      <c r="AA51" s="179"/>
-      <c r="AB51" s="179"/>
-      <c r="AC51" s="179"/>
-      <c r="AD51" s="179"/>
-      <c r="AE51" s="179"/>
-      <c r="AF51" s="179"/>
-      <c r="AG51" s="179"/>
-      <c r="AH51" s="180"/>
+      <c r="U51" s="202"/>
+      <c r="V51" s="203"/>
+      <c r="W51" s="203"/>
+      <c r="X51" s="203"/>
+      <c r="Y51" s="204"/>
+      <c r="Z51" s="225"/>
+      <c r="AA51" s="226"/>
+      <c r="AB51" s="226"/>
+      <c r="AC51" s="226"/>
+      <c r="AD51" s="226"/>
+      <c r="AE51" s="226"/>
+      <c r="AF51" s="226"/>
+      <c r="AG51" s="226"/>
+      <c r="AH51" s="227"/>
       <c r="AI51" s="50"/>
     </row>
     <row r="52" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="200"/>
-      <c r="B52" s="201"/>
-      <c r="C52" s="201"/>
-      <c r="D52" s="201"/>
-      <c r="E52" s="202"/>
-      <c r="F52" s="212"/>
-      <c r="G52" s="210"/>
-      <c r="H52" s="210"/>
-      <c r="I52" s="210"/>
-      <c r="J52" s="210"/>
-      <c r="K52" s="210"/>
-      <c r="L52" s="210"/>
-      <c r="M52" s="211"/>
+      <c r="A52" s="202"/>
+      <c r="B52" s="203"/>
+      <c r="C52" s="203"/>
+      <c r="D52" s="203"/>
+      <c r="E52" s="204"/>
+      <c r="F52" s="217"/>
+      <c r="G52" s="215"/>
+      <c r="H52" s="215"/>
+      <c r="I52" s="215"/>
+      <c r="J52" s="215"/>
+      <c r="K52" s="215"/>
+      <c r="L52" s="215"/>
+      <c r="M52" s="216"/>
       <c r="N52" s="50"/>
       <c r="O52" s="49"/>
-      <c r="U52" s="200"/>
-      <c r="V52" s="201"/>
-      <c r="W52" s="201"/>
-      <c r="X52" s="201"/>
-      <c r="Y52" s="202"/>
-      <c r="Z52" s="178"/>
-      <c r="AA52" s="179"/>
-      <c r="AB52" s="179"/>
-      <c r="AC52" s="179"/>
-      <c r="AD52" s="179"/>
-      <c r="AE52" s="179"/>
-      <c r="AF52" s="179"/>
-      <c r="AG52" s="179"/>
-      <c r="AH52" s="180"/>
+      <c r="U52" s="202"/>
+      <c r="V52" s="203"/>
+      <c r="W52" s="203"/>
+      <c r="X52" s="203"/>
+      <c r="Y52" s="204"/>
+      <c r="Z52" s="225"/>
+      <c r="AA52" s="226"/>
+      <c r="AB52" s="226"/>
+      <c r="AC52" s="226"/>
+      <c r="AD52" s="226"/>
+      <c r="AE52" s="226"/>
+      <c r="AF52" s="226"/>
+      <c r="AG52" s="226"/>
+      <c r="AH52" s="227"/>
       <c r="AI52" s="50"/>
     </row>
     <row r="53" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="200"/>
-      <c r="B53" s="201"/>
-      <c r="C53" s="201"/>
-      <c r="D53" s="201"/>
-      <c r="E53" s="202"/>
-      <c r="F53" s="212"/>
-      <c r="G53" s="210"/>
-      <c r="H53" s="210"/>
-      <c r="I53" s="210"/>
-      <c r="J53" s="210"/>
-      <c r="K53" s="210"/>
-      <c r="L53" s="210"/>
-      <c r="M53" s="211"/>
+      <c r="A53" s="202"/>
+      <c r="B53" s="203"/>
+      <c r="C53" s="203"/>
+      <c r="D53" s="203"/>
+      <c r="E53" s="204"/>
+      <c r="F53" s="217"/>
+      <c r="G53" s="215"/>
+      <c r="H53" s="215"/>
+      <c r="I53" s="215"/>
+      <c r="J53" s="215"/>
+      <c r="K53" s="215"/>
+      <c r="L53" s="215"/>
+      <c r="M53" s="216"/>
       <c r="N53" s="50"/>
       <c r="O53" s="49"/>
-      <c r="U53" s="200"/>
-      <c r="V53" s="201"/>
-      <c r="W53" s="201"/>
-      <c r="X53" s="201"/>
-      <c r="Y53" s="202"/>
-      <c r="Z53" s="178"/>
-      <c r="AA53" s="179"/>
-      <c r="AB53" s="179"/>
-      <c r="AC53" s="179"/>
-      <c r="AD53" s="179"/>
-      <c r="AE53" s="179"/>
-      <c r="AF53" s="179"/>
-      <c r="AG53" s="179"/>
-      <c r="AH53" s="180"/>
+      <c r="U53" s="202"/>
+      <c r="V53" s="203"/>
+      <c r="W53" s="203"/>
+      <c r="X53" s="203"/>
+      <c r="Y53" s="204"/>
+      <c r="Z53" s="225"/>
+      <c r="AA53" s="226"/>
+      <c r="AB53" s="226"/>
+      <c r="AC53" s="226"/>
+      <c r="AD53" s="226"/>
+      <c r="AE53" s="226"/>
+      <c r="AF53" s="226"/>
+      <c r="AG53" s="226"/>
+      <c r="AH53" s="227"/>
       <c r="AI53" s="50"/>
     </row>
     <row r="54" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="200"/>
-      <c r="B54" s="201"/>
-      <c r="C54" s="201"/>
-      <c r="D54" s="201"/>
-      <c r="E54" s="202"/>
-      <c r="F54" s="212"/>
-      <c r="G54" s="210"/>
-      <c r="H54" s="210"/>
-      <c r="I54" s="210"/>
-      <c r="J54" s="210"/>
-      <c r="K54" s="210"/>
-      <c r="L54" s="210"/>
-      <c r="M54" s="211"/>
+      <c r="A54" s="202"/>
+      <c r="B54" s="203"/>
+      <c r="C54" s="203"/>
+      <c r="D54" s="203"/>
+      <c r="E54" s="204"/>
+      <c r="F54" s="217"/>
+      <c r="G54" s="215"/>
+      <c r="H54" s="215"/>
+      <c r="I54" s="215"/>
+      <c r="J54" s="215"/>
+      <c r="K54" s="215"/>
+      <c r="L54" s="215"/>
+      <c r="M54" s="216"/>
       <c r="N54" s="50"/>
       <c r="O54" s="49"/>
-      <c r="U54" s="200"/>
-      <c r="V54" s="201"/>
-      <c r="W54" s="201"/>
-      <c r="X54" s="201"/>
-      <c r="Y54" s="202"/>
-      <c r="Z54" s="178"/>
-      <c r="AA54" s="179"/>
-      <c r="AB54" s="179"/>
-      <c r="AC54" s="179"/>
-      <c r="AD54" s="179"/>
-      <c r="AE54" s="179"/>
-      <c r="AF54" s="179"/>
-      <c r="AG54" s="179"/>
-      <c r="AH54" s="180"/>
+      <c r="U54" s="202"/>
+      <c r="V54" s="203"/>
+      <c r="W54" s="203"/>
+      <c r="X54" s="203"/>
+      <c r="Y54" s="204"/>
+      <c r="Z54" s="225"/>
+      <c r="AA54" s="226"/>
+      <c r="AB54" s="226"/>
+      <c r="AC54" s="226"/>
+      <c r="AD54" s="226"/>
+      <c r="AE54" s="226"/>
+      <c r="AF54" s="226"/>
+      <c r="AG54" s="226"/>
+      <c r="AH54" s="227"/>
       <c r="AI54" s="50"/>
     </row>
     <row r="55" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="200"/>
-      <c r="B55" s="201"/>
-      <c r="C55" s="201"/>
-      <c r="D55" s="201"/>
-      <c r="E55" s="202"/>
-      <c r="F55" s="212"/>
-      <c r="G55" s="210"/>
-      <c r="H55" s="210"/>
-      <c r="I55" s="210"/>
-      <c r="J55" s="210"/>
-      <c r="K55" s="210"/>
-      <c r="L55" s="210"/>
-      <c r="M55" s="211"/>
+      <c r="A55" s="202"/>
+      <c r="B55" s="203"/>
+      <c r="C55" s="203"/>
+      <c r="D55" s="203"/>
+      <c r="E55" s="204"/>
+      <c r="F55" s="217"/>
+      <c r="G55" s="215"/>
+      <c r="H55" s="215"/>
+      <c r="I55" s="215"/>
+      <c r="J55" s="215"/>
+      <c r="K55" s="215"/>
+      <c r="L55" s="215"/>
+      <c r="M55" s="216"/>
       <c r="N55" s="50"/>
       <c r="O55" s="49"/>
-      <c r="U55" s="200"/>
-      <c r="V55" s="201"/>
-      <c r="W55" s="201"/>
-      <c r="X55" s="201"/>
-      <c r="Y55" s="202"/>
-      <c r="Z55" s="178"/>
-      <c r="AA55" s="179"/>
-      <c r="AB55" s="179"/>
-      <c r="AC55" s="179"/>
-      <c r="AD55" s="179"/>
-      <c r="AE55" s="179"/>
-      <c r="AF55" s="179"/>
-      <c r="AG55" s="179"/>
-      <c r="AH55" s="180"/>
+      <c r="U55" s="202"/>
+      <c r="V55" s="203"/>
+      <c r="W55" s="203"/>
+      <c r="X55" s="203"/>
+      <c r="Y55" s="204"/>
+      <c r="Z55" s="225"/>
+      <c r="AA55" s="226"/>
+      <c r="AB55" s="226"/>
+      <c r="AC55" s="226"/>
+      <c r="AD55" s="226"/>
+      <c r="AE55" s="226"/>
+      <c r="AF55" s="226"/>
+      <c r="AG55" s="226"/>
+      <c r="AH55" s="227"/>
       <c r="AI55" s="50"/>
     </row>
     <row r="56" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="200"/>
-      <c r="B56" s="201"/>
-      <c r="C56" s="201"/>
-      <c r="D56" s="201"/>
-      <c r="E56" s="202"/>
-      <c r="F56" s="212"/>
-      <c r="G56" s="210"/>
-      <c r="H56" s="210"/>
-      <c r="I56" s="210"/>
-      <c r="J56" s="210"/>
-      <c r="K56" s="210"/>
-      <c r="L56" s="210"/>
-      <c r="M56" s="211"/>
+      <c r="A56" s="202"/>
+      <c r="B56" s="203"/>
+      <c r="C56" s="203"/>
+      <c r="D56" s="203"/>
+      <c r="E56" s="204"/>
+      <c r="F56" s="217"/>
+      <c r="G56" s="215"/>
+      <c r="H56" s="215"/>
+      <c r="I56" s="215"/>
+      <c r="J56" s="215"/>
+      <c r="K56" s="215"/>
+      <c r="L56" s="215"/>
+      <c r="M56" s="216"/>
       <c r="N56" s="50"/>
       <c r="O56" s="49"/>
-      <c r="U56" s="200"/>
-      <c r="V56" s="201"/>
-      <c r="W56" s="201"/>
-      <c r="X56" s="201"/>
-      <c r="Y56" s="202"/>
-      <c r="Z56" s="178"/>
-      <c r="AA56" s="179"/>
-      <c r="AB56" s="179"/>
-      <c r="AC56" s="179"/>
-      <c r="AD56" s="179"/>
-      <c r="AE56" s="179"/>
-      <c r="AF56" s="179"/>
-      <c r="AG56" s="179"/>
-      <c r="AH56" s="180"/>
+      <c r="U56" s="202"/>
+      <c r="V56" s="203"/>
+      <c r="W56" s="203"/>
+      <c r="X56" s="203"/>
+      <c r="Y56" s="204"/>
+      <c r="Z56" s="225"/>
+      <c r="AA56" s="226"/>
+      <c r="AB56" s="226"/>
+      <c r="AC56" s="226"/>
+      <c r="AD56" s="226"/>
+      <c r="AE56" s="226"/>
+      <c r="AF56" s="226"/>
+      <c r="AG56" s="226"/>
+      <c r="AH56" s="227"/>
       <c r="AI56" s="50"/>
     </row>
     <row r="57" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="200"/>
-      <c r="B57" s="201"/>
-      <c r="C57" s="201"/>
-      <c r="D57" s="201"/>
-      <c r="E57" s="202"/>
-      <c r="F57" s="212"/>
-      <c r="G57" s="210"/>
-      <c r="H57" s="210"/>
-      <c r="I57" s="210"/>
-      <c r="J57" s="210"/>
-      <c r="K57" s="210"/>
-      <c r="L57" s="210"/>
-      <c r="M57" s="211"/>
+      <c r="A57" s="202"/>
+      <c r="B57" s="203"/>
+      <c r="C57" s="203"/>
+      <c r="D57" s="203"/>
+      <c r="E57" s="204"/>
+      <c r="F57" s="217"/>
+      <c r="G57" s="215"/>
+      <c r="H57" s="215"/>
+      <c r="I57" s="215"/>
+      <c r="J57" s="215"/>
+      <c r="K57" s="215"/>
+      <c r="L57" s="215"/>
+      <c r="M57" s="216"/>
       <c r="N57" s="50"/>
       <c r="O57" s="49"/>
-      <c r="U57" s="200"/>
-      <c r="V57" s="201"/>
-      <c r="W57" s="201"/>
-      <c r="X57" s="201"/>
-      <c r="Y57" s="202"/>
-      <c r="Z57" s="178"/>
-      <c r="AA57" s="179"/>
-      <c r="AB57" s="179"/>
-      <c r="AC57" s="179"/>
-      <c r="AD57" s="179"/>
-      <c r="AE57" s="179"/>
-      <c r="AF57" s="179"/>
-      <c r="AG57" s="179"/>
-      <c r="AH57" s="180"/>
+      <c r="U57" s="202"/>
+      <c r="V57" s="203"/>
+      <c r="W57" s="203"/>
+      <c r="X57" s="203"/>
+      <c r="Y57" s="204"/>
+      <c r="Z57" s="225"/>
+      <c r="AA57" s="226"/>
+      <c r="AB57" s="226"/>
+      <c r="AC57" s="226"/>
+      <c r="AD57" s="226"/>
+      <c r="AE57" s="226"/>
+      <c r="AF57" s="226"/>
+      <c r="AG57" s="226"/>
+      <c r="AH57" s="227"/>
       <c r="AI57" s="50"/>
     </row>
     <row r="58" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="200"/>
-      <c r="B58" s="201"/>
-      <c r="C58" s="201"/>
-      <c r="D58" s="201"/>
-      <c r="E58" s="202"/>
-      <c r="F58" s="212"/>
-      <c r="G58" s="210"/>
-      <c r="H58" s="210"/>
-      <c r="I58" s="210"/>
-      <c r="J58" s="210"/>
-      <c r="K58" s="210"/>
-      <c r="L58" s="210"/>
-      <c r="M58" s="211"/>
+      <c r="A58" s="202"/>
+      <c r="B58" s="203"/>
+      <c r="C58" s="203"/>
+      <c r="D58" s="203"/>
+      <c r="E58" s="204"/>
+      <c r="F58" s="217"/>
+      <c r="G58" s="215"/>
+      <c r="H58" s="215"/>
+      <c r="I58" s="215"/>
+      <c r="J58" s="215"/>
+      <c r="K58" s="215"/>
+      <c r="L58" s="215"/>
+      <c r="M58" s="216"/>
       <c r="N58" s="50"/>
       <c r="O58" s="49"/>
-      <c r="U58" s="200"/>
-      <c r="V58" s="201"/>
-      <c r="W58" s="201"/>
-      <c r="X58" s="201"/>
-      <c r="Y58" s="202"/>
-      <c r="Z58" s="178"/>
-      <c r="AA58" s="179"/>
-      <c r="AB58" s="179"/>
-      <c r="AC58" s="179"/>
-      <c r="AD58" s="179"/>
-      <c r="AE58" s="179"/>
-      <c r="AF58" s="179"/>
-      <c r="AG58" s="179"/>
-      <c r="AH58" s="180"/>
+      <c r="U58" s="202"/>
+      <c r="V58" s="203"/>
+      <c r="W58" s="203"/>
+      <c r="X58" s="203"/>
+      <c r="Y58" s="204"/>
+      <c r="Z58" s="225"/>
+      <c r="AA58" s="226"/>
+      <c r="AB58" s="226"/>
+      <c r="AC58" s="226"/>
+      <c r="AD58" s="226"/>
+      <c r="AE58" s="226"/>
+      <c r="AF58" s="226"/>
+      <c r="AG58" s="226"/>
+      <c r="AH58" s="227"/>
       <c r="AI58" s="50"/>
     </row>
     <row r="59" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="200"/>
-      <c r="B59" s="201"/>
-      <c r="C59" s="201"/>
-      <c r="D59" s="201"/>
-      <c r="E59" s="202"/>
-      <c r="F59" s="212"/>
-      <c r="G59" s="210"/>
-      <c r="H59" s="210"/>
-      <c r="I59" s="210"/>
-      <c r="J59" s="210"/>
-      <c r="K59" s="210"/>
-      <c r="L59" s="210"/>
-      <c r="M59" s="211"/>
+      <c r="A59" s="202"/>
+      <c r="B59" s="203"/>
+      <c r="C59" s="203"/>
+      <c r="D59" s="203"/>
+      <c r="E59" s="204"/>
+      <c r="F59" s="217"/>
+      <c r="G59" s="215"/>
+      <c r="H59" s="215"/>
+      <c r="I59" s="215"/>
+      <c r="J59" s="215"/>
+      <c r="K59" s="215"/>
+      <c r="L59" s="215"/>
+      <c r="M59" s="216"/>
       <c r="N59" s="50"/>
       <c r="O59" s="49"/>
-      <c r="U59" s="200"/>
-      <c r="V59" s="201"/>
-      <c r="W59" s="201"/>
-      <c r="X59" s="201"/>
-      <c r="Y59" s="202"/>
-      <c r="Z59" s="178"/>
-      <c r="AA59" s="179"/>
-      <c r="AB59" s="179"/>
-      <c r="AC59" s="179"/>
-      <c r="AD59" s="179"/>
-      <c r="AE59" s="179"/>
-      <c r="AF59" s="179"/>
-      <c r="AG59" s="179"/>
-      <c r="AH59" s="180"/>
+      <c r="U59" s="202"/>
+      <c r="V59" s="203"/>
+      <c r="W59" s="203"/>
+      <c r="X59" s="203"/>
+      <c r="Y59" s="204"/>
+      <c r="Z59" s="225"/>
+      <c r="AA59" s="226"/>
+      <c r="AB59" s="226"/>
+      <c r="AC59" s="226"/>
+      <c r="AD59" s="226"/>
+      <c r="AE59" s="226"/>
+      <c r="AF59" s="226"/>
+      <c r="AG59" s="226"/>
+      <c r="AH59" s="227"/>
       <c r="AI59" s="50"/>
     </row>
     <row r="60" spans="1:35" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="200"/>
-      <c r="B60" s="201"/>
-      <c r="C60" s="201"/>
-      <c r="D60" s="201"/>
-      <c r="E60" s="202"/>
-      <c r="F60" s="212"/>
-      <c r="G60" s="210"/>
-      <c r="H60" s="210"/>
-      <c r="I60" s="210"/>
-      <c r="J60" s="210"/>
-      <c r="K60" s="210"/>
-      <c r="L60" s="210"/>
-      <c r="M60" s="211"/>
+      <c r="A60" s="202"/>
+      <c r="B60" s="203"/>
+      <c r="C60" s="203"/>
+      <c r="D60" s="203"/>
+      <c r="E60" s="204"/>
+      <c r="F60" s="217"/>
+      <c r="G60" s="215"/>
+      <c r="H60" s="215"/>
+      <c r="I60" s="215"/>
+      <c r="J60" s="215"/>
+      <c r="K60" s="215"/>
+      <c r="L60" s="215"/>
+      <c r="M60" s="216"/>
       <c r="N60" s="50"/>
       <c r="O60" s="49"/>
-      <c r="U60" s="200"/>
-      <c r="V60" s="201"/>
-      <c r="W60" s="201"/>
-      <c r="X60" s="201"/>
-      <c r="Y60" s="202"/>
-      <c r="Z60" s="178"/>
-      <c r="AA60" s="179"/>
-      <c r="AB60" s="179"/>
-      <c r="AC60" s="179"/>
-      <c r="AD60" s="179"/>
-      <c r="AE60" s="179"/>
-      <c r="AF60" s="179"/>
-      <c r="AG60" s="179"/>
-      <c r="AH60" s="180"/>
+      <c r="U60" s="202"/>
+      <c r="V60" s="203"/>
+      <c r="W60" s="203"/>
+      <c r="X60" s="203"/>
+      <c r="Y60" s="204"/>
+      <c r="Z60" s="225"/>
+      <c r="AA60" s="226"/>
+      <c r="AB60" s="226"/>
+      <c r="AC60" s="226"/>
+      <c r="AD60" s="226"/>
+      <c r="AE60" s="226"/>
+      <c r="AF60" s="226"/>
+      <c r="AG60" s="226"/>
+      <c r="AH60" s="227"/>
       <c r="AI60" s="50"/>
     </row>
     <row r="61" spans="1:35" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="200"/>
-      <c r="B61" s="201"/>
-      <c r="C61" s="201"/>
-      <c r="D61" s="201"/>
-      <c r="E61" s="202"/>
-      <c r="F61" s="212"/>
-      <c r="G61" s="210"/>
-      <c r="H61" s="210"/>
-      <c r="I61" s="210"/>
-      <c r="J61" s="210"/>
-      <c r="K61" s="210"/>
-      <c r="L61" s="210"/>
-      <c r="M61" s="211"/>
+      <c r="A61" s="202"/>
+      <c r="B61" s="203"/>
+      <c r="C61" s="203"/>
+      <c r="D61" s="203"/>
+      <c r="E61" s="204"/>
+      <c r="F61" s="217"/>
+      <c r="G61" s="215"/>
+      <c r="H61" s="215"/>
+      <c r="I61" s="215"/>
+      <c r="J61" s="215"/>
+      <c r="K61" s="215"/>
+      <c r="L61" s="215"/>
+      <c r="M61" s="216"/>
       <c r="N61" s="50"/>
       <c r="O61" s="49"/>
-      <c r="U61" s="200"/>
-      <c r="V61" s="201"/>
-      <c r="W61" s="201"/>
-      <c r="X61" s="201"/>
-      <c r="Y61" s="202"/>
-      <c r="Z61" s="178"/>
-      <c r="AA61" s="179"/>
-      <c r="AB61" s="179"/>
-      <c r="AC61" s="179"/>
-      <c r="AD61" s="179"/>
-      <c r="AE61" s="179"/>
-      <c r="AF61" s="179"/>
-      <c r="AG61" s="179"/>
-      <c r="AH61" s="180"/>
+      <c r="U61" s="202"/>
+      <c r="V61" s="203"/>
+      <c r="W61" s="203"/>
+      <c r="X61" s="203"/>
+      <c r="Y61" s="204"/>
+      <c r="Z61" s="225"/>
+      <c r="AA61" s="226"/>
+      <c r="AB61" s="226"/>
+      <c r="AC61" s="226"/>
+      <c r="AD61" s="226"/>
+      <c r="AE61" s="226"/>
+      <c r="AF61" s="226"/>
+      <c r="AG61" s="226"/>
+      <c r="AH61" s="227"/>
       <c r="AI61" s="50"/>
     </row>
     <row r="62" spans="1:35" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="203"/>
-      <c r="B62" s="204"/>
-      <c r="C62" s="204"/>
-      <c r="D62" s="204"/>
-      <c r="E62" s="205"/>
-      <c r="F62" s="213"/>
-      <c r="G62" s="214"/>
-      <c r="H62" s="214"/>
-      <c r="I62" s="214"/>
-      <c r="J62" s="214"/>
-      <c r="K62" s="214"/>
-      <c r="L62" s="214"/>
-      <c r="M62" s="215"/>
+      <c r="A62" s="205"/>
+      <c r="B62" s="206"/>
+      <c r="C62" s="206"/>
+      <c r="D62" s="206"/>
+      <c r="E62" s="207"/>
+      <c r="F62" s="218"/>
+      <c r="G62" s="219"/>
+      <c r="H62" s="219"/>
+      <c r="I62" s="219"/>
+      <c r="J62" s="219"/>
+      <c r="K62" s="219"/>
+      <c r="L62" s="219"/>
+      <c r="M62" s="220"/>
       <c r="N62" s="50"/>
       <c r="O62" s="49"/>
-      <c r="U62" s="203"/>
-      <c r="V62" s="204"/>
-      <c r="W62" s="204"/>
-      <c r="X62" s="204"/>
-      <c r="Y62" s="205"/>
-      <c r="Z62" s="181"/>
-      <c r="AA62" s="182"/>
-      <c r="AB62" s="182"/>
-      <c r="AC62" s="182"/>
-      <c r="AD62" s="182"/>
-      <c r="AE62" s="182"/>
-      <c r="AF62" s="182"/>
-      <c r="AG62" s="182"/>
-      <c r="AH62" s="183"/>
+      <c r="U62" s="205"/>
+      <c r="V62" s="206"/>
+      <c r="W62" s="206"/>
+      <c r="X62" s="206"/>
+      <c r="Y62" s="207"/>
+      <c r="Z62" s="228"/>
+      <c r="AA62" s="229"/>
+      <c r="AB62" s="229"/>
+      <c r="AC62" s="229"/>
+      <c r="AD62" s="229"/>
+      <c r="AE62" s="229"/>
+      <c r="AF62" s="229"/>
+      <c r="AG62" s="229"/>
+      <c r="AH62" s="230"/>
       <c r="AI62" s="50"/>
     </row>
     <row r="63" spans="1:35" x14ac:dyDescent="0.2">
@@ -6595,34 +6595,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="U47:Y47"/>
-    <mergeCell ref="Z47:AH47"/>
-    <mergeCell ref="A48:E62"/>
-    <mergeCell ref="F48:M62"/>
-    <mergeCell ref="U48:Y62"/>
-    <mergeCell ref="Z48:AH62"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="F47:M47"/>
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="Q33:R33"/>
-    <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="P38:S38"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="Q30:R30"/>
-    <mergeCell ref="U30:V30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="Q31:R31"/>
-    <mergeCell ref="U31:V31"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="A28:S28"/>
-    <mergeCell ref="U28:AJ28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="P29:R29"/>
-    <mergeCell ref="U29:V29"/>
-    <mergeCell ref="AF29:AG29"/>
-    <mergeCell ref="AJ29:AL29"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="B2:E3"/>
     <mergeCell ref="I3:L3"/>
@@ -6635,6 +6607,34 @@
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="A28:S28"/>
+    <mergeCell ref="U28:AJ28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="P29:R29"/>
+    <mergeCell ref="U29:V29"/>
+    <mergeCell ref="AF29:AG29"/>
+    <mergeCell ref="AJ29:AL29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="U30:V30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="Q31:R31"/>
+    <mergeCell ref="U31:V31"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="P38:S38"/>
+    <mergeCell ref="U47:Y47"/>
+    <mergeCell ref="Z47:AH47"/>
+    <mergeCell ref="A48:E62"/>
+    <mergeCell ref="F48:M62"/>
+    <mergeCell ref="U48:Y62"/>
+    <mergeCell ref="Z48:AH62"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="F47:M47"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6869,15 +6869,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="03fd382f-fd16-45b5-8306-1be73a58e004" xsi:nil="true"/>
@@ -6886,6 +6877,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6908,14 +6908,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74D37766-22C8-4101-A6A1-3DEEE84685D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49A4B1E7-D809-4F18-8A5B-250753158AE8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -6924,4 +6916,12 @@
     <ds:schemaRef ds:uri="3314f2a4-48e9-4e28-8da9-3bfbc3a74041"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74D37766-22C8-4101-A6A1-3DEEE84685D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Enhance data processing in sql_data_handler; add methods for complex data retrieval and improve handling of Excel data addresses
</commit_message>
<xml_diff>
--- a/datasheets/20250708 Runsheet.xlsx
+++ b/datasheets/20250708 Runsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C376038\Documents\python_code\cvd_sql\datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE8F530-BF56-4DD9-ACB4-7148B1684636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C91A793-6162-4742-A6C3-F1E53BE5FB91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38340" yWindow="2865" windowWidth="14400" windowHeight="7365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-10760" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Run 1" sheetId="26" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="128">
   <si>
     <t>Lab 104D SierraTherm CVD Coater Data Sheet</t>
   </si>
@@ -1816,80 +1816,74 @@
     <xf numFmtId="0" fontId="22" fillId="2" borderId="58" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="10" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="16" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="38" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="30" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="39" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1924,15 +1918,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1954,58 +1939,73 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="10" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="16" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="38" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="30" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2330,7 +2330,7 @@
   <dimension ref="A1:AM76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47:M47"/>
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="10" x14ac:dyDescent="0.2"/>
@@ -2395,12 +2395,12 @@
     </row>
     <row r="2" spans="1:25" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
-      <c r="B2" s="175" t="s">
+      <c r="B2" s="233" t="s">
         <v>119</v>
       </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
+      <c r="C2" s="233"/>
+      <c r="D2" s="233"/>
+      <c r="E2" s="233"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -2417,21 +2417,21 @@
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="176"/>
-      <c r="C3" s="176"/>
-      <c r="D3" s="176"/>
-      <c r="E3" s="176"/>
+      <c r="B3" s="234"/>
+      <c r="C3" s="234"/>
+      <c r="D3" s="234"/>
+      <c r="E3" s="234"/>
       <c r="F3" s="5"/>
       <c r="G3" s="6"/>
       <c r="H3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="177">
+      <c r="I3" s="235">
         <v>20250708</v>
       </c>
-      <c r="J3" s="177"/>
-      <c r="K3" s="177"/>
-      <c r="L3" s="177"/>
+      <c r="J3" s="235"/>
+      <c r="K3" s="235"/>
+      <c r="L3" s="235"/>
       <c r="M3" s="8" t="s">
         <v>3</v>
       </c>
@@ -2463,25 +2463,25 @@
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="178">
+      <c r="B5" s="236">
         <v>45846</v>
       </c>
-      <c r="C5" s="178"/>
-      <c r="D5" s="178"/>
-      <c r="E5" s="178"/>
+      <c r="C5" s="236"/>
+      <c r="D5" s="236"/>
+      <c r="E5" s="236"/>
       <c r="F5" s="5"/>
       <c r="G5" s="6"/>
       <c r="H5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="177" t="s">
+      <c r="I5" s="235" t="s">
         <v>120</v>
       </c>
-      <c r="J5" s="177"/>
-      <c r="K5" s="177"/>
-      <c r="L5" s="177"/>
-      <c r="M5" s="177"/>
-      <c r="N5" s="177"/>
+      <c r="J5" s="235"/>
+      <c r="K5" s="235"/>
+      <c r="L5" s="235"/>
+      <c r="M5" s="235"/>
+      <c r="N5" s="235"/>
       <c r="O5" s="155"/>
       <c r="Y5" s="29"/>
     </row>
@@ -2539,11 +2539,11 @@
       <c r="F9" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="179" t="s">
+      <c r="G9" s="237" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="180"/>
-      <c r="I9" s="180"/>
+      <c r="H9" s="238"/>
+      <c r="I9" s="238"/>
       <c r="J9" s="19" t="s">
         <v>10</v>
       </c>
@@ -2574,11 +2574,11 @@
       <c r="F10" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="189" t="s">
+      <c r="G10" s="222" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="190"/>
-      <c r="I10" s="190"/>
+      <c r="H10" s="223"/>
+      <c r="I10" s="223"/>
       <c r="J10" s="21" t="s">
         <v>10</v>
       </c>
@@ -2609,11 +2609,11 @@
       <c r="F11" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="191" t="s">
+      <c r="G11" s="224" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="192"/>
-      <c r="I11" s="192"/>
+      <c r="H11" s="225"/>
+      <c r="I11" s="225"/>
       <c r="J11" s="62" t="s">
         <v>10</v>
       </c>
@@ -2774,10 +2774,10 @@
       <c r="B19" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="221" t="s">
+      <c r="E19" s="194" t="s">
         <v>46</v>
       </c>
-      <c r="F19" s="222"/>
+      <c r="F19" s="195"/>
       <c r="G19" s="20">
         <v>200</v>
       </c>
@@ -2794,10 +2794,10 @@
         <v>48</v>
       </c>
       <c r="B20" s="21"/>
-      <c r="E20" s="223" t="s">
+      <c r="E20" s="196" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="224"/>
+      <c r="F20" s="197"/>
       <c r="G20" s="22">
         <v>100</v>
       </c>
@@ -2808,10 +2808,10 @@
         <v>50</v>
       </c>
       <c r="B21" s="65"/>
-      <c r="E21" s="223" t="s">
+      <c r="E21" s="196" t="s">
         <v>51</v>
       </c>
-      <c r="F21" s="224"/>
+      <c r="F21" s="197"/>
       <c r="G21" s="22">
         <v>50</v>
       </c>
@@ -2822,10 +2822,10 @@
         <v>52</v>
       </c>
       <c r="B22" s="66"/>
-      <c r="E22" s="223" t="s">
+      <c r="E22" s="196" t="s">
         <v>53</v>
       </c>
-      <c r="F22" s="224"/>
+      <c r="F22" s="197"/>
       <c r="G22" s="23">
         <v>120</v>
       </c>
@@ -2838,10 +2838,10 @@
       <c r="B23" s="24">
         <v>5</v>
       </c>
-      <c r="E23" s="223" t="s">
+      <c r="E23" s="196" t="s">
         <v>55</v>
       </c>
-      <c r="F23" s="224"/>
+      <c r="F23" s="197"/>
       <c r="G23" s="23">
         <v>200</v>
       </c>
@@ -2854,10 +2854,10 @@
       <c r="B24" s="24">
         <v>5</v>
       </c>
-      <c r="E24" s="231" t="s">
+      <c r="E24" s="184" t="s">
         <v>57</v>
       </c>
-      <c r="F24" s="232"/>
+      <c r="F24" s="185"/>
       <c r="G24" s="25">
         <v>0.03</v>
       </c>
@@ -2889,50 +2889,50 @@
     </row>
     <row r="27" spans="1:39" ht="10.5" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="1:39" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="184" t="s">
+      <c r="A28" s="217" t="s">
         <v>59</v>
       </c>
-      <c r="B28" s="184"/>
-      <c r="C28" s="184"/>
-      <c r="D28" s="184"/>
-      <c r="E28" s="184"/>
-      <c r="F28" s="184"/>
-      <c r="G28" s="185"/>
-      <c r="H28" s="185"/>
-      <c r="I28" s="185"/>
-      <c r="J28" s="185"/>
-      <c r="K28" s="185"/>
-      <c r="L28" s="185"/>
-      <c r="M28" s="185"/>
-      <c r="N28" s="185"/>
-      <c r="O28" s="185"/>
-      <c r="P28" s="185"/>
-      <c r="Q28" s="185"/>
-      <c r="R28" s="185"/>
-      <c r="S28" s="185"/>
-      <c r="U28" s="185" t="s">
+      <c r="B28" s="217"/>
+      <c r="C28" s="217"/>
+      <c r="D28" s="217"/>
+      <c r="E28" s="217"/>
+      <c r="F28" s="217"/>
+      <c r="G28" s="218"/>
+      <c r="H28" s="218"/>
+      <c r="I28" s="218"/>
+      <c r="J28" s="218"/>
+      <c r="K28" s="218"/>
+      <c r="L28" s="218"/>
+      <c r="M28" s="218"/>
+      <c r="N28" s="218"/>
+      <c r="O28" s="218"/>
+      <c r="P28" s="218"/>
+      <c r="Q28" s="218"/>
+      <c r="R28" s="218"/>
+      <c r="S28" s="218"/>
+      <c r="U28" s="218" t="s">
         <v>60</v>
       </c>
-      <c r="V28" s="185"/>
-      <c r="W28" s="185"/>
-      <c r="X28" s="185"/>
-      <c r="Y28" s="185"/>
-      <c r="Z28" s="185"/>
-      <c r="AA28" s="185"/>
-      <c r="AB28" s="185"/>
-      <c r="AC28" s="185"/>
-      <c r="AD28" s="185"/>
-      <c r="AE28" s="185"/>
-      <c r="AF28" s="185"/>
-      <c r="AG28" s="185"/>
-      <c r="AH28" s="185"/>
-      <c r="AI28" s="185"/>
-      <c r="AJ28" s="185"/>
+      <c r="V28" s="218"/>
+      <c r="W28" s="218"/>
+      <c r="X28" s="218"/>
+      <c r="Y28" s="218"/>
+      <c r="Z28" s="218"/>
+      <c r="AA28" s="218"/>
+      <c r="AB28" s="218"/>
+      <c r="AC28" s="218"/>
+      <c r="AD28" s="218"/>
+      <c r="AE28" s="218"/>
+      <c r="AF28" s="218"/>
+      <c r="AG28" s="218"/>
+      <c r="AH28" s="218"/>
+      <c r="AI28" s="218"/>
+      <c r="AJ28" s="218"/>
       <c r="AM28" s="51"/>
     </row>
     <row r="29" spans="1:39" ht="18" x14ac:dyDescent="0.4">
-      <c r="A29" s="181"/>
-      <c r="B29" s="199"/>
+      <c r="A29" s="192"/>
+      <c r="B29" s="232"/>
       <c r="C29" s="54" t="s">
         <v>61</v>
       </c>
@@ -2945,19 +2945,19 @@
       <c r="F29" s="28">
         <v>3</v>
       </c>
-      <c r="L29" s="181" t="s">
+      <c r="L29" s="192" t="s">
         <v>127</v>
       </c>
-      <c r="M29" s="183"/>
+      <c r="M29" s="193"/>
       <c r="N29" s="157"/>
       <c r="O29" s="158"/>
-      <c r="P29" s="181" t="s">
+      <c r="P29" s="192" t="s">
         <v>63</v>
       </c>
-      <c r="Q29" s="182"/>
-      <c r="R29" s="183"/>
-      <c r="U29" s="233"/>
-      <c r="V29" s="234"/>
+      <c r="Q29" s="216"/>
+      <c r="R29" s="193"/>
+      <c r="U29" s="186"/>
+      <c r="V29" s="187"/>
       <c r="W29" s="54" t="s">
         <v>61</v>
       </c>
@@ -2971,22 +2971,22 @@
         <v>3</v>
       </c>
       <c r="AE29" s="121"/>
-      <c r="AF29" s="181" t="s">
+      <c r="AF29" s="192" t="s">
         <v>62</v>
       </c>
-      <c r="AG29" s="183"/>
+      <c r="AG29" s="193"/>
       <c r="AH29" s="153"/>
-      <c r="AJ29" s="181" t="s">
+      <c r="AJ29" s="192" t="s">
         <v>63</v>
       </c>
-      <c r="AK29" s="182"/>
-      <c r="AL29" s="183"/>
+      <c r="AK29" s="216"/>
+      <c r="AL29" s="193"/>
     </row>
     <row r="30" spans="1:39" ht="20" x14ac:dyDescent="0.4">
-      <c r="A30" s="197" t="s">
+      <c r="A30" s="230" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="198"/>
+      <c r="B30" s="231"/>
       <c r="C30" s="52">
         <v>6</v>
       </c>
@@ -3010,12 +3010,12 @@
       <c r="P30" s="125" t="s">
         <v>66</v>
       </c>
-      <c r="Q30" s="193"/>
-      <c r="R30" s="194"/>
-      <c r="U30" s="235" t="s">
+      <c r="Q30" s="226"/>
+      <c r="R30" s="227"/>
+      <c r="U30" s="188" t="s">
         <v>64</v>
       </c>
-      <c r="V30" s="236"/>
+      <c r="V30" s="189"/>
       <c r="W30" s="52"/>
       <c r="X30" s="53"/>
       <c r="Y30" s="53"/>
@@ -3033,10 +3033,10 @@
       <c r="AL30" s="145"/>
     </row>
     <row r="31" spans="1:39" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="200" t="s">
+      <c r="A31" s="198" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="201"/>
+      <c r="B31" s="199"/>
       <c r="C31" s="56">
         <v>46.2</v>
       </c>
@@ -3060,12 +3060,12 @@
       <c r="P31" s="125" t="s">
         <v>69</v>
       </c>
-      <c r="Q31" s="193"/>
-      <c r="R31" s="194"/>
-      <c r="U31" s="237" t="s">
+      <c r="Q31" s="226"/>
+      <c r="R31" s="227"/>
+      <c r="U31" s="190" t="s">
         <v>67</v>
       </c>
-      <c r="V31" s="238"/>
+      <c r="V31" s="191"/>
       <c r="W31" s="56"/>
       <c r="X31" s="56"/>
       <c r="Y31" s="56"/>
@@ -3092,8 +3092,8 @@
       <c r="P32" s="125" t="s">
         <v>70</v>
       </c>
-      <c r="Q32" s="193"/>
-      <c r="R32" s="194"/>
+      <c r="Q32" s="226"/>
+      <c r="R32" s="227"/>
       <c r="U32" s="146"/>
       <c r="V32" s="29"/>
       <c r="W32" s="29"/>
@@ -3138,8 +3138,8 @@
       <c r="P33" s="125" t="s">
         <v>76</v>
       </c>
-      <c r="Q33" s="193"/>
-      <c r="R33" s="194"/>
+      <c r="Q33" s="226"/>
+      <c r="R33" s="227"/>
       <c r="U33" s="147"/>
       <c r="V33" s="30" t="s">
         <v>71</v>
@@ -3196,8 +3196,8 @@
       <c r="P34" s="125" t="s">
         <v>77</v>
       </c>
-      <c r="Q34" s="193"/>
-      <c r="R34" s="194"/>
+      <c r="Q34" s="226"/>
+      <c r="R34" s="227"/>
       <c r="W34" s="33">
         <v>160</v>
       </c>
@@ -3254,8 +3254,8 @@
       <c r="P36" s="148" t="s">
         <v>78</v>
       </c>
-      <c r="Q36" s="195"/>
-      <c r="R36" s="196"/>
+      <c r="Q36" s="228"/>
+      <c r="R36" s="229"/>
       <c r="U36" s="169"/>
       <c r="V36" s="170"/>
       <c r="W36" s="170"/>
@@ -3349,12 +3349,12 @@
         <v>90</v>
       </c>
       <c r="N38" s="165"/>
-      <c r="P38" s="186" t="s">
+      <c r="P38" s="219" t="s">
         <v>91</v>
       </c>
-      <c r="Q38" s="187"/>
-      <c r="R38" s="187"/>
-      <c r="S38" s="188"/>
+      <c r="Q38" s="220"/>
+      <c r="R38" s="220"/>
+      <c r="S38" s="221"/>
       <c r="U38" s="107" t="s">
         <v>80</v>
       </c>
@@ -3754,8 +3754,8 @@
       <c r="C44" s="18"/>
       <c r="D44" s="18"/>
       <c r="E44" s="18"/>
-      <c r="F44" s="68">
-        <v>2</v>
+      <c r="F44" s="68" t="s">
+        <v>115</v>
       </c>
       <c r="G44" s="161"/>
       <c r="H44" s="162"/>
@@ -3814,527 +3814,527 @@
     </row>
     <row r="46" spans="1:38" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="1:38" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="208" t="s">
+      <c r="A47" s="206" t="s">
         <v>116</v>
       </c>
-      <c r="B47" s="209"/>
-      <c r="C47" s="209"/>
-      <c r="D47" s="209"/>
-      <c r="E47" s="210"/>
-      <c r="F47" s="211" t="s">
+      <c r="B47" s="207"/>
+      <c r="C47" s="207"/>
+      <c r="D47" s="207"/>
+      <c r="E47" s="208"/>
+      <c r="F47" s="175" t="s">
         <v>117</v>
       </c>
-      <c r="G47" s="212"/>
-      <c r="H47" s="212"/>
-      <c r="I47" s="212"/>
-      <c r="J47" s="212"/>
-      <c r="K47" s="212"/>
-      <c r="L47" s="212"/>
-      <c r="M47" s="213"/>
+      <c r="G47" s="176"/>
+      <c r="H47" s="176"/>
+      <c r="I47" s="176"/>
+      <c r="J47" s="176"/>
+      <c r="K47" s="176"/>
+      <c r="L47" s="176"/>
+      <c r="M47" s="177"/>
       <c r="N47" s="50"/>
       <c r="O47" s="49"/>
-      <c r="U47" s="208" t="s">
+      <c r="U47" s="206" t="s">
         <v>118</v>
       </c>
-      <c r="V47" s="209"/>
-      <c r="W47" s="209"/>
-      <c r="X47" s="209"/>
-      <c r="Y47" s="210"/>
-      <c r="Z47" s="211" t="s">
+      <c r="V47" s="207"/>
+      <c r="W47" s="207"/>
+      <c r="X47" s="207"/>
+      <c r="Y47" s="208"/>
+      <c r="Z47" s="175" t="s">
         <v>117</v>
       </c>
-      <c r="AA47" s="212"/>
-      <c r="AB47" s="212"/>
-      <c r="AC47" s="212"/>
-      <c r="AD47" s="212"/>
-      <c r="AE47" s="212"/>
-      <c r="AF47" s="212"/>
-      <c r="AG47" s="212"/>
-      <c r="AH47" s="213"/>
+      <c r="AA47" s="176"/>
+      <c r="AB47" s="176"/>
+      <c r="AC47" s="176"/>
+      <c r="AD47" s="176"/>
+      <c r="AE47" s="176"/>
+      <c r="AF47" s="176"/>
+      <c r="AG47" s="176"/>
+      <c r="AH47" s="177"/>
       <c r="AI47" s="50"/>
     </row>
     <row r="48" spans="1:38" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="202" t="s">
+      <c r="A48" s="200" t="s">
         <v>124</v>
       </c>
-      <c r="B48" s="203"/>
-      <c r="C48" s="203"/>
-      <c r="D48" s="203"/>
-      <c r="E48" s="204"/>
-      <c r="F48" s="214" t="s">
+      <c r="B48" s="201"/>
+      <c r="C48" s="201"/>
+      <c r="D48" s="201"/>
+      <c r="E48" s="202"/>
+      <c r="F48" s="209" t="s">
         <v>122</v>
       </c>
-      <c r="G48" s="215"/>
-      <c r="H48" s="215"/>
-      <c r="I48" s="215"/>
-      <c r="J48" s="215"/>
-      <c r="K48" s="215"/>
-      <c r="L48" s="215"/>
-      <c r="M48" s="216"/>
+      <c r="G48" s="210"/>
+      <c r="H48" s="210"/>
+      <c r="I48" s="210"/>
+      <c r="J48" s="210"/>
+      <c r="K48" s="210"/>
+      <c r="L48" s="210"/>
+      <c r="M48" s="211"/>
       <c r="N48" s="50"/>
       <c r="O48" s="49"/>
-      <c r="U48" s="202"/>
-      <c r="V48" s="203"/>
-      <c r="W48" s="203"/>
-      <c r="X48" s="203"/>
-      <c r="Y48" s="204"/>
-      <c r="Z48" s="225"/>
-      <c r="AA48" s="226"/>
-      <c r="AB48" s="226"/>
-      <c r="AC48" s="226"/>
-      <c r="AD48" s="226"/>
-      <c r="AE48" s="226"/>
-      <c r="AF48" s="226"/>
-      <c r="AG48" s="226"/>
-      <c r="AH48" s="227"/>
+      <c r="U48" s="200"/>
+      <c r="V48" s="201"/>
+      <c r="W48" s="201"/>
+      <c r="X48" s="201"/>
+      <c r="Y48" s="202"/>
+      <c r="Z48" s="178"/>
+      <c r="AA48" s="179"/>
+      <c r="AB48" s="179"/>
+      <c r="AC48" s="179"/>
+      <c r="AD48" s="179"/>
+      <c r="AE48" s="179"/>
+      <c r="AF48" s="179"/>
+      <c r="AG48" s="179"/>
+      <c r="AH48" s="180"/>
       <c r="AI48" s="50"/>
     </row>
     <row r="49" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="202"/>
-      <c r="B49" s="203"/>
-      <c r="C49" s="203"/>
-      <c r="D49" s="203"/>
-      <c r="E49" s="204"/>
-      <c r="F49" s="217"/>
-      <c r="G49" s="215"/>
-      <c r="H49" s="215"/>
-      <c r="I49" s="215"/>
-      <c r="J49" s="215"/>
-      <c r="K49" s="215"/>
-      <c r="L49" s="215"/>
-      <c r="M49" s="216"/>
+      <c r="A49" s="200"/>
+      <c r="B49" s="201"/>
+      <c r="C49" s="201"/>
+      <c r="D49" s="201"/>
+      <c r="E49" s="202"/>
+      <c r="F49" s="212"/>
+      <c r="G49" s="210"/>
+      <c r="H49" s="210"/>
+      <c r="I49" s="210"/>
+      <c r="J49" s="210"/>
+      <c r="K49" s="210"/>
+      <c r="L49" s="210"/>
+      <c r="M49" s="211"/>
       <c r="N49" s="50"/>
       <c r="O49" s="49"/>
-      <c r="U49" s="202"/>
-      <c r="V49" s="203"/>
-      <c r="W49" s="203"/>
-      <c r="X49" s="203"/>
-      <c r="Y49" s="204"/>
-      <c r="Z49" s="225"/>
-      <c r="AA49" s="226"/>
-      <c r="AB49" s="226"/>
-      <c r="AC49" s="226"/>
-      <c r="AD49" s="226"/>
-      <c r="AE49" s="226"/>
-      <c r="AF49" s="226"/>
-      <c r="AG49" s="226"/>
-      <c r="AH49" s="227"/>
+      <c r="U49" s="200"/>
+      <c r="V49" s="201"/>
+      <c r="W49" s="201"/>
+      <c r="X49" s="201"/>
+      <c r="Y49" s="202"/>
+      <c r="Z49" s="178"/>
+      <c r="AA49" s="179"/>
+      <c r="AB49" s="179"/>
+      <c r="AC49" s="179"/>
+      <c r="AD49" s="179"/>
+      <c r="AE49" s="179"/>
+      <c r="AF49" s="179"/>
+      <c r="AG49" s="179"/>
+      <c r="AH49" s="180"/>
       <c r="AI49" s="50"/>
     </row>
     <row r="50" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="202"/>
-      <c r="B50" s="203"/>
-      <c r="C50" s="203"/>
-      <c r="D50" s="203"/>
-      <c r="E50" s="204"/>
-      <c r="F50" s="217"/>
-      <c r="G50" s="215"/>
-      <c r="H50" s="215"/>
-      <c r="I50" s="215"/>
-      <c r="J50" s="215"/>
-      <c r="K50" s="215"/>
-      <c r="L50" s="215"/>
-      <c r="M50" s="216"/>
+      <c r="A50" s="200"/>
+      <c r="B50" s="201"/>
+      <c r="C50" s="201"/>
+      <c r="D50" s="201"/>
+      <c r="E50" s="202"/>
+      <c r="F50" s="212"/>
+      <c r="G50" s="210"/>
+      <c r="H50" s="210"/>
+      <c r="I50" s="210"/>
+      <c r="J50" s="210"/>
+      <c r="K50" s="210"/>
+      <c r="L50" s="210"/>
+      <c r="M50" s="211"/>
       <c r="N50" s="50"/>
       <c r="O50" s="49"/>
-      <c r="U50" s="202"/>
-      <c r="V50" s="203"/>
-      <c r="W50" s="203"/>
-      <c r="X50" s="203"/>
-      <c r="Y50" s="204"/>
-      <c r="Z50" s="225"/>
-      <c r="AA50" s="226"/>
-      <c r="AB50" s="226"/>
-      <c r="AC50" s="226"/>
-      <c r="AD50" s="226"/>
-      <c r="AE50" s="226"/>
-      <c r="AF50" s="226"/>
-      <c r="AG50" s="226"/>
-      <c r="AH50" s="227"/>
+      <c r="U50" s="200"/>
+      <c r="V50" s="201"/>
+      <c r="W50" s="201"/>
+      <c r="X50" s="201"/>
+      <c r="Y50" s="202"/>
+      <c r="Z50" s="178"/>
+      <c r="AA50" s="179"/>
+      <c r="AB50" s="179"/>
+      <c r="AC50" s="179"/>
+      <c r="AD50" s="179"/>
+      <c r="AE50" s="179"/>
+      <c r="AF50" s="179"/>
+      <c r="AG50" s="179"/>
+      <c r="AH50" s="180"/>
       <c r="AI50" s="50"/>
     </row>
     <row r="51" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="202"/>
-      <c r="B51" s="203"/>
-      <c r="C51" s="203"/>
-      <c r="D51" s="203"/>
-      <c r="E51" s="204"/>
-      <c r="F51" s="217"/>
-      <c r="G51" s="215"/>
-      <c r="H51" s="215"/>
-      <c r="I51" s="215"/>
-      <c r="J51" s="215"/>
-      <c r="K51" s="215"/>
-      <c r="L51" s="215"/>
-      <c r="M51" s="216"/>
+      <c r="A51" s="200"/>
+      <c r="B51" s="201"/>
+      <c r="C51" s="201"/>
+      <c r="D51" s="201"/>
+      <c r="E51" s="202"/>
+      <c r="F51" s="212"/>
+      <c r="G51" s="210"/>
+      <c r="H51" s="210"/>
+      <c r="I51" s="210"/>
+      <c r="J51" s="210"/>
+      <c r="K51" s="210"/>
+      <c r="L51" s="210"/>
+      <c r="M51" s="211"/>
       <c r="N51" s="50"/>
       <c r="O51" s="49"/>
-      <c r="U51" s="202"/>
-      <c r="V51" s="203"/>
-      <c r="W51" s="203"/>
-      <c r="X51" s="203"/>
-      <c r="Y51" s="204"/>
-      <c r="Z51" s="225"/>
-      <c r="AA51" s="226"/>
-      <c r="AB51" s="226"/>
-      <c r="AC51" s="226"/>
-      <c r="AD51" s="226"/>
-      <c r="AE51" s="226"/>
-      <c r="AF51" s="226"/>
-      <c r="AG51" s="226"/>
-      <c r="AH51" s="227"/>
+      <c r="U51" s="200"/>
+      <c r="V51" s="201"/>
+      <c r="W51" s="201"/>
+      <c r="X51" s="201"/>
+      <c r="Y51" s="202"/>
+      <c r="Z51" s="178"/>
+      <c r="AA51" s="179"/>
+      <c r="AB51" s="179"/>
+      <c r="AC51" s="179"/>
+      <c r="AD51" s="179"/>
+      <c r="AE51" s="179"/>
+      <c r="AF51" s="179"/>
+      <c r="AG51" s="179"/>
+      <c r="AH51" s="180"/>
       <c r="AI51" s="50"/>
     </row>
     <row r="52" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="202"/>
-      <c r="B52" s="203"/>
-      <c r="C52" s="203"/>
-      <c r="D52" s="203"/>
-      <c r="E52" s="204"/>
-      <c r="F52" s="217"/>
-      <c r="G52" s="215"/>
-      <c r="H52" s="215"/>
-      <c r="I52" s="215"/>
-      <c r="J52" s="215"/>
-      <c r="K52" s="215"/>
-      <c r="L52" s="215"/>
-      <c r="M52" s="216"/>
+      <c r="A52" s="200"/>
+      <c r="B52" s="201"/>
+      <c r="C52" s="201"/>
+      <c r="D52" s="201"/>
+      <c r="E52" s="202"/>
+      <c r="F52" s="212"/>
+      <c r="G52" s="210"/>
+      <c r="H52" s="210"/>
+      <c r="I52" s="210"/>
+      <c r="J52" s="210"/>
+      <c r="K52" s="210"/>
+      <c r="L52" s="210"/>
+      <c r="M52" s="211"/>
       <c r="N52" s="50"/>
       <c r="O52" s="49"/>
-      <c r="U52" s="202"/>
-      <c r="V52" s="203"/>
-      <c r="W52" s="203"/>
-      <c r="X52" s="203"/>
-      <c r="Y52" s="204"/>
-      <c r="Z52" s="225"/>
-      <c r="AA52" s="226"/>
-      <c r="AB52" s="226"/>
-      <c r="AC52" s="226"/>
-      <c r="AD52" s="226"/>
-      <c r="AE52" s="226"/>
-      <c r="AF52" s="226"/>
-      <c r="AG52" s="226"/>
-      <c r="AH52" s="227"/>
+      <c r="U52" s="200"/>
+      <c r="V52" s="201"/>
+      <c r="W52" s="201"/>
+      <c r="X52" s="201"/>
+      <c r="Y52" s="202"/>
+      <c r="Z52" s="178"/>
+      <c r="AA52" s="179"/>
+      <c r="AB52" s="179"/>
+      <c r="AC52" s="179"/>
+      <c r="AD52" s="179"/>
+      <c r="AE52" s="179"/>
+      <c r="AF52" s="179"/>
+      <c r="AG52" s="179"/>
+      <c r="AH52" s="180"/>
       <c r="AI52" s="50"/>
     </row>
     <row r="53" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="202"/>
-      <c r="B53" s="203"/>
-      <c r="C53" s="203"/>
-      <c r="D53" s="203"/>
-      <c r="E53" s="204"/>
-      <c r="F53" s="217"/>
-      <c r="G53" s="215"/>
-      <c r="H53" s="215"/>
-      <c r="I53" s="215"/>
-      <c r="J53" s="215"/>
-      <c r="K53" s="215"/>
-      <c r="L53" s="215"/>
-      <c r="M53" s="216"/>
+      <c r="A53" s="200"/>
+      <c r="B53" s="201"/>
+      <c r="C53" s="201"/>
+      <c r="D53" s="201"/>
+      <c r="E53" s="202"/>
+      <c r="F53" s="212"/>
+      <c r="G53" s="210"/>
+      <c r="H53" s="210"/>
+      <c r="I53" s="210"/>
+      <c r="J53" s="210"/>
+      <c r="K53" s="210"/>
+      <c r="L53" s="210"/>
+      <c r="M53" s="211"/>
       <c r="N53" s="50"/>
       <c r="O53" s="49"/>
-      <c r="U53" s="202"/>
-      <c r="V53" s="203"/>
-      <c r="W53" s="203"/>
-      <c r="X53" s="203"/>
-      <c r="Y53" s="204"/>
-      <c r="Z53" s="225"/>
-      <c r="AA53" s="226"/>
-      <c r="AB53" s="226"/>
-      <c r="AC53" s="226"/>
-      <c r="AD53" s="226"/>
-      <c r="AE53" s="226"/>
-      <c r="AF53" s="226"/>
-      <c r="AG53" s="226"/>
-      <c r="AH53" s="227"/>
+      <c r="U53" s="200"/>
+      <c r="V53" s="201"/>
+      <c r="W53" s="201"/>
+      <c r="X53" s="201"/>
+      <c r="Y53" s="202"/>
+      <c r="Z53" s="178"/>
+      <c r="AA53" s="179"/>
+      <c r="AB53" s="179"/>
+      <c r="AC53" s="179"/>
+      <c r="AD53" s="179"/>
+      <c r="AE53" s="179"/>
+      <c r="AF53" s="179"/>
+      <c r="AG53" s="179"/>
+      <c r="AH53" s="180"/>
       <c r="AI53" s="50"/>
     </row>
     <row r="54" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="202"/>
-      <c r="B54" s="203"/>
-      <c r="C54" s="203"/>
-      <c r="D54" s="203"/>
-      <c r="E54" s="204"/>
-      <c r="F54" s="217"/>
-      <c r="G54" s="215"/>
-      <c r="H54" s="215"/>
-      <c r="I54" s="215"/>
-      <c r="J54" s="215"/>
-      <c r="K54" s="215"/>
-      <c r="L54" s="215"/>
-      <c r="M54" s="216"/>
+      <c r="A54" s="200"/>
+      <c r="B54" s="201"/>
+      <c r="C54" s="201"/>
+      <c r="D54" s="201"/>
+      <c r="E54" s="202"/>
+      <c r="F54" s="212"/>
+      <c r="G54" s="210"/>
+      <c r="H54" s="210"/>
+      <c r="I54" s="210"/>
+      <c r="J54" s="210"/>
+      <c r="K54" s="210"/>
+      <c r="L54" s="210"/>
+      <c r="M54" s="211"/>
       <c r="N54" s="50"/>
       <c r="O54" s="49"/>
-      <c r="U54" s="202"/>
-      <c r="V54" s="203"/>
-      <c r="W54" s="203"/>
-      <c r="X54" s="203"/>
-      <c r="Y54" s="204"/>
-      <c r="Z54" s="225"/>
-      <c r="AA54" s="226"/>
-      <c r="AB54" s="226"/>
-      <c r="AC54" s="226"/>
-      <c r="AD54" s="226"/>
-      <c r="AE54" s="226"/>
-      <c r="AF54" s="226"/>
-      <c r="AG54" s="226"/>
-      <c r="AH54" s="227"/>
+      <c r="U54" s="200"/>
+      <c r="V54" s="201"/>
+      <c r="W54" s="201"/>
+      <c r="X54" s="201"/>
+      <c r="Y54" s="202"/>
+      <c r="Z54" s="178"/>
+      <c r="AA54" s="179"/>
+      <c r="AB54" s="179"/>
+      <c r="AC54" s="179"/>
+      <c r="AD54" s="179"/>
+      <c r="AE54" s="179"/>
+      <c r="AF54" s="179"/>
+      <c r="AG54" s="179"/>
+      <c r="AH54" s="180"/>
       <c r="AI54" s="50"/>
     </row>
     <row r="55" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="202"/>
-      <c r="B55" s="203"/>
-      <c r="C55" s="203"/>
-      <c r="D55" s="203"/>
-      <c r="E55" s="204"/>
-      <c r="F55" s="217"/>
-      <c r="G55" s="215"/>
-      <c r="H55" s="215"/>
-      <c r="I55" s="215"/>
-      <c r="J55" s="215"/>
-      <c r="K55" s="215"/>
-      <c r="L55" s="215"/>
-      <c r="M55" s="216"/>
+      <c r="A55" s="200"/>
+      <c r="B55" s="201"/>
+      <c r="C55" s="201"/>
+      <c r="D55" s="201"/>
+      <c r="E55" s="202"/>
+      <c r="F55" s="212"/>
+      <c r="G55" s="210"/>
+      <c r="H55" s="210"/>
+      <c r="I55" s="210"/>
+      <c r="J55" s="210"/>
+      <c r="K55" s="210"/>
+      <c r="L55" s="210"/>
+      <c r="M55" s="211"/>
       <c r="N55" s="50"/>
       <c r="O55" s="49"/>
-      <c r="U55" s="202"/>
-      <c r="V55" s="203"/>
-      <c r="W55" s="203"/>
-      <c r="X55" s="203"/>
-      <c r="Y55" s="204"/>
-      <c r="Z55" s="225"/>
-      <c r="AA55" s="226"/>
-      <c r="AB55" s="226"/>
-      <c r="AC55" s="226"/>
-      <c r="AD55" s="226"/>
-      <c r="AE55" s="226"/>
-      <c r="AF55" s="226"/>
-      <c r="AG55" s="226"/>
-      <c r="AH55" s="227"/>
+      <c r="U55" s="200"/>
+      <c r="V55" s="201"/>
+      <c r="W55" s="201"/>
+      <c r="X55" s="201"/>
+      <c r="Y55" s="202"/>
+      <c r="Z55" s="178"/>
+      <c r="AA55" s="179"/>
+      <c r="AB55" s="179"/>
+      <c r="AC55" s="179"/>
+      <c r="AD55" s="179"/>
+      <c r="AE55" s="179"/>
+      <c r="AF55" s="179"/>
+      <c r="AG55" s="179"/>
+      <c r="AH55" s="180"/>
       <c r="AI55" s="50"/>
     </row>
     <row r="56" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="202"/>
-      <c r="B56" s="203"/>
-      <c r="C56" s="203"/>
-      <c r="D56" s="203"/>
-      <c r="E56" s="204"/>
-      <c r="F56" s="217"/>
-      <c r="G56" s="215"/>
-      <c r="H56" s="215"/>
-      <c r="I56" s="215"/>
-      <c r="J56" s="215"/>
-      <c r="K56" s="215"/>
-      <c r="L56" s="215"/>
-      <c r="M56" s="216"/>
+      <c r="A56" s="200"/>
+      <c r="B56" s="201"/>
+      <c r="C56" s="201"/>
+      <c r="D56" s="201"/>
+      <c r="E56" s="202"/>
+      <c r="F56" s="212"/>
+      <c r="G56" s="210"/>
+      <c r="H56" s="210"/>
+      <c r="I56" s="210"/>
+      <c r="J56" s="210"/>
+      <c r="K56" s="210"/>
+      <c r="L56" s="210"/>
+      <c r="M56" s="211"/>
       <c r="N56" s="50"/>
       <c r="O56" s="49"/>
-      <c r="U56" s="202"/>
-      <c r="V56" s="203"/>
-      <c r="W56" s="203"/>
-      <c r="X56" s="203"/>
-      <c r="Y56" s="204"/>
-      <c r="Z56" s="225"/>
-      <c r="AA56" s="226"/>
-      <c r="AB56" s="226"/>
-      <c r="AC56" s="226"/>
-      <c r="AD56" s="226"/>
-      <c r="AE56" s="226"/>
-      <c r="AF56" s="226"/>
-      <c r="AG56" s="226"/>
-      <c r="AH56" s="227"/>
+      <c r="U56" s="200"/>
+      <c r="V56" s="201"/>
+      <c r="W56" s="201"/>
+      <c r="X56" s="201"/>
+      <c r="Y56" s="202"/>
+      <c r="Z56" s="178"/>
+      <c r="AA56" s="179"/>
+      <c r="AB56" s="179"/>
+      <c r="AC56" s="179"/>
+      <c r="AD56" s="179"/>
+      <c r="AE56" s="179"/>
+      <c r="AF56" s="179"/>
+      <c r="AG56" s="179"/>
+      <c r="AH56" s="180"/>
       <c r="AI56" s="50"/>
     </row>
     <row r="57" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="202"/>
-      <c r="B57" s="203"/>
-      <c r="C57" s="203"/>
-      <c r="D57" s="203"/>
-      <c r="E57" s="204"/>
-      <c r="F57" s="217"/>
-      <c r="G57" s="215"/>
-      <c r="H57" s="215"/>
-      <c r="I57" s="215"/>
-      <c r="J57" s="215"/>
-      <c r="K57" s="215"/>
-      <c r="L57" s="215"/>
-      <c r="M57" s="216"/>
+      <c r="A57" s="200"/>
+      <c r="B57" s="201"/>
+      <c r="C57" s="201"/>
+      <c r="D57" s="201"/>
+      <c r="E57" s="202"/>
+      <c r="F57" s="212"/>
+      <c r="G57" s="210"/>
+      <c r="H57" s="210"/>
+      <c r="I57" s="210"/>
+      <c r="J57" s="210"/>
+      <c r="K57" s="210"/>
+      <c r="L57" s="210"/>
+      <c r="M57" s="211"/>
       <c r="N57" s="50"/>
       <c r="O57" s="49"/>
-      <c r="U57" s="202"/>
-      <c r="V57" s="203"/>
-      <c r="W57" s="203"/>
-      <c r="X57" s="203"/>
-      <c r="Y57" s="204"/>
-      <c r="Z57" s="225"/>
-      <c r="AA57" s="226"/>
-      <c r="AB57" s="226"/>
-      <c r="AC57" s="226"/>
-      <c r="AD57" s="226"/>
-      <c r="AE57" s="226"/>
-      <c r="AF57" s="226"/>
-      <c r="AG57" s="226"/>
-      <c r="AH57" s="227"/>
+      <c r="U57" s="200"/>
+      <c r="V57" s="201"/>
+      <c r="W57" s="201"/>
+      <c r="X57" s="201"/>
+      <c r="Y57" s="202"/>
+      <c r="Z57" s="178"/>
+      <c r="AA57" s="179"/>
+      <c r="AB57" s="179"/>
+      <c r="AC57" s="179"/>
+      <c r="AD57" s="179"/>
+      <c r="AE57" s="179"/>
+      <c r="AF57" s="179"/>
+      <c r="AG57" s="179"/>
+      <c r="AH57" s="180"/>
       <c r="AI57" s="50"/>
     </row>
     <row r="58" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="202"/>
-      <c r="B58" s="203"/>
-      <c r="C58" s="203"/>
-      <c r="D58" s="203"/>
-      <c r="E58" s="204"/>
-      <c r="F58" s="217"/>
-      <c r="G58" s="215"/>
-      <c r="H58" s="215"/>
-      <c r="I58" s="215"/>
-      <c r="J58" s="215"/>
-      <c r="K58" s="215"/>
-      <c r="L58" s="215"/>
-      <c r="M58" s="216"/>
+      <c r="A58" s="200"/>
+      <c r="B58" s="201"/>
+      <c r="C58" s="201"/>
+      <c r="D58" s="201"/>
+      <c r="E58" s="202"/>
+      <c r="F58" s="212"/>
+      <c r="G58" s="210"/>
+      <c r="H58" s="210"/>
+      <c r="I58" s="210"/>
+      <c r="J58" s="210"/>
+      <c r="K58" s="210"/>
+      <c r="L58" s="210"/>
+      <c r="M58" s="211"/>
       <c r="N58" s="50"/>
       <c r="O58" s="49"/>
-      <c r="U58" s="202"/>
-      <c r="V58" s="203"/>
-      <c r="W58" s="203"/>
-      <c r="X58" s="203"/>
-      <c r="Y58" s="204"/>
-      <c r="Z58" s="225"/>
-      <c r="AA58" s="226"/>
-      <c r="AB58" s="226"/>
-      <c r="AC58" s="226"/>
-      <c r="AD58" s="226"/>
-      <c r="AE58" s="226"/>
-      <c r="AF58" s="226"/>
-      <c r="AG58" s="226"/>
-      <c r="AH58" s="227"/>
+      <c r="U58" s="200"/>
+      <c r="V58" s="201"/>
+      <c r="W58" s="201"/>
+      <c r="X58" s="201"/>
+      <c r="Y58" s="202"/>
+      <c r="Z58" s="178"/>
+      <c r="AA58" s="179"/>
+      <c r="AB58" s="179"/>
+      <c r="AC58" s="179"/>
+      <c r="AD58" s="179"/>
+      <c r="AE58" s="179"/>
+      <c r="AF58" s="179"/>
+      <c r="AG58" s="179"/>
+      <c r="AH58" s="180"/>
       <c r="AI58" s="50"/>
     </row>
     <row r="59" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="202"/>
-      <c r="B59" s="203"/>
-      <c r="C59" s="203"/>
-      <c r="D59" s="203"/>
-      <c r="E59" s="204"/>
-      <c r="F59" s="217"/>
-      <c r="G59" s="215"/>
-      <c r="H59" s="215"/>
-      <c r="I59" s="215"/>
-      <c r="J59" s="215"/>
-      <c r="K59" s="215"/>
-      <c r="L59" s="215"/>
-      <c r="M59" s="216"/>
+      <c r="A59" s="200"/>
+      <c r="B59" s="201"/>
+      <c r="C59" s="201"/>
+      <c r="D59" s="201"/>
+      <c r="E59" s="202"/>
+      <c r="F59" s="212"/>
+      <c r="G59" s="210"/>
+      <c r="H59" s="210"/>
+      <c r="I59" s="210"/>
+      <c r="J59" s="210"/>
+      <c r="K59" s="210"/>
+      <c r="L59" s="210"/>
+      <c r="M59" s="211"/>
       <c r="N59" s="50"/>
       <c r="O59" s="49"/>
-      <c r="U59" s="202"/>
-      <c r="V59" s="203"/>
-      <c r="W59" s="203"/>
-      <c r="X59" s="203"/>
-      <c r="Y59" s="204"/>
-      <c r="Z59" s="225"/>
-      <c r="AA59" s="226"/>
-      <c r="AB59" s="226"/>
-      <c r="AC59" s="226"/>
-      <c r="AD59" s="226"/>
-      <c r="AE59" s="226"/>
-      <c r="AF59" s="226"/>
-      <c r="AG59" s="226"/>
-      <c r="AH59" s="227"/>
+      <c r="U59" s="200"/>
+      <c r="V59" s="201"/>
+      <c r="W59" s="201"/>
+      <c r="X59" s="201"/>
+      <c r="Y59" s="202"/>
+      <c r="Z59" s="178"/>
+      <c r="AA59" s="179"/>
+      <c r="AB59" s="179"/>
+      <c r="AC59" s="179"/>
+      <c r="AD59" s="179"/>
+      <c r="AE59" s="179"/>
+      <c r="AF59" s="179"/>
+      <c r="AG59" s="179"/>
+      <c r="AH59" s="180"/>
       <c r="AI59" s="50"/>
     </row>
     <row r="60" spans="1:35" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="202"/>
-      <c r="B60" s="203"/>
-      <c r="C60" s="203"/>
-      <c r="D60" s="203"/>
-      <c r="E60" s="204"/>
-      <c r="F60" s="217"/>
-      <c r="G60" s="215"/>
-      <c r="H60" s="215"/>
-      <c r="I60" s="215"/>
-      <c r="J60" s="215"/>
-      <c r="K60" s="215"/>
-      <c r="L60" s="215"/>
-      <c r="M60" s="216"/>
+      <c r="A60" s="200"/>
+      <c r="B60" s="201"/>
+      <c r="C60" s="201"/>
+      <c r="D60" s="201"/>
+      <c r="E60" s="202"/>
+      <c r="F60" s="212"/>
+      <c r="G60" s="210"/>
+      <c r="H60" s="210"/>
+      <c r="I60" s="210"/>
+      <c r="J60" s="210"/>
+      <c r="K60" s="210"/>
+      <c r="L60" s="210"/>
+      <c r="M60" s="211"/>
       <c r="N60" s="50"/>
       <c r="O60" s="49"/>
-      <c r="U60" s="202"/>
-      <c r="V60" s="203"/>
-      <c r="W60" s="203"/>
-      <c r="X60" s="203"/>
-      <c r="Y60" s="204"/>
-      <c r="Z60" s="225"/>
-      <c r="AA60" s="226"/>
-      <c r="AB60" s="226"/>
-      <c r="AC60" s="226"/>
-      <c r="AD60" s="226"/>
-      <c r="AE60" s="226"/>
-      <c r="AF60" s="226"/>
-      <c r="AG60" s="226"/>
-      <c r="AH60" s="227"/>
+      <c r="U60" s="200"/>
+      <c r="V60" s="201"/>
+      <c r="W60" s="201"/>
+      <c r="X60" s="201"/>
+      <c r="Y60" s="202"/>
+      <c r="Z60" s="178"/>
+      <c r="AA60" s="179"/>
+      <c r="AB60" s="179"/>
+      <c r="AC60" s="179"/>
+      <c r="AD60" s="179"/>
+      <c r="AE60" s="179"/>
+      <c r="AF60" s="179"/>
+      <c r="AG60" s="179"/>
+      <c r="AH60" s="180"/>
       <c r="AI60" s="50"/>
     </row>
     <row r="61" spans="1:35" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="202"/>
-      <c r="B61" s="203"/>
-      <c r="C61" s="203"/>
-      <c r="D61" s="203"/>
-      <c r="E61" s="204"/>
-      <c r="F61" s="217"/>
-      <c r="G61" s="215"/>
-      <c r="H61" s="215"/>
-      <c r="I61" s="215"/>
-      <c r="J61" s="215"/>
-      <c r="K61" s="215"/>
-      <c r="L61" s="215"/>
-      <c r="M61" s="216"/>
+      <c r="A61" s="200"/>
+      <c r="B61" s="201"/>
+      <c r="C61" s="201"/>
+      <c r="D61" s="201"/>
+      <c r="E61" s="202"/>
+      <c r="F61" s="212"/>
+      <c r="G61" s="210"/>
+      <c r="H61" s="210"/>
+      <c r="I61" s="210"/>
+      <c r="J61" s="210"/>
+      <c r="K61" s="210"/>
+      <c r="L61" s="210"/>
+      <c r="M61" s="211"/>
       <c r="N61" s="50"/>
       <c r="O61" s="49"/>
-      <c r="U61" s="202"/>
-      <c r="V61" s="203"/>
-      <c r="W61" s="203"/>
-      <c r="X61" s="203"/>
-      <c r="Y61" s="204"/>
-      <c r="Z61" s="225"/>
-      <c r="AA61" s="226"/>
-      <c r="AB61" s="226"/>
-      <c r="AC61" s="226"/>
-      <c r="AD61" s="226"/>
-      <c r="AE61" s="226"/>
-      <c r="AF61" s="226"/>
-      <c r="AG61" s="226"/>
-      <c r="AH61" s="227"/>
+      <c r="U61" s="200"/>
+      <c r="V61" s="201"/>
+      <c r="W61" s="201"/>
+      <c r="X61" s="201"/>
+      <c r="Y61" s="202"/>
+      <c r="Z61" s="178"/>
+      <c r="AA61" s="179"/>
+      <c r="AB61" s="179"/>
+      <c r="AC61" s="179"/>
+      <c r="AD61" s="179"/>
+      <c r="AE61" s="179"/>
+      <c r="AF61" s="179"/>
+      <c r="AG61" s="179"/>
+      <c r="AH61" s="180"/>
       <c r="AI61" s="50"/>
     </row>
     <row r="62" spans="1:35" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="205"/>
-      <c r="B62" s="206"/>
-      <c r="C62" s="206"/>
-      <c r="D62" s="206"/>
-      <c r="E62" s="207"/>
-      <c r="F62" s="218"/>
-      <c r="G62" s="219"/>
-      <c r="H62" s="219"/>
-      <c r="I62" s="219"/>
-      <c r="J62" s="219"/>
-      <c r="K62" s="219"/>
-      <c r="L62" s="219"/>
-      <c r="M62" s="220"/>
+      <c r="A62" s="203"/>
+      <c r="B62" s="204"/>
+      <c r="C62" s="204"/>
+      <c r="D62" s="204"/>
+      <c r="E62" s="205"/>
+      <c r="F62" s="213"/>
+      <c r="G62" s="214"/>
+      <c r="H62" s="214"/>
+      <c r="I62" s="214"/>
+      <c r="J62" s="214"/>
+      <c r="K62" s="214"/>
+      <c r="L62" s="214"/>
+      <c r="M62" s="215"/>
       <c r="N62" s="50"/>
       <c r="O62" s="49"/>
-      <c r="U62" s="205"/>
-      <c r="V62" s="206"/>
-      <c r="W62" s="206"/>
-      <c r="X62" s="206"/>
-      <c r="Y62" s="207"/>
-      <c r="Z62" s="228"/>
-      <c r="AA62" s="229"/>
-      <c r="AB62" s="229"/>
-      <c r="AC62" s="229"/>
-      <c r="AD62" s="229"/>
-      <c r="AE62" s="229"/>
-      <c r="AF62" s="229"/>
-      <c r="AG62" s="229"/>
-      <c r="AH62" s="230"/>
+      <c r="U62" s="203"/>
+      <c r="V62" s="204"/>
+      <c r="W62" s="204"/>
+      <c r="X62" s="204"/>
+      <c r="Y62" s="205"/>
+      <c r="Z62" s="181"/>
+      <c r="AA62" s="182"/>
+      <c r="AB62" s="182"/>
+      <c r="AC62" s="182"/>
+      <c r="AD62" s="182"/>
+      <c r="AE62" s="182"/>
+      <c r="AF62" s="182"/>
+      <c r="AG62" s="182"/>
+      <c r="AH62" s="183"/>
       <c r="AI62" s="50"/>
     </row>
     <row r="63" spans="1:35" x14ac:dyDescent="0.2">
@@ -4437,25 +4437,11 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="Z47:AH47"/>
-    <mergeCell ref="Z48:AH62"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="U29:V29"/>
-    <mergeCell ref="U30:V30"/>
-    <mergeCell ref="U31:V31"/>
-    <mergeCell ref="AF29:AG29"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="U48:Y62"/>
-    <mergeCell ref="U47:Y47"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="A48:E62"/>
-    <mergeCell ref="F47:M47"/>
-    <mergeCell ref="F48:M62"/>
+    <mergeCell ref="B2:E3"/>
+    <mergeCell ref="I3:L3"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="I5:N5"/>
+    <mergeCell ref="G9:I9"/>
     <mergeCell ref="AJ29:AL29"/>
     <mergeCell ref="A28:S28"/>
     <mergeCell ref="P38:S38"/>
@@ -4472,11 +4458,25 @@
     <mergeCell ref="U28:AJ28"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A29:B29"/>
-    <mergeCell ref="B2:E3"/>
-    <mergeCell ref="I3:L3"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="I5:N5"/>
-    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="U48:Y62"/>
+    <mergeCell ref="U47:Y47"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="A48:E62"/>
+    <mergeCell ref="F47:M47"/>
+    <mergeCell ref="F48:M62"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="Z47:AH47"/>
+    <mergeCell ref="Z48:AH62"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="U29:V29"/>
+    <mergeCell ref="U30:V30"/>
+    <mergeCell ref="U31:V31"/>
+    <mergeCell ref="AF29:AG29"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4557,12 +4557,12 @@
     </row>
     <row r="2" spans="1:25" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
-      <c r="B2" s="175" t="s">
+      <c r="B2" s="233" t="s">
         <v>119</v>
       </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
+      <c r="C2" s="233"/>
+      <c r="D2" s="233"/>
+      <c r="E2" s="233"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -4579,21 +4579,21 @@
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="176"/>
-      <c r="C3" s="176"/>
-      <c r="D3" s="176"/>
-      <c r="E3" s="176"/>
+      <c r="B3" s="234"/>
+      <c r="C3" s="234"/>
+      <c r="D3" s="234"/>
+      <c r="E3" s="234"/>
       <c r="F3" s="5"/>
       <c r="G3" s="6"/>
       <c r="H3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="177">
+      <c r="I3" s="235">
         <v>20250708</v>
       </c>
-      <c r="J3" s="177"/>
-      <c r="K3" s="177"/>
-      <c r="L3" s="177"/>
+      <c r="J3" s="235"/>
+      <c r="K3" s="235"/>
+      <c r="L3" s="235"/>
       <c r="M3" s="8" t="s">
         <v>3</v>
       </c>
@@ -4625,25 +4625,25 @@
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="178">
+      <c r="B5" s="236">
         <v>45846</v>
       </c>
-      <c r="C5" s="178"/>
-      <c r="D5" s="178"/>
-      <c r="E5" s="178"/>
+      <c r="C5" s="236"/>
+      <c r="D5" s="236"/>
+      <c r="E5" s="236"/>
       <c r="F5" s="5"/>
       <c r="G5" s="6"/>
       <c r="H5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="177" t="s">
+      <c r="I5" s="235" t="s">
         <v>120</v>
       </c>
-      <c r="J5" s="177"/>
-      <c r="K5" s="177"/>
-      <c r="L5" s="177"/>
-      <c r="M5" s="177"/>
-      <c r="N5" s="177"/>
+      <c r="J5" s="235"/>
+      <c r="K5" s="235"/>
+      <c r="L5" s="235"/>
+      <c r="M5" s="235"/>
+      <c r="N5" s="235"/>
       <c r="O5" s="155"/>
       <c r="Y5" s="29"/>
     </row>
@@ -4701,11 +4701,11 @@
       <c r="F9" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="179" t="s">
+      <c r="G9" s="237" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="180"/>
-      <c r="I9" s="180"/>
+      <c r="H9" s="238"/>
+      <c r="I9" s="238"/>
       <c r="J9" s="19" t="s">
         <v>10</v>
       </c>
@@ -4736,11 +4736,11 @@
       <c r="F10" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="189" t="s">
+      <c r="G10" s="222" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="190"/>
-      <c r="I10" s="190"/>
+      <c r="H10" s="223"/>
+      <c r="I10" s="223"/>
       <c r="J10" s="21" t="s">
         <v>10</v>
       </c>
@@ -4771,11 +4771,11 @@
       <c r="F11" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="191" t="s">
+      <c r="G11" s="224" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="192"/>
-      <c r="I11" s="192"/>
+      <c r="H11" s="225"/>
+      <c r="I11" s="225"/>
       <c r="J11" s="62" t="s">
         <v>10</v>
       </c>
@@ -4936,10 +4936,10 @@
       <c r="B19" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="221" t="s">
+      <c r="E19" s="194" t="s">
         <v>46</v>
       </c>
-      <c r="F19" s="222"/>
+      <c r="F19" s="195"/>
       <c r="G19" s="20">
         <v>200</v>
       </c>
@@ -4956,10 +4956,10 @@
         <v>48</v>
       </c>
       <c r="B20" s="21"/>
-      <c r="E20" s="223" t="s">
+      <c r="E20" s="196" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="224"/>
+      <c r="F20" s="197"/>
       <c r="G20" s="22">
         <v>100</v>
       </c>
@@ -4970,10 +4970,10 @@
         <v>50</v>
       </c>
       <c r="B21" s="65"/>
-      <c r="E21" s="223" t="s">
+      <c r="E21" s="196" t="s">
         <v>51</v>
       </c>
-      <c r="F21" s="224"/>
+      <c r="F21" s="197"/>
       <c r="G21" s="22">
         <v>50</v>
       </c>
@@ -4984,10 +4984,10 @@
         <v>52</v>
       </c>
       <c r="B22" s="66"/>
-      <c r="E22" s="223" t="s">
+      <c r="E22" s="196" t="s">
         <v>53</v>
       </c>
-      <c r="F22" s="224"/>
+      <c r="F22" s="197"/>
       <c r="G22" s="23">
         <v>120</v>
       </c>
@@ -5000,10 +5000,10 @@
       <c r="B23" s="24">
         <v>5</v>
       </c>
-      <c r="E23" s="223" t="s">
+      <c r="E23" s="196" t="s">
         <v>55</v>
       </c>
-      <c r="F23" s="224"/>
+      <c r="F23" s="197"/>
       <c r="G23" s="23">
         <v>200</v>
       </c>
@@ -5016,10 +5016,10 @@
       <c r="B24" s="24">
         <v>5</v>
       </c>
-      <c r="E24" s="231" t="s">
+      <c r="E24" s="184" t="s">
         <v>57</v>
       </c>
-      <c r="F24" s="232"/>
+      <c r="F24" s="185"/>
       <c r="G24" s="25">
         <v>0.03</v>
       </c>
@@ -5051,50 +5051,50 @@
     </row>
     <row r="27" spans="1:39" ht="10.5" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="1:39" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="184" t="s">
+      <c r="A28" s="217" t="s">
         <v>59</v>
       </c>
-      <c r="B28" s="184"/>
-      <c r="C28" s="184"/>
-      <c r="D28" s="184"/>
-      <c r="E28" s="184"/>
-      <c r="F28" s="184"/>
-      <c r="G28" s="185"/>
-      <c r="H28" s="185"/>
-      <c r="I28" s="185"/>
-      <c r="J28" s="185"/>
-      <c r="K28" s="185"/>
-      <c r="L28" s="185"/>
-      <c r="M28" s="185"/>
-      <c r="N28" s="185"/>
-      <c r="O28" s="185"/>
-      <c r="P28" s="185"/>
-      <c r="Q28" s="185"/>
-      <c r="R28" s="185"/>
-      <c r="S28" s="185"/>
-      <c r="U28" s="185" t="s">
+      <c r="B28" s="217"/>
+      <c r="C28" s="217"/>
+      <c r="D28" s="217"/>
+      <c r="E28" s="217"/>
+      <c r="F28" s="217"/>
+      <c r="G28" s="218"/>
+      <c r="H28" s="218"/>
+      <c r="I28" s="218"/>
+      <c r="J28" s="218"/>
+      <c r="K28" s="218"/>
+      <c r="L28" s="218"/>
+      <c r="M28" s="218"/>
+      <c r="N28" s="218"/>
+      <c r="O28" s="218"/>
+      <c r="P28" s="218"/>
+      <c r="Q28" s="218"/>
+      <c r="R28" s="218"/>
+      <c r="S28" s="218"/>
+      <c r="U28" s="218" t="s">
         <v>60</v>
       </c>
-      <c r="V28" s="185"/>
-      <c r="W28" s="185"/>
-      <c r="X28" s="185"/>
-      <c r="Y28" s="185"/>
-      <c r="Z28" s="185"/>
-      <c r="AA28" s="185"/>
-      <c r="AB28" s="185"/>
-      <c r="AC28" s="185"/>
-      <c r="AD28" s="185"/>
-      <c r="AE28" s="185"/>
-      <c r="AF28" s="185"/>
-      <c r="AG28" s="185"/>
-      <c r="AH28" s="185"/>
-      <c r="AI28" s="185"/>
-      <c r="AJ28" s="185"/>
+      <c r="V28" s="218"/>
+      <c r="W28" s="218"/>
+      <c r="X28" s="218"/>
+      <c r="Y28" s="218"/>
+      <c r="Z28" s="218"/>
+      <c r="AA28" s="218"/>
+      <c r="AB28" s="218"/>
+      <c r="AC28" s="218"/>
+      <c r="AD28" s="218"/>
+      <c r="AE28" s="218"/>
+      <c r="AF28" s="218"/>
+      <c r="AG28" s="218"/>
+      <c r="AH28" s="218"/>
+      <c r="AI28" s="218"/>
+      <c r="AJ28" s="218"/>
       <c r="AM28" s="51"/>
     </row>
     <row r="29" spans="1:39" ht="18" x14ac:dyDescent="0.4">
-      <c r="A29" s="181"/>
-      <c r="B29" s="199"/>
+      <c r="A29" s="192"/>
+      <c r="B29" s="232"/>
       <c r="C29" s="54" t="s">
         <v>61</v>
       </c>
@@ -5107,19 +5107,19 @@
       <c r="F29" s="28">
         <v>3</v>
       </c>
-      <c r="L29" s="181" t="s">
+      <c r="L29" s="192" t="s">
         <v>62</v>
       </c>
-      <c r="M29" s="183"/>
+      <c r="M29" s="193"/>
       <c r="N29" s="157"/>
       <c r="O29" s="158"/>
-      <c r="P29" s="181" t="s">
+      <c r="P29" s="192" t="s">
         <v>63</v>
       </c>
-      <c r="Q29" s="182"/>
-      <c r="R29" s="183"/>
-      <c r="U29" s="233"/>
-      <c r="V29" s="234"/>
+      <c r="Q29" s="216"/>
+      <c r="R29" s="193"/>
+      <c r="U29" s="186"/>
+      <c r="V29" s="187"/>
       <c r="W29" s="54" t="s">
         <v>61</v>
       </c>
@@ -5133,22 +5133,22 @@
         <v>3</v>
       </c>
       <c r="AE29" s="121"/>
-      <c r="AF29" s="181" t="s">
+      <c r="AF29" s="192" t="s">
         <v>62</v>
       </c>
-      <c r="AG29" s="183"/>
+      <c r="AG29" s="193"/>
       <c r="AH29" s="153"/>
-      <c r="AJ29" s="181" t="s">
+      <c r="AJ29" s="192" t="s">
         <v>63</v>
       </c>
-      <c r="AK29" s="182"/>
-      <c r="AL29" s="183"/>
+      <c r="AK29" s="216"/>
+      <c r="AL29" s="193"/>
     </row>
     <row r="30" spans="1:39" ht="20" x14ac:dyDescent="0.4">
-      <c r="A30" s="197" t="s">
+      <c r="A30" s="230" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="198"/>
+      <c r="B30" s="231"/>
       <c r="C30" s="52">
         <v>6</v>
       </c>
@@ -5172,12 +5172,12 @@
       <c r="P30" s="125" t="s">
         <v>66</v>
       </c>
-      <c r="Q30" s="193"/>
-      <c r="R30" s="194"/>
-      <c r="U30" s="235" t="s">
+      <c r="Q30" s="226"/>
+      <c r="R30" s="227"/>
+      <c r="U30" s="188" t="s">
         <v>64</v>
       </c>
-      <c r="V30" s="236"/>
+      <c r="V30" s="189"/>
       <c r="W30" s="52"/>
       <c r="X30" s="53"/>
       <c r="Y30" s="53"/>
@@ -5195,10 +5195,10 @@
       <c r="AL30" s="145"/>
     </row>
     <row r="31" spans="1:39" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="200" t="s">
+      <c r="A31" s="198" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="201"/>
+      <c r="B31" s="199"/>
       <c r="C31" s="56">
         <v>45.4</v>
       </c>
@@ -5222,12 +5222,12 @@
       <c r="P31" s="125" t="s">
         <v>69</v>
       </c>
-      <c r="Q31" s="193"/>
-      <c r="R31" s="194"/>
-      <c r="U31" s="237" t="s">
+      <c r="Q31" s="226"/>
+      <c r="R31" s="227"/>
+      <c r="U31" s="190" t="s">
         <v>67</v>
       </c>
-      <c r="V31" s="238"/>
+      <c r="V31" s="191"/>
       <c r="W31" s="56"/>
       <c r="X31" s="56"/>
       <c r="Y31" s="56"/>
@@ -5254,8 +5254,8 @@
       <c r="P32" s="125" t="s">
         <v>70</v>
       </c>
-      <c r="Q32" s="193"/>
-      <c r="R32" s="194"/>
+      <c r="Q32" s="226"/>
+      <c r="R32" s="227"/>
       <c r="U32" s="146"/>
       <c r="V32" s="29"/>
       <c r="W32" s="29"/>
@@ -5300,8 +5300,8 @@
       <c r="P33" s="125" t="s">
         <v>76</v>
       </c>
-      <c r="Q33" s="193"/>
-      <c r="R33" s="194"/>
+      <c r="Q33" s="226"/>
+      <c r="R33" s="227"/>
       <c r="U33" s="147"/>
       <c r="V33" s="30" t="s">
         <v>71</v>
@@ -5358,8 +5358,8 @@
       <c r="P34" s="125" t="s">
         <v>77</v>
       </c>
-      <c r="Q34" s="193"/>
-      <c r="R34" s="194"/>
+      <c r="Q34" s="226"/>
+      <c r="R34" s="227"/>
       <c r="W34" s="33">
         <v>160</v>
       </c>
@@ -5416,8 +5416,8 @@
       <c r="P36" s="148" t="s">
         <v>78</v>
       </c>
-      <c r="Q36" s="195"/>
-      <c r="R36" s="196"/>
+      <c r="Q36" s="228"/>
+      <c r="R36" s="229"/>
       <c r="U36" s="169"/>
       <c r="V36" s="170"/>
       <c r="W36" s="170"/>
@@ -5509,12 +5509,12 @@
         <v>90</v>
       </c>
       <c r="N38" s="165"/>
-      <c r="P38" s="186" t="s">
+      <c r="P38" s="219" t="s">
         <v>91</v>
       </c>
-      <c r="Q38" s="187"/>
-      <c r="R38" s="187"/>
-      <c r="S38" s="188"/>
+      <c r="Q38" s="220"/>
+      <c r="R38" s="220"/>
+      <c r="S38" s="221"/>
       <c r="U38" s="107" t="s">
         <v>80</v>
       </c>
@@ -5972,527 +5972,527 @@
     </row>
     <row r="46" spans="1:38" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="1:38" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="208" t="s">
+      <c r="A47" s="206" t="s">
         <v>116</v>
       </c>
-      <c r="B47" s="209"/>
-      <c r="C47" s="209"/>
-      <c r="D47" s="209"/>
-      <c r="E47" s="210"/>
-      <c r="F47" s="211" t="s">
+      <c r="B47" s="207"/>
+      <c r="C47" s="207"/>
+      <c r="D47" s="207"/>
+      <c r="E47" s="208"/>
+      <c r="F47" s="175" t="s">
         <v>117</v>
       </c>
-      <c r="G47" s="212"/>
-      <c r="H47" s="212"/>
-      <c r="I47" s="212"/>
-      <c r="J47" s="212"/>
-      <c r="K47" s="212"/>
-      <c r="L47" s="212"/>
-      <c r="M47" s="213"/>
+      <c r="G47" s="176"/>
+      <c r="H47" s="176"/>
+      <c r="I47" s="176"/>
+      <c r="J47" s="176"/>
+      <c r="K47" s="176"/>
+      <c r="L47" s="176"/>
+      <c r="M47" s="177"/>
       <c r="N47" s="50"/>
       <c r="O47" s="49"/>
-      <c r="U47" s="208" t="s">
+      <c r="U47" s="206" t="s">
         <v>118</v>
       </c>
-      <c r="V47" s="209"/>
-      <c r="W47" s="209"/>
-      <c r="X47" s="209"/>
-      <c r="Y47" s="210"/>
-      <c r="Z47" s="211" t="s">
+      <c r="V47" s="207"/>
+      <c r="W47" s="207"/>
+      <c r="X47" s="207"/>
+      <c r="Y47" s="208"/>
+      <c r="Z47" s="175" t="s">
         <v>117</v>
       </c>
-      <c r="AA47" s="212"/>
-      <c r="AB47" s="212"/>
-      <c r="AC47" s="212"/>
-      <c r="AD47" s="212"/>
-      <c r="AE47" s="212"/>
-      <c r="AF47" s="212"/>
-      <c r="AG47" s="212"/>
-      <c r="AH47" s="213"/>
+      <c r="AA47" s="176"/>
+      <c r="AB47" s="176"/>
+      <c r="AC47" s="176"/>
+      <c r="AD47" s="176"/>
+      <c r="AE47" s="176"/>
+      <c r="AF47" s="176"/>
+      <c r="AG47" s="176"/>
+      <c r="AH47" s="177"/>
       <c r="AI47" s="50"/>
     </row>
     <row r="48" spans="1:38" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="202" t="s">
+      <c r="A48" s="200" t="s">
         <v>125</v>
       </c>
-      <c r="B48" s="203"/>
-      <c r="C48" s="203"/>
-      <c r="D48" s="203"/>
-      <c r="E48" s="204"/>
-      <c r="F48" s="217" t="s">
+      <c r="B48" s="201"/>
+      <c r="C48" s="201"/>
+      <c r="D48" s="201"/>
+      <c r="E48" s="202"/>
+      <c r="F48" s="212" t="s">
         <v>123</v>
       </c>
-      <c r="G48" s="215"/>
-      <c r="H48" s="215"/>
-      <c r="I48" s="215"/>
-      <c r="J48" s="215"/>
-      <c r="K48" s="215"/>
-      <c r="L48" s="215"/>
-      <c r="M48" s="216"/>
+      <c r="G48" s="210"/>
+      <c r="H48" s="210"/>
+      <c r="I48" s="210"/>
+      <c r="J48" s="210"/>
+      <c r="K48" s="210"/>
+      <c r="L48" s="210"/>
+      <c r="M48" s="211"/>
       <c r="N48" s="50"/>
       <c r="O48" s="49"/>
-      <c r="U48" s="202"/>
-      <c r="V48" s="203"/>
-      <c r="W48" s="203"/>
-      <c r="X48" s="203"/>
-      <c r="Y48" s="204"/>
-      <c r="Z48" s="225"/>
-      <c r="AA48" s="226"/>
-      <c r="AB48" s="226"/>
-      <c r="AC48" s="226"/>
-      <c r="AD48" s="226"/>
-      <c r="AE48" s="226"/>
-      <c r="AF48" s="226"/>
-      <c r="AG48" s="226"/>
-      <c r="AH48" s="227"/>
+      <c r="U48" s="200"/>
+      <c r="V48" s="201"/>
+      <c r="W48" s="201"/>
+      <c r="X48" s="201"/>
+      <c r="Y48" s="202"/>
+      <c r="Z48" s="178"/>
+      <c r="AA48" s="179"/>
+      <c r="AB48" s="179"/>
+      <c r="AC48" s="179"/>
+      <c r="AD48" s="179"/>
+      <c r="AE48" s="179"/>
+      <c r="AF48" s="179"/>
+      <c r="AG48" s="179"/>
+      <c r="AH48" s="180"/>
       <c r="AI48" s="50"/>
     </row>
     <row r="49" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="202"/>
-      <c r="B49" s="203"/>
-      <c r="C49" s="203"/>
-      <c r="D49" s="203"/>
-      <c r="E49" s="204"/>
-      <c r="F49" s="217"/>
-      <c r="G49" s="215"/>
-      <c r="H49" s="215"/>
-      <c r="I49" s="215"/>
-      <c r="J49" s="215"/>
-      <c r="K49" s="215"/>
-      <c r="L49" s="215"/>
-      <c r="M49" s="216"/>
+      <c r="A49" s="200"/>
+      <c r="B49" s="201"/>
+      <c r="C49" s="201"/>
+      <c r="D49" s="201"/>
+      <c r="E49" s="202"/>
+      <c r="F49" s="212"/>
+      <c r="G49" s="210"/>
+      <c r="H49" s="210"/>
+      <c r="I49" s="210"/>
+      <c r="J49" s="210"/>
+      <c r="K49" s="210"/>
+      <c r="L49" s="210"/>
+      <c r="M49" s="211"/>
       <c r="N49" s="50"/>
       <c r="O49" s="49"/>
-      <c r="U49" s="202"/>
-      <c r="V49" s="203"/>
-      <c r="W49" s="203"/>
-      <c r="X49" s="203"/>
-      <c r="Y49" s="204"/>
-      <c r="Z49" s="225"/>
-      <c r="AA49" s="226"/>
-      <c r="AB49" s="226"/>
-      <c r="AC49" s="226"/>
-      <c r="AD49" s="226"/>
-      <c r="AE49" s="226"/>
-      <c r="AF49" s="226"/>
-      <c r="AG49" s="226"/>
-      <c r="AH49" s="227"/>
+      <c r="U49" s="200"/>
+      <c r="V49" s="201"/>
+      <c r="W49" s="201"/>
+      <c r="X49" s="201"/>
+      <c r="Y49" s="202"/>
+      <c r="Z49" s="178"/>
+      <c r="AA49" s="179"/>
+      <c r="AB49" s="179"/>
+      <c r="AC49" s="179"/>
+      <c r="AD49" s="179"/>
+      <c r="AE49" s="179"/>
+      <c r="AF49" s="179"/>
+      <c r="AG49" s="179"/>
+      <c r="AH49" s="180"/>
       <c r="AI49" s="50"/>
     </row>
     <row r="50" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="202"/>
-      <c r="B50" s="203"/>
-      <c r="C50" s="203"/>
-      <c r="D50" s="203"/>
-      <c r="E50" s="204"/>
-      <c r="F50" s="217"/>
-      <c r="G50" s="215"/>
-      <c r="H50" s="215"/>
-      <c r="I50" s="215"/>
-      <c r="J50" s="215"/>
-      <c r="K50" s="215"/>
-      <c r="L50" s="215"/>
-      <c r="M50" s="216"/>
+      <c r="A50" s="200"/>
+      <c r="B50" s="201"/>
+      <c r="C50" s="201"/>
+      <c r="D50" s="201"/>
+      <c r="E50" s="202"/>
+      <c r="F50" s="212"/>
+      <c r="G50" s="210"/>
+      <c r="H50" s="210"/>
+      <c r="I50" s="210"/>
+      <c r="J50" s="210"/>
+      <c r="K50" s="210"/>
+      <c r="L50" s="210"/>
+      <c r="M50" s="211"/>
       <c r="N50" s="50"/>
       <c r="O50" s="49"/>
-      <c r="U50" s="202"/>
-      <c r="V50" s="203"/>
-      <c r="W50" s="203"/>
-      <c r="X50" s="203"/>
-      <c r="Y50" s="204"/>
-      <c r="Z50" s="225"/>
-      <c r="AA50" s="226"/>
-      <c r="AB50" s="226"/>
-      <c r="AC50" s="226"/>
-      <c r="AD50" s="226"/>
-      <c r="AE50" s="226"/>
-      <c r="AF50" s="226"/>
-      <c r="AG50" s="226"/>
-      <c r="AH50" s="227"/>
+      <c r="U50" s="200"/>
+      <c r="V50" s="201"/>
+      <c r="W50" s="201"/>
+      <c r="X50" s="201"/>
+      <c r="Y50" s="202"/>
+      <c r="Z50" s="178"/>
+      <c r="AA50" s="179"/>
+      <c r="AB50" s="179"/>
+      <c r="AC50" s="179"/>
+      <c r="AD50" s="179"/>
+      <c r="AE50" s="179"/>
+      <c r="AF50" s="179"/>
+      <c r="AG50" s="179"/>
+      <c r="AH50" s="180"/>
       <c r="AI50" s="50"/>
     </row>
     <row r="51" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="202"/>
-      <c r="B51" s="203"/>
-      <c r="C51" s="203"/>
-      <c r="D51" s="203"/>
-      <c r="E51" s="204"/>
-      <c r="F51" s="217"/>
-      <c r="G51" s="215"/>
-      <c r="H51" s="215"/>
-      <c r="I51" s="215"/>
-      <c r="J51" s="215"/>
-      <c r="K51" s="215"/>
-      <c r="L51" s="215"/>
-      <c r="M51" s="216"/>
+      <c r="A51" s="200"/>
+      <c r="B51" s="201"/>
+      <c r="C51" s="201"/>
+      <c r="D51" s="201"/>
+      <c r="E51" s="202"/>
+      <c r="F51" s="212"/>
+      <c r="G51" s="210"/>
+      <c r="H51" s="210"/>
+      <c r="I51" s="210"/>
+      <c r="J51" s="210"/>
+      <c r="K51" s="210"/>
+      <c r="L51" s="210"/>
+      <c r="M51" s="211"/>
       <c r="N51" s="50"/>
       <c r="O51" s="49"/>
-      <c r="U51" s="202"/>
-      <c r="V51" s="203"/>
-      <c r="W51" s="203"/>
-      <c r="X51" s="203"/>
-      <c r="Y51" s="204"/>
-      <c r="Z51" s="225"/>
-      <c r="AA51" s="226"/>
-      <c r="AB51" s="226"/>
-      <c r="AC51" s="226"/>
-      <c r="AD51" s="226"/>
-      <c r="AE51" s="226"/>
-      <c r="AF51" s="226"/>
-      <c r="AG51" s="226"/>
-      <c r="AH51" s="227"/>
+      <c r="U51" s="200"/>
+      <c r="V51" s="201"/>
+      <c r="W51" s="201"/>
+      <c r="X51" s="201"/>
+      <c r="Y51" s="202"/>
+      <c r="Z51" s="178"/>
+      <c r="AA51" s="179"/>
+      <c r="AB51" s="179"/>
+      <c r="AC51" s="179"/>
+      <c r="AD51" s="179"/>
+      <c r="AE51" s="179"/>
+      <c r="AF51" s="179"/>
+      <c r="AG51" s="179"/>
+      <c r="AH51" s="180"/>
       <c r="AI51" s="50"/>
     </row>
     <row r="52" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="202"/>
-      <c r="B52" s="203"/>
-      <c r="C52" s="203"/>
-      <c r="D52" s="203"/>
-      <c r="E52" s="204"/>
-      <c r="F52" s="217"/>
-      <c r="G52" s="215"/>
-      <c r="H52" s="215"/>
-      <c r="I52" s="215"/>
-      <c r="J52" s="215"/>
-      <c r="K52" s="215"/>
-      <c r="L52" s="215"/>
-      <c r="M52" s="216"/>
+      <c r="A52" s="200"/>
+      <c r="B52" s="201"/>
+      <c r="C52" s="201"/>
+      <c r="D52" s="201"/>
+      <c r="E52" s="202"/>
+      <c r="F52" s="212"/>
+      <c r="G52" s="210"/>
+      <c r="H52" s="210"/>
+      <c r="I52" s="210"/>
+      <c r="J52" s="210"/>
+      <c r="K52" s="210"/>
+      <c r="L52" s="210"/>
+      <c r="M52" s="211"/>
       <c r="N52" s="50"/>
       <c r="O52" s="49"/>
-      <c r="U52" s="202"/>
-      <c r="V52" s="203"/>
-      <c r="W52" s="203"/>
-      <c r="X52" s="203"/>
-      <c r="Y52" s="204"/>
-      <c r="Z52" s="225"/>
-      <c r="AA52" s="226"/>
-      <c r="AB52" s="226"/>
-      <c r="AC52" s="226"/>
-      <c r="AD52" s="226"/>
-      <c r="AE52" s="226"/>
-      <c r="AF52" s="226"/>
-      <c r="AG52" s="226"/>
-      <c r="AH52" s="227"/>
+      <c r="U52" s="200"/>
+      <c r="V52" s="201"/>
+      <c r="W52" s="201"/>
+      <c r="X52" s="201"/>
+      <c r="Y52" s="202"/>
+      <c r="Z52" s="178"/>
+      <c r="AA52" s="179"/>
+      <c r="AB52" s="179"/>
+      <c r="AC52" s="179"/>
+      <c r="AD52" s="179"/>
+      <c r="AE52" s="179"/>
+      <c r="AF52" s="179"/>
+      <c r="AG52" s="179"/>
+      <c r="AH52" s="180"/>
       <c r="AI52" s="50"/>
     </row>
     <row r="53" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="202"/>
-      <c r="B53" s="203"/>
-      <c r="C53" s="203"/>
-      <c r="D53" s="203"/>
-      <c r="E53" s="204"/>
-      <c r="F53" s="217"/>
-      <c r="G53" s="215"/>
-      <c r="H53" s="215"/>
-      <c r="I53" s="215"/>
-      <c r="J53" s="215"/>
-      <c r="K53" s="215"/>
-      <c r="L53" s="215"/>
-      <c r="M53" s="216"/>
+      <c r="A53" s="200"/>
+      <c r="B53" s="201"/>
+      <c r="C53" s="201"/>
+      <c r="D53" s="201"/>
+      <c r="E53" s="202"/>
+      <c r="F53" s="212"/>
+      <c r="G53" s="210"/>
+      <c r="H53" s="210"/>
+      <c r="I53" s="210"/>
+      <c r="J53" s="210"/>
+      <c r="K53" s="210"/>
+      <c r="L53" s="210"/>
+      <c r="M53" s="211"/>
       <c r="N53" s="50"/>
       <c r="O53" s="49"/>
-      <c r="U53" s="202"/>
-      <c r="V53" s="203"/>
-      <c r="W53" s="203"/>
-      <c r="X53" s="203"/>
-      <c r="Y53" s="204"/>
-      <c r="Z53" s="225"/>
-      <c r="AA53" s="226"/>
-      <c r="AB53" s="226"/>
-      <c r="AC53" s="226"/>
-      <c r="AD53" s="226"/>
-      <c r="AE53" s="226"/>
-      <c r="AF53" s="226"/>
-      <c r="AG53" s="226"/>
-      <c r="AH53" s="227"/>
+      <c r="U53" s="200"/>
+      <c r="V53" s="201"/>
+      <c r="W53" s="201"/>
+      <c r="X53" s="201"/>
+      <c r="Y53" s="202"/>
+      <c r="Z53" s="178"/>
+      <c r="AA53" s="179"/>
+      <c r="AB53" s="179"/>
+      <c r="AC53" s="179"/>
+      <c r="AD53" s="179"/>
+      <c r="AE53" s="179"/>
+      <c r="AF53" s="179"/>
+      <c r="AG53" s="179"/>
+      <c r="AH53" s="180"/>
       <c r="AI53" s="50"/>
     </row>
     <row r="54" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="202"/>
-      <c r="B54" s="203"/>
-      <c r="C54" s="203"/>
-      <c r="D54" s="203"/>
-      <c r="E54" s="204"/>
-      <c r="F54" s="217"/>
-      <c r="G54" s="215"/>
-      <c r="H54" s="215"/>
-      <c r="I54" s="215"/>
-      <c r="J54" s="215"/>
-      <c r="K54" s="215"/>
-      <c r="L54" s="215"/>
-      <c r="M54" s="216"/>
+      <c r="A54" s="200"/>
+      <c r="B54" s="201"/>
+      <c r="C54" s="201"/>
+      <c r="D54" s="201"/>
+      <c r="E54" s="202"/>
+      <c r="F54" s="212"/>
+      <c r="G54" s="210"/>
+      <c r="H54" s="210"/>
+      <c r="I54" s="210"/>
+      <c r="J54" s="210"/>
+      <c r="K54" s="210"/>
+      <c r="L54" s="210"/>
+      <c r="M54" s="211"/>
       <c r="N54" s="50"/>
       <c r="O54" s="49"/>
-      <c r="U54" s="202"/>
-      <c r="V54" s="203"/>
-      <c r="W54" s="203"/>
-      <c r="X54" s="203"/>
-      <c r="Y54" s="204"/>
-      <c r="Z54" s="225"/>
-      <c r="AA54" s="226"/>
-      <c r="AB54" s="226"/>
-      <c r="AC54" s="226"/>
-      <c r="AD54" s="226"/>
-      <c r="AE54" s="226"/>
-      <c r="AF54" s="226"/>
-      <c r="AG54" s="226"/>
-      <c r="AH54" s="227"/>
+      <c r="U54" s="200"/>
+      <c r="V54" s="201"/>
+      <c r="W54" s="201"/>
+      <c r="X54" s="201"/>
+      <c r="Y54" s="202"/>
+      <c r="Z54" s="178"/>
+      <c r="AA54" s="179"/>
+      <c r="AB54" s="179"/>
+      <c r="AC54" s="179"/>
+      <c r="AD54" s="179"/>
+      <c r="AE54" s="179"/>
+      <c r="AF54" s="179"/>
+      <c r="AG54" s="179"/>
+      <c r="AH54" s="180"/>
       <c r="AI54" s="50"/>
     </row>
     <row r="55" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="202"/>
-      <c r="B55" s="203"/>
-      <c r="C55" s="203"/>
-      <c r="D55" s="203"/>
-      <c r="E55" s="204"/>
-      <c r="F55" s="217"/>
-      <c r="G55" s="215"/>
-      <c r="H55" s="215"/>
-      <c r="I55" s="215"/>
-      <c r="J55" s="215"/>
-      <c r="K55" s="215"/>
-      <c r="L55" s="215"/>
-      <c r="M55" s="216"/>
+      <c r="A55" s="200"/>
+      <c r="B55" s="201"/>
+      <c r="C55" s="201"/>
+      <c r="D55" s="201"/>
+      <c r="E55" s="202"/>
+      <c r="F55" s="212"/>
+      <c r="G55" s="210"/>
+      <c r="H55" s="210"/>
+      <c r="I55" s="210"/>
+      <c r="J55" s="210"/>
+      <c r="K55" s="210"/>
+      <c r="L55" s="210"/>
+      <c r="M55" s="211"/>
       <c r="N55" s="50"/>
       <c r="O55" s="49"/>
-      <c r="U55" s="202"/>
-      <c r="V55" s="203"/>
-      <c r="W55" s="203"/>
-      <c r="X55" s="203"/>
-      <c r="Y55" s="204"/>
-      <c r="Z55" s="225"/>
-      <c r="AA55" s="226"/>
-      <c r="AB55" s="226"/>
-      <c r="AC55" s="226"/>
-      <c r="AD55" s="226"/>
-      <c r="AE55" s="226"/>
-      <c r="AF55" s="226"/>
-      <c r="AG55" s="226"/>
-      <c r="AH55" s="227"/>
+      <c r="U55" s="200"/>
+      <c r="V55" s="201"/>
+      <c r="W55" s="201"/>
+      <c r="X55" s="201"/>
+      <c r="Y55" s="202"/>
+      <c r="Z55" s="178"/>
+      <c r="AA55" s="179"/>
+      <c r="AB55" s="179"/>
+      <c r="AC55" s="179"/>
+      <c r="AD55" s="179"/>
+      <c r="AE55" s="179"/>
+      <c r="AF55" s="179"/>
+      <c r="AG55" s="179"/>
+      <c r="AH55" s="180"/>
       <c r="AI55" s="50"/>
     </row>
     <row r="56" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="202"/>
-      <c r="B56" s="203"/>
-      <c r="C56" s="203"/>
-      <c r="D56" s="203"/>
-      <c r="E56" s="204"/>
-      <c r="F56" s="217"/>
-      <c r="G56" s="215"/>
-      <c r="H56" s="215"/>
-      <c r="I56" s="215"/>
-      <c r="J56" s="215"/>
-      <c r="K56" s="215"/>
-      <c r="L56" s="215"/>
-      <c r="M56" s="216"/>
+      <c r="A56" s="200"/>
+      <c r="B56" s="201"/>
+      <c r="C56" s="201"/>
+      <c r="D56" s="201"/>
+      <c r="E56" s="202"/>
+      <c r="F56" s="212"/>
+      <c r="G56" s="210"/>
+      <c r="H56" s="210"/>
+      <c r="I56" s="210"/>
+      <c r="J56" s="210"/>
+      <c r="K56" s="210"/>
+      <c r="L56" s="210"/>
+      <c r="M56" s="211"/>
       <c r="N56" s="50"/>
       <c r="O56" s="49"/>
-      <c r="U56" s="202"/>
-      <c r="V56" s="203"/>
-      <c r="W56" s="203"/>
-      <c r="X56" s="203"/>
-      <c r="Y56" s="204"/>
-      <c r="Z56" s="225"/>
-      <c r="AA56" s="226"/>
-      <c r="AB56" s="226"/>
-      <c r="AC56" s="226"/>
-      <c r="AD56" s="226"/>
-      <c r="AE56" s="226"/>
-      <c r="AF56" s="226"/>
-      <c r="AG56" s="226"/>
-      <c r="AH56" s="227"/>
+      <c r="U56" s="200"/>
+      <c r="V56" s="201"/>
+      <c r="W56" s="201"/>
+      <c r="X56" s="201"/>
+      <c r="Y56" s="202"/>
+      <c r="Z56" s="178"/>
+      <c r="AA56" s="179"/>
+      <c r="AB56" s="179"/>
+      <c r="AC56" s="179"/>
+      <c r="AD56" s="179"/>
+      <c r="AE56" s="179"/>
+      <c r="AF56" s="179"/>
+      <c r="AG56" s="179"/>
+      <c r="AH56" s="180"/>
       <c r="AI56" s="50"/>
     </row>
     <row r="57" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="202"/>
-      <c r="B57" s="203"/>
-      <c r="C57" s="203"/>
-      <c r="D57" s="203"/>
-      <c r="E57" s="204"/>
-      <c r="F57" s="217"/>
-      <c r="G57" s="215"/>
-      <c r="H57" s="215"/>
-      <c r="I57" s="215"/>
-      <c r="J57" s="215"/>
-      <c r="K57" s="215"/>
-      <c r="L57" s="215"/>
-      <c r="M57" s="216"/>
+      <c r="A57" s="200"/>
+      <c r="B57" s="201"/>
+      <c r="C57" s="201"/>
+      <c r="D57" s="201"/>
+      <c r="E57" s="202"/>
+      <c r="F57" s="212"/>
+      <c r="G57" s="210"/>
+      <c r="H57" s="210"/>
+      <c r="I57" s="210"/>
+      <c r="J57" s="210"/>
+      <c r="K57" s="210"/>
+      <c r="L57" s="210"/>
+      <c r="M57" s="211"/>
       <c r="N57" s="50"/>
       <c r="O57" s="49"/>
-      <c r="U57" s="202"/>
-      <c r="V57" s="203"/>
-      <c r="W57" s="203"/>
-      <c r="X57" s="203"/>
-      <c r="Y57" s="204"/>
-      <c r="Z57" s="225"/>
-      <c r="AA57" s="226"/>
-      <c r="AB57" s="226"/>
-      <c r="AC57" s="226"/>
-      <c r="AD57" s="226"/>
-      <c r="AE57" s="226"/>
-      <c r="AF57" s="226"/>
-      <c r="AG57" s="226"/>
-      <c r="AH57" s="227"/>
+      <c r="U57" s="200"/>
+      <c r="V57" s="201"/>
+      <c r="W57" s="201"/>
+      <c r="X57" s="201"/>
+      <c r="Y57" s="202"/>
+      <c r="Z57" s="178"/>
+      <c r="AA57" s="179"/>
+      <c r="AB57" s="179"/>
+      <c r="AC57" s="179"/>
+      <c r="AD57" s="179"/>
+      <c r="AE57" s="179"/>
+      <c r="AF57" s="179"/>
+      <c r="AG57" s="179"/>
+      <c r="AH57" s="180"/>
       <c r="AI57" s="50"/>
     </row>
     <row r="58" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="202"/>
-      <c r="B58" s="203"/>
-      <c r="C58" s="203"/>
-      <c r="D58" s="203"/>
-      <c r="E58" s="204"/>
-      <c r="F58" s="217"/>
-      <c r="G58" s="215"/>
-      <c r="H58" s="215"/>
-      <c r="I58" s="215"/>
-      <c r="J58" s="215"/>
-      <c r="K58" s="215"/>
-      <c r="L58" s="215"/>
-      <c r="M58" s="216"/>
+      <c r="A58" s="200"/>
+      <c r="B58" s="201"/>
+      <c r="C58" s="201"/>
+      <c r="D58" s="201"/>
+      <c r="E58" s="202"/>
+      <c r="F58" s="212"/>
+      <c r="G58" s="210"/>
+      <c r="H58" s="210"/>
+      <c r="I58" s="210"/>
+      <c r="J58" s="210"/>
+      <c r="K58" s="210"/>
+      <c r="L58" s="210"/>
+      <c r="M58" s="211"/>
       <c r="N58" s="50"/>
       <c r="O58" s="49"/>
-      <c r="U58" s="202"/>
-      <c r="V58" s="203"/>
-      <c r="W58" s="203"/>
-      <c r="X58" s="203"/>
-      <c r="Y58" s="204"/>
-      <c r="Z58" s="225"/>
-      <c r="AA58" s="226"/>
-      <c r="AB58" s="226"/>
-      <c r="AC58" s="226"/>
-      <c r="AD58" s="226"/>
-      <c r="AE58" s="226"/>
-      <c r="AF58" s="226"/>
-      <c r="AG58" s="226"/>
-      <c r="AH58" s="227"/>
+      <c r="U58" s="200"/>
+      <c r="V58" s="201"/>
+      <c r="W58" s="201"/>
+      <c r="X58" s="201"/>
+      <c r="Y58" s="202"/>
+      <c r="Z58" s="178"/>
+      <c r="AA58" s="179"/>
+      <c r="AB58" s="179"/>
+      <c r="AC58" s="179"/>
+      <c r="AD58" s="179"/>
+      <c r="AE58" s="179"/>
+      <c r="AF58" s="179"/>
+      <c r="AG58" s="179"/>
+      <c r="AH58" s="180"/>
       <c r="AI58" s="50"/>
     </row>
     <row r="59" spans="1:35" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="202"/>
-      <c r="B59" s="203"/>
-      <c r="C59" s="203"/>
-      <c r="D59" s="203"/>
-      <c r="E59" s="204"/>
-      <c r="F59" s="217"/>
-      <c r="G59" s="215"/>
-      <c r="H59" s="215"/>
-      <c r="I59" s="215"/>
-      <c r="J59" s="215"/>
-      <c r="K59" s="215"/>
-      <c r="L59" s="215"/>
-      <c r="M59" s="216"/>
+      <c r="A59" s="200"/>
+      <c r="B59" s="201"/>
+      <c r="C59" s="201"/>
+      <c r="D59" s="201"/>
+      <c r="E59" s="202"/>
+      <c r="F59" s="212"/>
+      <c r="G59" s="210"/>
+      <c r="H59" s="210"/>
+      <c r="I59" s="210"/>
+      <c r="J59" s="210"/>
+      <c r="K59" s="210"/>
+      <c r="L59" s="210"/>
+      <c r="M59" s="211"/>
       <c r="N59" s="50"/>
       <c r="O59" s="49"/>
-      <c r="U59" s="202"/>
-      <c r="V59" s="203"/>
-      <c r="W59" s="203"/>
-      <c r="X59" s="203"/>
-      <c r="Y59" s="204"/>
-      <c r="Z59" s="225"/>
-      <c r="AA59" s="226"/>
-      <c r="AB59" s="226"/>
-      <c r="AC59" s="226"/>
-      <c r="AD59" s="226"/>
-      <c r="AE59" s="226"/>
-      <c r="AF59" s="226"/>
-      <c r="AG59" s="226"/>
-      <c r="AH59" s="227"/>
+      <c r="U59" s="200"/>
+      <c r="V59" s="201"/>
+      <c r="W59" s="201"/>
+      <c r="X59" s="201"/>
+      <c r="Y59" s="202"/>
+      <c r="Z59" s="178"/>
+      <c r="AA59" s="179"/>
+      <c r="AB59" s="179"/>
+      <c r="AC59" s="179"/>
+      <c r="AD59" s="179"/>
+      <c r="AE59" s="179"/>
+      <c r="AF59" s="179"/>
+      <c r="AG59" s="179"/>
+      <c r="AH59" s="180"/>
       <c r="AI59" s="50"/>
     </row>
     <row r="60" spans="1:35" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="202"/>
-      <c r="B60" s="203"/>
-      <c r="C60" s="203"/>
-      <c r="D60" s="203"/>
-      <c r="E60" s="204"/>
-      <c r="F60" s="217"/>
-      <c r="G60" s="215"/>
-      <c r="H60" s="215"/>
-      <c r="I60" s="215"/>
-      <c r="J60" s="215"/>
-      <c r="K60" s="215"/>
-      <c r="L60" s="215"/>
-      <c r="M60" s="216"/>
+      <c r="A60" s="200"/>
+      <c r="B60" s="201"/>
+      <c r="C60" s="201"/>
+      <c r="D60" s="201"/>
+      <c r="E60" s="202"/>
+      <c r="F60" s="212"/>
+      <c r="G60" s="210"/>
+      <c r="H60" s="210"/>
+      <c r="I60" s="210"/>
+      <c r="J60" s="210"/>
+      <c r="K60" s="210"/>
+      <c r="L60" s="210"/>
+      <c r="M60" s="211"/>
       <c r="N60" s="50"/>
       <c r="O60" s="49"/>
-      <c r="U60" s="202"/>
-      <c r="V60" s="203"/>
-      <c r="W60" s="203"/>
-      <c r="X60" s="203"/>
-      <c r="Y60" s="204"/>
-      <c r="Z60" s="225"/>
-      <c r="AA60" s="226"/>
-      <c r="AB60" s="226"/>
-      <c r="AC60" s="226"/>
-      <c r="AD60" s="226"/>
-      <c r="AE60" s="226"/>
-      <c r="AF60" s="226"/>
-      <c r="AG60" s="226"/>
-      <c r="AH60" s="227"/>
+      <c r="U60" s="200"/>
+      <c r="V60" s="201"/>
+      <c r="W60" s="201"/>
+      <c r="X60" s="201"/>
+      <c r="Y60" s="202"/>
+      <c r="Z60" s="178"/>
+      <c r="AA60" s="179"/>
+      <c r="AB60" s="179"/>
+      <c r="AC60" s="179"/>
+      <c r="AD60" s="179"/>
+      <c r="AE60" s="179"/>
+      <c r="AF60" s="179"/>
+      <c r="AG60" s="179"/>
+      <c r="AH60" s="180"/>
       <c r="AI60" s="50"/>
     </row>
     <row r="61" spans="1:35" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="202"/>
-      <c r="B61" s="203"/>
-      <c r="C61" s="203"/>
-      <c r="D61" s="203"/>
-      <c r="E61" s="204"/>
-      <c r="F61" s="217"/>
-      <c r="G61" s="215"/>
-      <c r="H61" s="215"/>
-      <c r="I61" s="215"/>
-      <c r="J61" s="215"/>
-      <c r="K61" s="215"/>
-      <c r="L61" s="215"/>
-      <c r="M61" s="216"/>
+      <c r="A61" s="200"/>
+      <c r="B61" s="201"/>
+      <c r="C61" s="201"/>
+      <c r="D61" s="201"/>
+      <c r="E61" s="202"/>
+      <c r="F61" s="212"/>
+      <c r="G61" s="210"/>
+      <c r="H61" s="210"/>
+      <c r="I61" s="210"/>
+      <c r="J61" s="210"/>
+      <c r="K61" s="210"/>
+      <c r="L61" s="210"/>
+      <c r="M61" s="211"/>
       <c r="N61" s="50"/>
       <c r="O61" s="49"/>
-      <c r="U61" s="202"/>
-      <c r="V61" s="203"/>
-      <c r="W61" s="203"/>
-      <c r="X61" s="203"/>
-      <c r="Y61" s="204"/>
-      <c r="Z61" s="225"/>
-      <c r="AA61" s="226"/>
-      <c r="AB61" s="226"/>
-      <c r="AC61" s="226"/>
-      <c r="AD61" s="226"/>
-      <c r="AE61" s="226"/>
-      <c r="AF61" s="226"/>
-      <c r="AG61" s="226"/>
-      <c r="AH61" s="227"/>
+      <c r="U61" s="200"/>
+      <c r="V61" s="201"/>
+      <c r="W61" s="201"/>
+      <c r="X61" s="201"/>
+      <c r="Y61" s="202"/>
+      <c r="Z61" s="178"/>
+      <c r="AA61" s="179"/>
+      <c r="AB61" s="179"/>
+      <c r="AC61" s="179"/>
+      <c r="AD61" s="179"/>
+      <c r="AE61" s="179"/>
+      <c r="AF61" s="179"/>
+      <c r="AG61" s="179"/>
+      <c r="AH61" s="180"/>
       <c r="AI61" s="50"/>
     </row>
     <row r="62" spans="1:35" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="205"/>
-      <c r="B62" s="206"/>
-      <c r="C62" s="206"/>
-      <c r="D62" s="206"/>
-      <c r="E62" s="207"/>
-      <c r="F62" s="218"/>
-      <c r="G62" s="219"/>
-      <c r="H62" s="219"/>
-      <c r="I62" s="219"/>
-      <c r="J62" s="219"/>
-      <c r="K62" s="219"/>
-      <c r="L62" s="219"/>
-      <c r="M62" s="220"/>
+      <c r="A62" s="203"/>
+      <c r="B62" s="204"/>
+      <c r="C62" s="204"/>
+      <c r="D62" s="204"/>
+      <c r="E62" s="205"/>
+      <c r="F62" s="213"/>
+      <c r="G62" s="214"/>
+      <c r="H62" s="214"/>
+      <c r="I62" s="214"/>
+      <c r="J62" s="214"/>
+      <c r="K62" s="214"/>
+      <c r="L62" s="214"/>
+      <c r="M62" s="215"/>
       <c r="N62" s="50"/>
       <c r="O62" s="49"/>
-      <c r="U62" s="205"/>
-      <c r="V62" s="206"/>
-      <c r="W62" s="206"/>
-      <c r="X62" s="206"/>
-      <c r="Y62" s="207"/>
-      <c r="Z62" s="228"/>
-      <c r="AA62" s="229"/>
-      <c r="AB62" s="229"/>
-      <c r="AC62" s="229"/>
-      <c r="AD62" s="229"/>
-      <c r="AE62" s="229"/>
-      <c r="AF62" s="229"/>
-      <c r="AG62" s="229"/>
-      <c r="AH62" s="230"/>
+      <c r="U62" s="203"/>
+      <c r="V62" s="204"/>
+      <c r="W62" s="204"/>
+      <c r="X62" s="204"/>
+      <c r="Y62" s="205"/>
+      <c r="Z62" s="181"/>
+      <c r="AA62" s="182"/>
+      <c r="AB62" s="182"/>
+      <c r="AC62" s="182"/>
+      <c r="AD62" s="182"/>
+      <c r="AE62" s="182"/>
+      <c r="AF62" s="182"/>
+      <c r="AG62" s="182"/>
+      <c r="AH62" s="183"/>
       <c r="AI62" s="50"/>
     </row>
     <row r="63" spans="1:35" x14ac:dyDescent="0.2">
@@ -6595,6 +6595,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="U47:Y47"/>
+    <mergeCell ref="Z47:AH47"/>
+    <mergeCell ref="A48:E62"/>
+    <mergeCell ref="F48:M62"/>
+    <mergeCell ref="U48:Y62"/>
+    <mergeCell ref="Z48:AH62"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="F47:M47"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="P38:S38"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="U30:V30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="Q31:R31"/>
+    <mergeCell ref="U31:V31"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="A28:S28"/>
+    <mergeCell ref="U28:AJ28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="P29:R29"/>
+    <mergeCell ref="U29:V29"/>
+    <mergeCell ref="AF29:AG29"/>
+    <mergeCell ref="AJ29:AL29"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="B2:E3"/>
     <mergeCell ref="I3:L3"/>
@@ -6607,34 +6635,6 @@
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="A28:S28"/>
-    <mergeCell ref="U28:AJ28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="P29:R29"/>
-    <mergeCell ref="U29:V29"/>
-    <mergeCell ref="AF29:AG29"/>
-    <mergeCell ref="AJ29:AL29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="Q30:R30"/>
-    <mergeCell ref="U30:V30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="Q31:R31"/>
-    <mergeCell ref="U31:V31"/>
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="Q33:R33"/>
-    <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="P38:S38"/>
-    <mergeCell ref="U47:Y47"/>
-    <mergeCell ref="Z47:AH47"/>
-    <mergeCell ref="A48:E62"/>
-    <mergeCell ref="F48:M62"/>
-    <mergeCell ref="U48:Y62"/>
-    <mergeCell ref="Z48:AH62"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="F47:M47"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6869,6 +6869,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="03fd382f-fd16-45b5-8306-1be73a58e004" xsi:nil="true"/>
@@ -6877,15 +6886,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6908,6 +6908,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74D37766-22C8-4101-A6A1-3DEEE84685D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49A4B1E7-D809-4F18-8A5B-250753158AE8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -6916,12 +6924,4 @@
     <ds:schemaRef ds:uri="3314f2a4-48e9-4e28-8da9-3bfbc3a74041"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74D37766-22C8-4101-A6A1-3DEEE84685D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>